<commit_message>
adding some stuff to make it looks nice for when got the time
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Design peddle pirotS! (2)" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1077,27 +1076,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1116,150 +1097,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1269,170 +1118,320 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="48" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1901,6 +1900,66 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="6-Point Star 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6543674" y="4876800"/>
+          <a:ext cx="2009775" cy="1695450"/>
+        </a:xfrm>
+        <a:prstGeom prst="star6">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Could</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> use the animator to trigger the code use it as a timer</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2192,7 +2251,7 @@
   <dimension ref="A4:Y47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2202,803 +2261,803 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:24" ht="15" customHeight="1">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="102"/>
-      <c r="D4" s="82"/>
-      <c r="G4" s="83" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="G4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="I4" s="82"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1">
-      <c r="B5" s="76"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="75"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="75"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="39"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1">
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="123"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:24" ht="15" customHeight="1">
-      <c r="B8" s="122"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="121"/>
-      <c r="E8" s="120"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="108"/>
-      <c r="I8" s="108"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:24" ht="15" customHeight="1">
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="14"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="83" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="8"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="102"/>
-      <c r="L9" s="82"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="117" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="117"/>
-      <c r="D10" s="117"/>
-      <c r="E10" s="116"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="75"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="109"/>
-      <c r="C11" s="109"/>
-      <c r="D11" s="109"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="114" t="s">
+      <c r="G11" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="113"/>
-      <c r="I11" s="108"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="28"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="109"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="98" t="s">
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="97"/>
-      <c r="N12" s="97"/>
-      <c r="O12" s="97"/>
-      <c r="P12" s="97"/>
-      <c r="Q12" s="97"/>
-      <c r="R12" s="97"/>
-      <c r="S12" s="112"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="51"/>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1">
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="2"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="108"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="85"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85"/>
-      <c r="R13" s="85"/>
-      <c r="S13" s="110"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="54"/>
     </row>
     <row r="14" spans="1:24" ht="15" customHeight="1">
-      <c r="B14" s="109"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="G14" s="108"/>
-      <c r="H14" s="108"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:24" ht="15" customHeight="1">
-      <c r="B15" s="109"/>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="107"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="106" t="s">
+      <c r="Q15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="105"/>
-      <c r="S15" s="105"/>
-      <c r="T15" s="105"/>
-      <c r="U15" s="105"/>
-      <c r="V15" s="105"/>
-      <c r="W15" s="105"/>
-      <c r="X15" s="104"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="56"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="56"/>
+      <c r="X15" s="57"/>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1">
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="103"/>
-      <c r="M16" s="102" t="s">
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="102"/>
-      <c r="O16" s="82"/>
-      <c r="Q16" s="101"/>
-      <c r="R16" s="100"/>
-      <c r="S16" s="100"/>
-      <c r="T16" s="100"/>
-      <c r="U16" s="100"/>
-      <c r="V16" s="100"/>
-      <c r="W16" s="100"/>
-      <c r="X16" s="99"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="36"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="59"/>
+      <c r="S16" s="59"/>
+      <c r="T16" s="59"/>
+      <c r="U16" s="59"/>
+      <c r="V16" s="59"/>
+      <c r="W16" s="59"/>
+      <c r="X16" s="60"/>
     </row>
     <row r="17" spans="1:24" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="97"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="95" t="s">
+      <c r="C17" s="50"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="94"/>
-      <c r="G17" s="93"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="92"/>
-      <c r="M17" s="91"/>
-      <c r="N17" s="91"/>
-      <c r="O17" s="90"/>
-      <c r="Q17" s="89"/>
-      <c r="R17" s="88"/>
-      <c r="S17" s="88"/>
-      <c r="T17" s="88"/>
-      <c r="U17" s="88"/>
-      <c r="V17" s="88"/>
-      <c r="W17" s="88"/>
-      <c r="X17" s="87"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="65"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="62"/>
+      <c r="W17" s="62"/>
+      <c r="X17" s="63"/>
     </row>
     <row r="18" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="86"/>
-      <c r="C18" s="85"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="57" t="s">
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="56"/>
+      <c r="M18" s="70"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
     </row>
     <row r="19" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="83" t="s">
+      <c r="B19" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="82"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="56"/>
+      <c r="C19" s="36"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="70"/>
       <c r="N19" s="6"/>
-      <c r="O19" s="81" t="s">
+      <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="P19" s="80"/>
-      <c r="Q19" s="79" t="s">
+      <c r="P19" s="21"/>
+      <c r="Q19" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="78"/>
-      <c r="S19" s="78"/>
-      <c r="T19" s="78"/>
-      <c r="U19" s="78"/>
-      <c r="V19" s="78"/>
-      <c r="W19" s="78"/>
-      <c r="X19" s="77"/>
+      <c r="R19" s="72"/>
+      <c r="S19" s="72"/>
+      <c r="T19" s="72"/>
+      <c r="U19" s="72"/>
+      <c r="V19" s="72"/>
+      <c r="W19" s="72"/>
+      <c r="X19" s="73"/>
     </row>
     <row r="20" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="76"/>
-      <c r="C20" s="75"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="39"/>
       <c r="F20" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="73"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="57" t="s">
+      <c r="G20" s="75"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="56"/>
+      <c r="M20" s="70"/>
       <c r="N20" s="6"/>
-      <c r="O20" s="23"/>
-      <c r="Q20" s="44" t="s">
+      <c r="O20" s="14"/>
+      <c r="Q20" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="43"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
-      <c r="U20" s="43"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="43"/>
-      <c r="X20" s="42"/>
+      <c r="R20" s="88"/>
+      <c r="S20" s="88"/>
+      <c r="T20" s="88"/>
+      <c r="U20" s="88"/>
+      <c r="V20" s="88"/>
+      <c r="W20" s="88"/>
+      <c r="X20" s="89"/>
     </row>
     <row r="21" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="56"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="70"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="23" t="s">
+      <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="67" t="s">
+      <c r="Q21" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="66"/>
-      <c r="S21" s="66"/>
-      <c r="T21" s="66"/>
-      <c r="U21" s="66"/>
-      <c r="V21" s="66"/>
-      <c r="W21" s="66"/>
-      <c r="X21" s="65"/>
+      <c r="R21" s="91"/>
+      <c r="S21" s="91"/>
+      <c r="T21" s="91"/>
+      <c r="U21" s="91"/>
+      <c r="V21" s="91"/>
+      <c r="W21" s="91"/>
+      <c r="X21" s="92"/>
     </row>
     <row r="22" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="57" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="56"/>
+      <c r="M22" s="70"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="23"/>
-      <c r="X22" s="19"/>
+      <c r="O22" s="14"/>
+      <c r="X22" s="13"/>
     </row>
     <row r="23" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="44" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="43"/>
-      <c r="G23" s="51"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="56"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="93"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="23" t="s">
+      <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="64" t="s">
+      <c r="Q23" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="63"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="63"/>
-      <c r="U23" s="63"/>
-      <c r="V23" s="63"/>
-      <c r="W23" s="63"/>
-      <c r="X23" s="62"/>
+      <c r="R23" s="95"/>
+      <c r="S23" s="95"/>
+      <c r="T23" s="95"/>
+      <c r="U23" s="95"/>
+      <c r="V23" s="95"/>
+      <c r="W23" s="95"/>
+      <c r="X23" s="96"/>
     </row>
     <row r="24" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="57" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="56"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="6"/>
-      <c r="O24" s="23"/>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="60"/>
-      <c r="V24" s="60"/>
-      <c r="W24" s="60"/>
-      <c r="X24" s="59"/>
+      <c r="O24" s="14"/>
+      <c r="Q24" s="97"/>
+      <c r="R24" s="98"/>
+      <c r="S24" s="98"/>
+      <c r="T24" s="98"/>
+      <c r="U24" s="98"/>
+      <c r="V24" s="98"/>
+      <c r="W24" s="98"/>
+      <c r="X24" s="99"/>
     </row>
     <row r="25" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="56"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="70"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="23"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="54"/>
-      <c r="T25" s="54"/>
-      <c r="U25" s="54"/>
-      <c r="V25" s="54"/>
-      <c r="W25" s="54"/>
-      <c r="X25" s="53"/>
+      <c r="O25" s="14"/>
+      <c r="Q25" s="100"/>
+      <c r="R25" s="101"/>
+      <c r="S25" s="101"/>
+      <c r="T25" s="101"/>
+      <c r="U25" s="101"/>
+      <c r="V25" s="101"/>
+      <c r="W25" s="101"/>
+      <c r="X25" s="102"/>
     </row>
     <row r="26" spans="1:24" ht="15" customHeight="1" thickTop="1">
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="51"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="88"/>
+      <c r="K26" s="93"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="23" t="s">
+      <c r="N26" s="12"/>
+      <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="50" t="s">
+      <c r="Q26" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="49"/>
-      <c r="S26" s="49"/>
-      <c r="T26" s="49"/>
-      <c r="U26" s="49"/>
-      <c r="V26" s="49"/>
-      <c r="W26" s="49"/>
-      <c r="X26" s="48"/>
+      <c r="R26" s="110"/>
+      <c r="S26" s="110"/>
+      <c r="T26" s="110"/>
+      <c r="U26" s="110"/>
+      <c r="V26" s="110"/>
+      <c r="W26" s="110"/>
+      <c r="X26" s="111"/>
     </row>
     <row r="27" spans="1:24" ht="15" customHeight="1">
-      <c r="N27" s="18"/>
-      <c r="O27" s="23"/>
-      <c r="Q27" s="47"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="46"/>
-      <c r="T27" s="46"/>
-      <c r="U27" s="46"/>
-      <c r="V27" s="46"/>
-      <c r="W27" s="46"/>
-      <c r="X27" s="45"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="14"/>
+      <c r="Q27" s="112"/>
+      <c r="R27" s="113"/>
+      <c r="S27" s="113"/>
+      <c r="T27" s="113"/>
+      <c r="U27" s="113"/>
+      <c r="V27" s="113"/>
+      <c r="W27" s="113"/>
+      <c r="X27" s="114"/>
     </row>
     <row r="28" spans="1:24" ht="15" customHeight="1">
-      <c r="N28" s="18"/>
-      <c r="O28" s="23"/>
-      <c r="X28" s="19"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="14"/>
+      <c r="X28" s="13"/>
     </row>
     <row r="29" spans="1:24" ht="15" customHeight="1">
-      <c r="N29" s="18"/>
-      <c r="O29" s="23" t="s">
+      <c r="N29" s="12"/>
+      <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="44" t="s">
+      <c r="Q29" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="43"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="43"/>
-      <c r="U29" s="43"/>
-      <c r="V29" s="43"/>
-      <c r="W29" s="43"/>
-      <c r="X29" s="42"/>
+      <c r="R29" s="88"/>
+      <c r="S29" s="88"/>
+      <c r="T29" s="88"/>
+      <c r="U29" s="88"/>
+      <c r="V29" s="88"/>
+      <c r="W29" s="88"/>
+      <c r="X29" s="89"/>
     </row>
     <row r="30" spans="1:24" ht="15" customHeight="1">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="23"/>
-      <c r="X30" s="19"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="14"/>
+      <c r="X30" s="13"/>
     </row>
     <row r="31" spans="1:24" ht="15" customHeight="1">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="37"/>
+      <c r="B31" s="115"/>
+      <c r="C31" s="115"/>
+      <c r="D31" s="115"/>
+      <c r="E31" s="115"/>
+      <c r="F31" s="115"/>
+      <c r="G31" s="115"/>
+      <c r="H31" s="115"/>
+      <c r="I31" s="115"/>
+      <c r="J31" s="115"/>
+      <c r="K31" s="15"/>
       <c r="L31" s="4"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="41" t="s">
+      <c r="N31" s="12"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40"/>
-      <c r="T31" s="40"/>
-      <c r="U31" s="40"/>
-      <c r="V31" s="40"/>
-      <c r="W31" s="39"/>
-      <c r="X31" s="19"/>
+      <c r="Q31" s="117"/>
+      <c r="R31" s="117"/>
+      <c r="S31" s="117"/>
+      <c r="T31" s="117"/>
+      <c r="U31" s="117"/>
+      <c r="V31" s="117"/>
+      <c r="W31" s="118"/>
+      <c r="X31" s="13"/>
     </row>
     <row r="32" spans="1:24" ht="15" customHeight="1">
-      <c r="A32" s="38"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="37"/>
+      <c r="A32" s="115"/>
+      <c r="B32" s="115"/>
+      <c r="C32" s="115"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="115"/>
+      <c r="J32" s="115"/>
+      <c r="K32" s="15"/>
       <c r="L32" s="4"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29"/>
-      <c r="S32" s="29"/>
-      <c r="T32" s="29"/>
-      <c r="U32" s="29"/>
-      <c r="V32" s="29"/>
-      <c r="W32" s="28"/>
-      <c r="X32" s="19"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="119"/>
+      <c r="Q32" s="120"/>
+      <c r="R32" s="120"/>
+      <c r="S32" s="120"/>
+      <c r="T32" s="120"/>
+      <c r="U32" s="120"/>
+      <c r="V32" s="120"/>
+      <c r="W32" s="121"/>
+      <c r="X32" s="13"/>
     </row>
     <row r="33" spans="1:25" ht="15" customHeight="1">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
       <c r="L33" s="4"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="29"/>
-      <c r="R33" s="29"/>
-      <c r="S33" s="29"/>
-      <c r="T33" s="29"/>
-      <c r="U33" s="29"/>
-      <c r="V33" s="29"/>
-      <c r="W33" s="28"/>
-      <c r="X33" s="19"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="119"/>
+      <c r="Q33" s="120"/>
+      <c r="R33" s="120"/>
+      <c r="S33" s="120"/>
+      <c r="T33" s="120"/>
+      <c r="U33" s="120"/>
+      <c r="V33" s="120"/>
+      <c r="W33" s="121"/>
+      <c r="X33" s="13"/>
     </row>
     <row r="34" spans="1:25" ht="15" customHeight="1">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
+      <c r="C34" s="125"/>
+      <c r="D34" s="125"/>
+      <c r="E34" s="125"/>
+      <c r="F34" s="125"/>
+      <c r="G34" s="125"/>
+      <c r="H34" s="125"/>
+      <c r="I34" s="125"/>
+      <c r="J34" s="125"/>
+      <c r="K34" s="125"/>
       <c r="L34" s="4"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="29"/>
-      <c r="R34" s="29"/>
-      <c r="S34" s="29"/>
-      <c r="T34" s="29"/>
-      <c r="U34" s="29"/>
-      <c r="V34" s="29"/>
-      <c r="W34" s="28"/>
-      <c r="X34" s="19"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="119"/>
+      <c r="Q34" s="120"/>
+      <c r="R34" s="120"/>
+      <c r="S34" s="120"/>
+      <c r="T34" s="120"/>
+      <c r="U34" s="120"/>
+      <c r="V34" s="120"/>
+      <c r="W34" s="121"/>
+      <c r="X34" s="13"/>
     </row>
     <row r="35" spans="1:25" ht="15" customHeight="1">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="34"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="80"/>
       <c r="L35" s="4"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="29"/>
-      <c r="S35" s="29"/>
-      <c r="T35" s="29"/>
-      <c r="U35" s="29"/>
-      <c r="V35" s="29"/>
-      <c r="W35" s="28"/>
-      <c r="X35" s="19"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="119"/>
+      <c r="Q35" s="120"/>
+      <c r="R35" s="120"/>
+      <c r="S35" s="120"/>
+      <c r="T35" s="120"/>
+      <c r="U35" s="120"/>
+      <c r="V35" s="120"/>
+      <c r="W35" s="121"/>
+      <c r="X35" s="13"/>
     </row>
     <row r="36" spans="1:25" ht="15" customHeight="1">
-      <c r="A36" s="27"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="31"/>
+      <c r="A36" s="125"/>
+      <c r="B36" s="81"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="83"/>
       <c r="L36" s="4"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="29"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
-      <c r="V36" s="29"/>
-      <c r="W36" s="28"/>
-      <c r="X36" s="19"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="119"/>
+      <c r="Q36" s="120"/>
+      <c r="R36" s="120"/>
+      <c r="S36" s="120"/>
+      <c r="T36" s="120"/>
+      <c r="U36" s="120"/>
+      <c r="V36" s="120"/>
+      <c r="W36" s="121"/>
+      <c r="X36" s="13"/>
     </row>
     <row r="37" spans="1:25" ht="15" customHeight="1">
-      <c r="A37" s="27"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="24"/>
+      <c r="A37" s="125"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="86"/>
       <c r="L37" s="4"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="21"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="21"/>
-      <c r="V37" s="21"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="19"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="122"/>
+      <c r="Q37" s="123"/>
+      <c r="R37" s="123"/>
+      <c r="S37" s="123"/>
+      <c r="T37" s="123"/>
+      <c r="U37" s="123"/>
+      <c r="V37" s="123"/>
+      <c r="W37" s="124"/>
+      <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:25" ht="15" customHeight="1" thickBot="1">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="7"/>
+      <c r="C38" s="107"/>
+      <c r="D38" s="107"/>
+      <c r="E38" s="107"/>
+      <c r="F38" s="107"/>
+      <c r="G38" s="107"/>
+      <c r="H38" s="107"/>
+      <c r="I38" s="107"/>
+      <c r="J38" s="107"/>
+      <c r="K38" s="108"/>
       <c r="L38" s="4"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="16"/>
-      <c r="Q38" s="16"/>
-      <c r="R38" s="16"/>
-      <c r="S38" s="16"/>
-      <c r="T38" s="16"/>
-      <c r="U38" s="16"/>
-      <c r="V38" s="16"/>
-      <c r="W38" s="16"/>
-      <c r="X38" s="15"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="9"/>
     </row>
     <row r="39" spans="1:25" ht="15" customHeight="1">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="7"/>
+      <c r="C39" s="107"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="107"/>
+      <c r="F39" s="107"/>
+      <c r="G39" s="107"/>
+      <c r="H39" s="107"/>
+      <c r="I39" s="107"/>
+      <c r="J39" s="107"/>
+      <c r="K39" s="108"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:25" ht="15" customHeight="1">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="7"/>
+      <c r="C40" s="107"/>
+      <c r="D40" s="107"/>
+      <c r="E40" s="107"/>
+      <c r="F40" s="107"/>
+      <c r="G40" s="107"/>
+      <c r="H40" s="107"/>
+      <c r="I40" s="107"/>
+      <c r="J40" s="107"/>
+      <c r="K40" s="108"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
-      <c r="X40" s="14"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
     </row>
     <row r="41" spans="1:25" ht="15" customHeight="1">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="7"/>
+      <c r="C41" s="107"/>
+      <c r="D41" s="107"/>
+      <c r="E41" s="107"/>
+      <c r="F41" s="107"/>
+      <c r="G41" s="107"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="107"/>
+      <c r="K41" s="108"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="13" t="s">
+      <c r="M41" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="12"/>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="12"/>
-      <c r="S41" s="12"/>
-      <c r="T41" s="12"/>
-      <c r="U41" s="12"/>
-      <c r="V41" s="12"/>
-      <c r="W41" s="12"/>
-      <c r="X41" s="11"/>
+      <c r="N41" s="104"/>
+      <c r="O41" s="104"/>
+      <c r="P41" s="104"/>
+      <c r="Q41" s="104"/>
+      <c r="R41" s="104"/>
+      <c r="S41" s="104"/>
+      <c r="T41" s="104"/>
+      <c r="U41" s="104"/>
+      <c r="V41" s="104"/>
+      <c r="W41" s="104"/>
+      <c r="X41" s="105"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:25" ht="15" customHeight="1">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="7"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="106"/>
+      <c r="C42" s="107"/>
+      <c r="D42" s="107"/>
+      <c r="E42" s="107"/>
+      <c r="F42" s="107"/>
+      <c r="G42" s="107"/>
+      <c r="H42" s="107"/>
+      <c r="I42" s="107"/>
+      <c r="J42" s="107"/>
+      <c r="K42" s="108"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="13" t="s">
+      <c r="M42" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="12"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="12"/>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="12"/>
-      <c r="S42" s="12"/>
-      <c r="T42" s="12"/>
-      <c r="U42" s="12"/>
-      <c r="V42" s="12"/>
-      <c r="W42" s="12"/>
-      <c r="X42" s="11"/>
+      <c r="N42" s="104"/>
+      <c r="O42" s="104"/>
+      <c r="P42" s="104"/>
+      <c r="Q42" s="104"/>
+      <c r="R42" s="104"/>
+      <c r="S42" s="104"/>
+      <c r="T42" s="104"/>
+      <c r="U42" s="104"/>
+      <c r="V42" s="104"/>
+      <c r="W42" s="104"/>
+      <c r="X42" s="105"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:25" ht="15" customHeight="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="7"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="106"/>
+      <c r="C43" s="107"/>
+      <c r="D43" s="107"/>
+      <c r="E43" s="107"/>
+      <c r="F43" s="107"/>
+      <c r="G43" s="107"/>
+      <c r="H43" s="107"/>
+      <c r="I43" s="107"/>
+      <c r="J43" s="107"/>
+      <c r="K43" s="108"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -3015,17 +3074,17 @@
       <c r="Y43" s="4"/>
     </row>
     <row r="44" spans="1:25" ht="15" customHeight="1">
-      <c r="A44" s="10"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="7"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="106"/>
+      <c r="C44" s="107"/>
+      <c r="D44" s="107"/>
+      <c r="E44" s="107"/>
+      <c r="F44" s="107"/>
+      <c r="G44" s="107"/>
+      <c r="H44" s="107"/>
+      <c r="I44" s="107"/>
+      <c r="J44" s="107"/>
+      <c r="K44" s="108"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -3042,17 +3101,17 @@
       <c r="Y44" s="4"/>
     </row>
     <row r="45" spans="1:25" ht="15" customHeight="1">
-      <c r="A45" s="10"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="7"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="106"/>
+      <c r="C45" s="107"/>
+      <c r="D45" s="107"/>
+      <c r="E45" s="107"/>
+      <c r="F45" s="107"/>
+      <c r="G45" s="107"/>
+      <c r="H45" s="107"/>
+      <c r="I45" s="107"/>
+      <c r="J45" s="107"/>
+      <c r="K45" s="108"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -3069,17 +3128,17 @@
       <c r="Y45" s="4"/>
     </row>
     <row r="46" spans="1:25" ht="15" customHeight="1">
-      <c r="A46" s="10"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="7"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="106"/>
+      <c r="C46" s="107"/>
+      <c r="D46" s="107"/>
+      <c r="E46" s="107"/>
+      <c r="F46" s="107"/>
+      <c r="G46" s="107"/>
+      <c r="H46" s="107"/>
+      <c r="I46" s="107"/>
+      <c r="J46" s="107"/>
+      <c r="K46" s="108"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -3122,11 +3181,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="J9:L10"/>
-    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="M41:X41"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="M42:X42"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="Q26:X27"/>
+    <mergeCell ref="Q29:X29"/>
+    <mergeCell ref="A31:J32"/>
+    <mergeCell ref="P31:W37"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:K37"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="L12:S13"/>
     <mergeCell ref="Q15:X17"/>
@@ -3138,46 +3217,14 @@
     <mergeCell ref="Q19:X19"/>
     <mergeCell ref="F20:G21"/>
     <mergeCell ref="L20:M21"/>
-    <mergeCell ref="B35:K37"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="M41:X41"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="M42:X42"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="Q26:X27"/>
-    <mergeCell ref="Q29:X29"/>
-    <mergeCell ref="A31:J32"/>
-    <mergeCell ref="P31:W37"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="J9:L10"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
simplified the shrink for chose team stage is nicer now
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -1157,22 +1157,259 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1194,243 +1431,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1960,6 +1960,66 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="6-Point Star 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10791826" y="695325"/>
+          <a:ext cx="2667000" cy="1704975"/>
+        </a:xfrm>
+        <a:prstGeom prst="star6">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>could</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> use broadcast message to have loads methods syncronize e.g. DoYourStage1Method()</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2250,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2261,41 +2321,41 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:24" ht="15" customHeight="1">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="G4" s="34" t="s">
+      <c r="C4" s="101"/>
+      <c r="D4" s="102"/>
+      <c r="G4" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="102"/>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="110"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="110"/>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="121"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:24" ht="15" customHeight="1">
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="124"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2308,27 +2368,27 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="102"/>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="125" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
+      <c r="J10" s="109"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="110"/>
     </row>
     <row r="11" spans="1:24" ht="15" customHeight="1">
       <c r="A11" s="12"/>
@@ -2336,10 +2396,10 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="48"/>
+      <c r="H11" s="85"/>
       <c r="I11" s="28"/>
     </row>
     <row r="12" spans="1:24" ht="15" customHeight="1">
@@ -2353,16 +2413,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="49" t="s">
+      <c r="L12" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="51"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="87"/>
+      <c r="S12" s="88"/>
     </row>
     <row r="13" spans="1:24" ht="15" customHeight="1">
       <c r="B13" s="30"/>
@@ -2374,14 +2434,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="53"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="54"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
+      <c r="O13" s="90"/>
+      <c r="P13" s="90"/>
+      <c r="Q13" s="90"/>
+      <c r="R13" s="90"/>
+      <c r="S13" s="91"/>
     </row>
     <row r="14" spans="1:24" ht="15" customHeight="1">
       <c r="B14" s="29"/>
@@ -2403,76 +2463,76 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="55" t="s">
+      <c r="Q15" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="56"/>
-      <c r="V15" s="56"/>
-      <c r="W15" s="56"/>
-      <c r="X15" s="57"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="93"/>
+      <c r="T15" s="93"/>
+      <c r="U15" s="93"/>
+      <c r="V15" s="93"/>
+      <c r="W15" s="93"/>
+      <c r="X15" s="94"/>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1">
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="35" t="s">
+      <c r="M16" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="35"/>
-      <c r="O16" s="36"/>
-      <c r="Q16" s="58"/>
-      <c r="R16" s="59"/>
-      <c r="S16" s="59"/>
-      <c r="T16" s="59"/>
-      <c r="U16" s="59"/>
-      <c r="V16" s="59"/>
-      <c r="W16" s="59"/>
-      <c r="X16" s="60"/>
+      <c r="N16" s="101"/>
+      <c r="O16" s="102"/>
+      <c r="Q16" s="95"/>
+      <c r="R16" s="96"/>
+      <c r="S16" s="96"/>
+      <c r="T16" s="96"/>
+      <c r="U16" s="96"/>
+      <c r="V16" s="96"/>
+      <c r="W16" s="96"/>
+      <c r="X16" s="97"/>
     </row>
     <row r="17" spans="1:24" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="87"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="66" t="s">
+      <c r="E17" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="68"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="107"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="65"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="62"/>
-      <c r="V17" s="62"/>
-      <c r="W17" s="62"/>
-      <c r="X17" s="63"/>
+      <c r="M17" s="103"/>
+      <c r="N17" s="103"/>
+      <c r="O17" s="104"/>
+      <c r="Q17" s="98"/>
+      <c r="R17" s="99"/>
+      <c r="S17" s="99"/>
+      <c r="T17" s="99"/>
+      <c r="U17" s="99"/>
+      <c r="V17" s="99"/>
+      <c r="W17" s="99"/>
+      <c r="X17" s="100"/>
     </row>
     <row r="18" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="90"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="69" t="s">
+      <c r="L18" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="70"/>
+      <c r="M18" s="74"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -2486,97 +2546,97 @@
       <c r="X18" s="8"/>
     </row>
     <row r="19" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="102"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="70"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="74"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="71" t="s">
+      <c r="Q19" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="72"/>
-      <c r="S19" s="72"/>
-      <c r="T19" s="72"/>
-      <c r="U19" s="72"/>
-      <c r="V19" s="72"/>
-      <c r="W19" s="72"/>
-      <c r="X19" s="73"/>
+      <c r="R19" s="112"/>
+      <c r="S19" s="112"/>
+      <c r="T19" s="112"/>
+      <c r="U19" s="112"/>
+      <c r="V19" s="112"/>
+      <c r="W19" s="112"/>
+      <c r="X19" s="113"/>
     </row>
     <row r="20" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="37"/>
-      <c r="C20" s="39"/>
-      <c r="F20" s="74" t="s">
+      <c r="B20" s="109"/>
+      <c r="C20" s="110"/>
+      <c r="F20" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="75"/>
+      <c r="G20" s="115"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="69" t="s">
+      <c r="L20" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="70"/>
+      <c r="M20" s="74"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="87" t="s">
+      <c r="Q20" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="88"/>
-      <c r="S20" s="88"/>
-      <c r="T20" s="88"/>
-      <c r="U20" s="88"/>
-      <c r="V20" s="88"/>
-      <c r="W20" s="88"/>
-      <c r="X20" s="89"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="49"/>
     </row>
     <row r="21" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="77"/>
+      <c r="F21" s="116"/>
+      <c r="G21" s="117"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="70"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="74"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="90" t="s">
+      <c r="Q21" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="91"/>
-      <c r="S21" s="91"/>
-      <c r="T21" s="91"/>
-      <c r="U21" s="91"/>
-      <c r="V21" s="91"/>
-      <c r="W21" s="91"/>
-      <c r="X21" s="92"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="71"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="71"/>
+      <c r="V21" s="71"/>
+      <c r="W21" s="71"/>
+      <c r="X21" s="72"/>
     </row>
     <row r="22" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="69" t="s">
+      <c r="L22" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="70"/>
+      <c r="M22" s="74"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -2585,103 +2645,103 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="87" t="s">
+      <c r="E23" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="88"/>
-      <c r="G23" s="93"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="42"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="70"/>
+      <c r="L23" s="73"/>
+      <c r="M23" s="74"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="94" t="s">
+      <c r="Q23" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="95"/>
-      <c r="S23" s="95"/>
-      <c r="T23" s="95"/>
-      <c r="U23" s="95"/>
-      <c r="V23" s="95"/>
-      <c r="W23" s="95"/>
-      <c r="X23" s="96"/>
+      <c r="R23" s="76"/>
+      <c r="S23" s="76"/>
+      <c r="T23" s="76"/>
+      <c r="U23" s="76"/>
+      <c r="V23" s="76"/>
+      <c r="W23" s="76"/>
+      <c r="X23" s="77"/>
     </row>
     <row r="24" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="69" t="s">
+      <c r="L24" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="70"/>
+      <c r="M24" s="74"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="97"/>
-      <c r="R24" s="98"/>
-      <c r="S24" s="98"/>
-      <c r="T24" s="98"/>
-      <c r="U24" s="98"/>
-      <c r="V24" s="98"/>
-      <c r="W24" s="98"/>
-      <c r="X24" s="99"/>
+      <c r="Q24" s="78"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="79"/>
+      <c r="T24" s="79"/>
+      <c r="U24" s="79"/>
+      <c r="V24" s="79"/>
+      <c r="W24" s="79"/>
+      <c r="X24" s="80"/>
     </row>
     <row r="25" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="100"/>
-      <c r="R25" s="101"/>
-      <c r="S25" s="101"/>
-      <c r="T25" s="101"/>
-      <c r="U25" s="101"/>
-      <c r="V25" s="101"/>
-      <c r="W25" s="101"/>
-      <c r="X25" s="102"/>
+      <c r="Q25" s="81"/>
+      <c r="R25" s="82"/>
+      <c r="S25" s="82"/>
+      <c r="T25" s="82"/>
+      <c r="U25" s="82"/>
+      <c r="V25" s="82"/>
+      <c r="W25" s="82"/>
+      <c r="X25" s="83"/>
     </row>
     <row r="26" spans="1:24" ht="15" customHeight="1" thickTop="1">
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="93"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="42"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="109" t="s">
+      <c r="Q26" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="110"/>
-      <c r="S26" s="110"/>
-      <c r="T26" s="110"/>
-      <c r="U26" s="110"/>
-      <c r="V26" s="110"/>
-      <c r="W26" s="110"/>
-      <c r="X26" s="111"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="44"/>
+      <c r="X26" s="45"/>
     </row>
     <row r="27" spans="1:24" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="112"/>
-      <c r="R27" s="113"/>
-      <c r="S27" s="113"/>
-      <c r="T27" s="113"/>
-      <c r="U27" s="113"/>
-      <c r="V27" s="113"/>
-      <c r="W27" s="113"/>
-      <c r="X27" s="114"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="47"/>
+      <c r="T27" s="47"/>
+      <c r="U27" s="47"/>
+      <c r="V27" s="47"/>
+      <c r="W27" s="47"/>
+      <c r="X27" s="48"/>
     </row>
     <row r="28" spans="1:24" ht="15" customHeight="1">
       <c r="N28" s="12"/>
@@ -2693,16 +2753,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="87" t="s">
+      <c r="Q29" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="88"/>
-      <c r="S29" s="88"/>
-      <c r="T29" s="88"/>
-      <c r="U29" s="88"/>
-      <c r="V29" s="88"/>
-      <c r="W29" s="88"/>
-      <c r="X29" s="89"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="49"/>
     </row>
     <row r="30" spans="1:24" ht="15" customHeight="1">
       <c r="A30" s="8"/>
@@ -2721,57 +2781,57 @@
       <c r="X30" s="13"/>
     </row>
     <row r="31" spans="1:24" ht="15" customHeight="1">
-      <c r="A31" s="115" t="s">
+      <c r="A31" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="115"/>
-      <c r="C31" s="115"/>
-      <c r="D31" s="115"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="115"/>
-      <c r="H31" s="115"/>
-      <c r="I31" s="115"/>
-      <c r="J31" s="115"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="116" t="s">
+      <c r="P31" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="117"/>
-      <c r="R31" s="117"/>
-      <c r="S31" s="117"/>
-      <c r="T31" s="117"/>
-      <c r="U31" s="117"/>
-      <c r="V31" s="117"/>
-      <c r="W31" s="118"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="52"/>
+      <c r="S31" s="52"/>
+      <c r="T31" s="52"/>
+      <c r="U31" s="52"/>
+      <c r="V31" s="52"/>
+      <c r="W31" s="53"/>
       <c r="X31" s="13"/>
     </row>
     <row r="32" spans="1:24" ht="15" customHeight="1">
-      <c r="A32" s="115"/>
-      <c r="B32" s="115"/>
-      <c r="C32" s="115"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="115"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="115"/>
-      <c r="H32" s="115"/>
-      <c r="I32" s="115"/>
-      <c r="J32" s="115"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="119"/>
-      <c r="Q32" s="120"/>
-      <c r="R32" s="120"/>
-      <c r="S32" s="120"/>
-      <c r="T32" s="120"/>
-      <c r="U32" s="120"/>
-      <c r="V32" s="120"/>
-      <c r="W32" s="121"/>
+      <c r="P32" s="54"/>
+      <c r="Q32" s="55"/>
+      <c r="R32" s="55"/>
+      <c r="S32" s="55"/>
+      <c r="T32" s="55"/>
+      <c r="U32" s="55"/>
+      <c r="V32" s="55"/>
+      <c r="W32" s="56"/>
       <c r="X32" s="13"/>
     </row>
     <row r="33" spans="1:25" ht="15" customHeight="1">
@@ -2789,140 +2849,140 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="119"/>
-      <c r="Q33" s="120"/>
-      <c r="R33" s="120"/>
-      <c r="S33" s="120"/>
-      <c r="T33" s="120"/>
-      <c r="U33" s="120"/>
-      <c r="V33" s="120"/>
-      <c r="W33" s="121"/>
+      <c r="P33" s="54"/>
+      <c r="Q33" s="55"/>
+      <c r="R33" s="55"/>
+      <c r="S33" s="55"/>
+      <c r="T33" s="55"/>
+      <c r="U33" s="55"/>
+      <c r="V33" s="55"/>
+      <c r="W33" s="56"/>
       <c r="X33" s="13"/>
     </row>
     <row r="34" spans="1:25" ht="15" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="125" t="s">
+      <c r="B34" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="125"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="125"/>
-      <c r="F34" s="125"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="125"/>
-      <c r="I34" s="125"/>
-      <c r="J34" s="125"/>
-      <c r="K34" s="125"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="119"/>
-      <c r="Q34" s="120"/>
-      <c r="R34" s="120"/>
-      <c r="S34" s="120"/>
-      <c r="T34" s="120"/>
-      <c r="U34" s="120"/>
-      <c r="V34" s="120"/>
-      <c r="W34" s="121"/>
+      <c r="P34" s="54"/>
+      <c r="Q34" s="55"/>
+      <c r="R34" s="55"/>
+      <c r="S34" s="55"/>
+      <c r="T34" s="55"/>
+      <c r="U34" s="55"/>
+      <c r="V34" s="55"/>
+      <c r="W34" s="56"/>
       <c r="X34" s="13"/>
     </row>
     <row r="35" spans="1:25" ht="15" customHeight="1">
-      <c r="A35" s="125" t="s">
+      <c r="A35" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="78" t="s">
+      <c r="B35" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="80"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="63"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="119"/>
-      <c r="Q35" s="120"/>
-      <c r="R35" s="120"/>
-      <c r="S35" s="120"/>
-      <c r="T35" s="120"/>
-      <c r="U35" s="120"/>
-      <c r="V35" s="120"/>
-      <c r="W35" s="121"/>
+      <c r="P35" s="54"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="55"/>
+      <c r="T35" s="55"/>
+      <c r="U35" s="55"/>
+      <c r="V35" s="55"/>
+      <c r="W35" s="56"/>
       <c r="X35" s="13"/>
     </row>
     <row r="36" spans="1:25" ht="15" customHeight="1">
-      <c r="A36" s="125"/>
-      <c r="B36" s="81"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="82"/>
-      <c r="K36" s="83"/>
+      <c r="A36" s="60"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="66"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="119"/>
-      <c r="Q36" s="120"/>
-      <c r="R36" s="120"/>
-      <c r="S36" s="120"/>
-      <c r="T36" s="120"/>
-      <c r="U36" s="120"/>
-      <c r="V36" s="120"/>
-      <c r="W36" s="121"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="55"/>
+      <c r="U36" s="55"/>
+      <c r="V36" s="55"/>
+      <c r="W36" s="56"/>
       <c r="X36" s="13"/>
     </row>
     <row r="37" spans="1:25" ht="15" customHeight="1">
-      <c r="A37" s="125"/>
-      <c r="B37" s="84"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
-      <c r="F37" s="85"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="85"/>
-      <c r="J37" s="85"/>
-      <c r="K37" s="86"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="68"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="69"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="122"/>
-      <c r="Q37" s="123"/>
-      <c r="R37" s="123"/>
-      <c r="S37" s="123"/>
-      <c r="T37" s="123"/>
-      <c r="U37" s="123"/>
-      <c r="V37" s="123"/>
-      <c r="W37" s="124"/>
+      <c r="P37" s="57"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
+      <c r="T37" s="58"/>
+      <c r="U37" s="58"/>
+      <c r="V37" s="58"/>
+      <c r="W37" s="59"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:25" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="106" t="s">
+      <c r="B38" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="107"/>
-      <c r="F38" s="107"/>
-      <c r="G38" s="107"/>
-      <c r="H38" s="107"/>
-      <c r="I38" s="107"/>
-      <c r="J38" s="107"/>
-      <c r="K38" s="108"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="36"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -2940,36 +3000,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="106" t="s">
+      <c r="B39" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="107"/>
-      <c r="D39" s="107"/>
-      <c r="E39" s="107"/>
-      <c r="F39" s="107"/>
-      <c r="G39" s="107"/>
-      <c r="H39" s="107"/>
-      <c r="I39" s="107"/>
-      <c r="J39" s="107"/>
-      <c r="K39" s="108"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="36"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:25" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="106" t="s">
+      <c r="B40" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="107"/>
-      <c r="F40" s="107"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="107"/>
-      <c r="I40" s="107"/>
-      <c r="J40" s="107"/>
-      <c r="K40" s="108"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="36"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -2988,76 +3048,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="106" t="s">
+      <c r="B41" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="107"/>
-      <c r="D41" s="107"/>
-      <c r="E41" s="107"/>
-      <c r="F41" s="107"/>
-      <c r="G41" s="107"/>
-      <c r="H41" s="107"/>
-      <c r="I41" s="107"/>
-      <c r="J41" s="107"/>
-      <c r="K41" s="108"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="36"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="103" t="s">
+      <c r="M41" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="104"/>
-      <c r="O41" s="104"/>
-      <c r="P41" s="104"/>
-      <c r="Q41" s="104"/>
-      <c r="R41" s="104"/>
-      <c r="S41" s="104"/>
-      <c r="T41" s="104"/>
-      <c r="U41" s="104"/>
-      <c r="V41" s="104"/>
-      <c r="W41" s="104"/>
-      <c r="X41" s="105"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="38"/>
+      <c r="S41" s="38"/>
+      <c r="T41" s="38"/>
+      <c r="U41" s="38"/>
+      <c r="V41" s="38"/>
+      <c r="W41" s="38"/>
+      <c r="X41" s="39"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:25" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="106"/>
-      <c r="C42" s="107"/>
-      <c r="D42" s="107"/>
-      <c r="E42" s="107"/>
-      <c r="F42" s="107"/>
-      <c r="G42" s="107"/>
-      <c r="H42" s="107"/>
-      <c r="I42" s="107"/>
-      <c r="J42" s="107"/>
-      <c r="K42" s="108"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="36"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="103" t="s">
+      <c r="M42" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="104"/>
-      <c r="O42" s="104"/>
-      <c r="P42" s="104"/>
-      <c r="Q42" s="104"/>
-      <c r="R42" s="104"/>
-      <c r="S42" s="104"/>
-      <c r="T42" s="104"/>
-      <c r="U42" s="104"/>
-      <c r="V42" s="104"/>
-      <c r="W42" s="104"/>
-      <c r="X42" s="105"/>
+      <c r="N42" s="38"/>
+      <c r="O42" s="38"/>
+      <c r="P42" s="38"/>
+      <c r="Q42" s="38"/>
+      <c r="R42" s="38"/>
+      <c r="S42" s="38"/>
+      <c r="T42" s="38"/>
+      <c r="U42" s="38"/>
+      <c r="V42" s="38"/>
+      <c r="W42" s="38"/>
+      <c r="X42" s="39"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:25" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="106"/>
-      <c r="C43" s="107"/>
-      <c r="D43" s="107"/>
-      <c r="E43" s="107"/>
-      <c r="F43" s="107"/>
-      <c r="G43" s="107"/>
-      <c r="H43" s="107"/>
-      <c r="I43" s="107"/>
-      <c r="J43" s="107"/>
-      <c r="K43" s="108"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="36"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -3075,16 +3135,16 @@
     </row>
     <row r="44" spans="1:25" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="106"/>
-      <c r="C44" s="107"/>
-      <c r="D44" s="107"/>
-      <c r="E44" s="107"/>
-      <c r="F44" s="107"/>
-      <c r="G44" s="107"/>
-      <c r="H44" s="107"/>
-      <c r="I44" s="107"/>
-      <c r="J44" s="107"/>
-      <c r="K44" s="108"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="36"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -3102,16 +3162,16 @@
     </row>
     <row r="45" spans="1:25" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="106"/>
-      <c r="C45" s="107"/>
-      <c r="D45" s="107"/>
-      <c r="E45" s="107"/>
-      <c r="F45" s="107"/>
-      <c r="G45" s="107"/>
-      <c r="H45" s="107"/>
-      <c r="I45" s="107"/>
-      <c r="J45" s="107"/>
-      <c r="K45" s="108"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="36"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -3129,16 +3189,16 @@
     </row>
     <row r="46" spans="1:25" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="106"/>
-      <c r="C46" s="107"/>
-      <c r="D46" s="107"/>
-      <c r="E46" s="107"/>
-      <c r="F46" s="107"/>
-      <c r="G46" s="107"/>
-      <c r="H46" s="107"/>
-      <c r="I46" s="107"/>
-      <c r="J46" s="107"/>
-      <c r="K46" s="108"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="36"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -3181,14 +3241,28 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="J9:L10"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="Q19:X19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
     <mergeCell ref="M41:X41"/>
     <mergeCell ref="B42:K42"/>
     <mergeCell ref="M42:X42"/>
@@ -3200,28 +3274,14 @@
     <mergeCell ref="B34:K34"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:K37"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="Q19:X19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="J9:L10"/>
-    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
So trying to code the recognising that someone is trying to initiate start up sequence
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -171,6 +171,96 @@
   </si>
   <si>
     <t>Organiser Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stage 0 </t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>check for first player</t>
+  </si>
+  <si>
+    <t>trigger next stage</t>
+  </si>
+  <si>
+    <t>stage 1</t>
+  </si>
+  <si>
+    <t>check for other players</t>
+  </si>
+  <si>
+    <t>stage 2</t>
+  </si>
+  <si>
+    <t>time to do</t>
+  </si>
+  <si>
+    <t>chose team</t>
+  </si>
+  <si>
+    <t>set max</t>
+  </si>
+  <si>
+    <t>timer</t>
+  </si>
+  <si>
+    <t>Process to catch issues</t>
+  </si>
+  <si>
+    <t>reset process with flash up of explosion " no one rowed and the dock blowed"</t>
+  </si>
+  <si>
+    <t>reset process with flash up of explosion " no one rowed and the dock blowed" affordance maybe put a n explosion over the left panel when timer runs out so ppl watching get it</t>
+  </si>
+  <si>
+    <t>Later</t>
+  </si>
+  <si>
+    <t>minimal viable product</t>
+  </si>
+  <si>
+    <t>max too low using defaults (woody sets defaults in set up screen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Play! () </t>
+  </si>
+  <si>
+    <t>give a reset option (surrender?)</t>
+  </si>
+  <si>
+    <t>who to triggered</t>
+  </si>
+  <si>
+    <t>both bar needs to be green (si ti clear need to cycle twice if you start process  if not use text, e.g. Two sets of rower to light the fuse and start the war) - then everyone run to the wharfs</t>
+  </si>
+  <si>
+    <t>bigCounter selectors</t>
+  </si>
+  <si>
+    <t>shrink, activate arrow, activate panel, big timer, mini timer</t>
+  </si>
+  <si>
+    <t>both players peddling - enough to rotate match</t>
+  </si>
+  <si>
+    <t>match rotation</t>
+  </si>
+  <si>
+    <t>set in the event settings</t>
+  </si>
+  <si>
+    <t>21 3x7</t>
+  </si>
+  <si>
+    <t>want &lt; 1 min</t>
+  </si>
+  <si>
+    <t>deactivate arrow, activate max bar big timer</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1146,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1157,155 +1247,44 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1357,12 +1336,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1379,13 +1352,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1409,28 +1379,181 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -2020,6 +2143,53 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15059025" y="390525"/>
+          <a:ext cx="257175" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2308,59 +2478,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:Y47"/>
+  <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AL27" sqref="AL27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="27" width="9.140625" style="1"/>
+    <col min="28" max="28" width="30.85546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="34.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="39.85546875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="78.42578125" style="128" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:24" ht="15" customHeight="1">
-      <c r="B4" s="108" t="s">
+    <row r="1" spans="1:37" ht="15" customHeight="1">
+      <c r="Y1" s="131" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="132"/>
+    </row>
+    <row r="2" spans="1:37" ht="15" customHeight="1">
+      <c r="Y2" s="133"/>
+      <c r="Z2" s="134"/>
+      <c r="AF2" s="127"/>
+      <c r="AG2" s="127"/>
+      <c r="AH2" s="127"/>
+      <c r="AI2" s="127"/>
+      <c r="AJ2" s="127"/>
+      <c r="AK2" s="127"/>
+    </row>
+    <row r="3" spans="1:37" ht="15" customHeight="1">
+      <c r="Y3" s="135"/>
+      <c r="Z3" s="136"/>
+      <c r="AA3" s="126"/>
+      <c r="AB3" s="130" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC3" s="126"/>
+      <c r="AD3" s="126"/>
+      <c r="AE3" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF3" s="127"/>
+      <c r="AG3" s="127"/>
+      <c r="AH3" s="127"/>
+      <c r="AI3" s="127"/>
+      <c r="AJ3" s="127"/>
+      <c r="AK3" s="127"/>
+    </row>
+    <row r="4" spans="1:37" ht="15" customHeight="1">
+      <c r="B4" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="102"/>
-      <c r="G4" s="108" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="G4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="101"/>
-      <c r="I4" s="102"/>
-    </row>
-    <row r="5" spans="1:24" ht="15" customHeight="1">
-      <c r="B5" s="109"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="110"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="110"/>
-    </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1">
-      <c r="B7" s="119" t="s">
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+      <c r="Z4" s="126"/>
+      <c r="AA4" s="126"/>
+      <c r="AB4" s="126"/>
+      <c r="AC4" s="126"/>
+      <c r="AD4" s="126"/>
+      <c r="AF4" s="127"/>
+      <c r="AG4" s="127"/>
+      <c r="AH4" s="127"/>
+      <c r="AI4" s="127"/>
+      <c r="AJ4" s="127"/>
+      <c r="AK4" s="127"/>
+    </row>
+    <row r="5" spans="1:37" ht="15" customHeight="1">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="39"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="39"/>
+      <c r="Z5" s="126" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA5" s="126"/>
+      <c r="AB5" s="126"/>
+      <c r="AC5" s="126"/>
+      <c r="AD5" s="126"/>
+      <c r="AF5" s="127"/>
+      <c r="AG5" s="127"/>
+      <c r="AH5" s="127"/>
+      <c r="AI5" s="127"/>
+      <c r="AJ5" s="127"/>
+      <c r="AK5" s="127"/>
+    </row>
+    <row r="6" spans="1:37" ht="15" customHeight="1">
+      <c r="Z6" s="126" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA6" s="126" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB6" s="126" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="126" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD6" s="126" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE6" s="127" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF6" s="127"/>
+      <c r="AG6" s="127"/>
+      <c r="AH6" s="127"/>
+      <c r="AI6" s="127"/>
+      <c r="AJ6" s="127"/>
+      <c r="AK6" s="127"/>
+    </row>
+    <row r="7" spans="1:37" ht="15" customHeight="1">
+      <c r="B7" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="120"/>
-      <c r="D7" s="120"/>
-      <c r="E7" s="121"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1">
-      <c r="B8" s="122"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="124"/>
+      <c r="Z7" s="126" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA7" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB7" s="126" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC7" s="126" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD7" s="126" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE7" s="128" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF7" s="127"/>
+      <c r="AG7" s="127"/>
+      <c r="AH7" s="127"/>
+      <c r="AI7" s="127"/>
+      <c r="AJ7" s="127"/>
+      <c r="AK7" s="127"/>
+    </row>
+    <row r="8" spans="1:37" ht="15" customHeight="1">
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
-    </row>
-    <row r="9" spans="1:24" ht="15" customHeight="1">
+      <c r="Z8" s="126">
+        <v>10</v>
+      </c>
+      <c r="AA8" s="126" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB8" s="126" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC8" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD8" s="126" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE8" s="128" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF8" s="127"/>
+      <c r="AG8" s="127"/>
+      <c r="AH8" s="127"/>
+      <c r="AI8" s="127"/>
+      <c r="AJ8" s="127"/>
+      <c r="AK8" s="127"/>
+    </row>
+    <row r="9" spans="1:37" ht="15" customHeight="1">
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
@@ -2368,41 +2676,111 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="108" t="s">
+      <c r="J9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="101"/>
-      <c r="L9" s="102"/>
-    </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1">
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
+      <c r="Z9" s="126" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA9" s="126" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB9" s="126" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC9" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="126" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE9" s="128" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF9" s="127"/>
+      <c r="AG9" s="127"/>
+      <c r="AH9" s="127"/>
+      <c r="AI9" s="127"/>
+      <c r="AJ9" s="127"/>
+      <c r="AK9" s="127"/>
+    </row>
+    <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="125" t="s">
+      <c r="B10" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="109"/>
-      <c r="K10" s="118"/>
-      <c r="L10" s="110"/>
-    </row>
-    <row r="11" spans="1:24" ht="15" customHeight="1">
+      <c r="J10" s="37"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+      <c r="Z10" s="126">
+        <v>20</v>
+      </c>
+      <c r="AA10" s="126" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB10" s="126" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC10" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD10" s="126" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE10" s="128" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF10" s="127"/>
+      <c r="AG10" s="127"/>
+      <c r="AH10" s="127"/>
+      <c r="AI10" s="127"/>
+      <c r="AJ10" s="127"/>
+      <c r="AK10" s="127"/>
+    </row>
+    <row r="11" spans="1:37" ht="15" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="84" t="s">
+      <c r="G11" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="85"/>
+      <c r="H11" s="48"/>
       <c r="I11" s="28"/>
-    </row>
-    <row r="12" spans="1:24" ht="15" customHeight="1">
+      <c r="Z11" s="126">
+        <v>5</v>
+      </c>
+      <c r="AA11" s="126" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB11" s="126" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC11" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD11" s="126"/>
+      <c r="AE11" s="128" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF11" s="127"/>
+      <c r="AG11" s="127"/>
+      <c r="AH11" s="127"/>
+      <c r="AI11" s="127"/>
+      <c r="AJ11" s="127"/>
+      <c r="AK11" s="127"/>
+    </row>
+    <row r="12" spans="1:37" ht="15" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -2413,18 +2791,29 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="86" t="s">
+      <c r="L12" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="87"/>
-      <c r="Q12" s="87"/>
-      <c r="R12" s="87"/>
-      <c r="S12" s="88"/>
-    </row>
-    <row r="13" spans="1:24" ht="15" customHeight="1">
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="51"/>
+      <c r="Z12" s="126"/>
+      <c r="AA12" s="126"/>
+      <c r="AB12" s="126"/>
+      <c r="AC12" s="126"/>
+      <c r="AD12" s="126"/>
+      <c r="AF12" s="127"/>
+      <c r="AG12" s="127"/>
+      <c r="AH12" s="127"/>
+      <c r="AI12" s="127"/>
+      <c r="AJ12" s="127"/>
+      <c r="AK12" s="127"/>
+    </row>
+    <row r="13" spans="1:37" ht="15" customHeight="1">
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -2434,16 +2823,27 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="90"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="91"/>
-    </row>
-    <row r="14" spans="1:24" ht="15" customHeight="1">
+      <c r="L13" s="52"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="54"/>
+      <c r="Z13" s="126"/>
+      <c r="AA13" s="126"/>
+      <c r="AB13" s="126"/>
+      <c r="AC13" s="126"/>
+      <c r="AD13" s="126"/>
+      <c r="AF13" s="127"/>
+      <c r="AG13" s="127"/>
+      <c r="AH13" s="127"/>
+      <c r="AI13" s="127"/>
+      <c r="AJ13" s="127"/>
+      <c r="AK13" s="127"/>
+    </row>
+    <row r="14" spans="1:37" ht="15" customHeight="1">
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
@@ -2452,8 +2852,19 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
-    </row>
-    <row r="15" spans="1:24" ht="15" customHeight="1">
+      <c r="Z14" s="126"/>
+      <c r="AA14" s="126"/>
+      <c r="AB14" s="126"/>
+      <c r="AC14" s="126"/>
+      <c r="AD14" s="126"/>
+      <c r="AF14" s="127"/>
+      <c r="AG14" s="127"/>
+      <c r="AH14" s="127"/>
+      <c r="AI14" s="127"/>
+      <c r="AJ14" s="127"/>
+      <c r="AK14" s="127"/>
+    </row>
+    <row r="15" spans="1:37" ht="15" customHeight="1">
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
@@ -2463,76 +2874,109 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="92" t="s">
+      <c r="Q15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="93"/>
-      <c r="S15" s="93"/>
-      <c r="T15" s="93"/>
-      <c r="U15" s="93"/>
-      <c r="V15" s="93"/>
-      <c r="W15" s="93"/>
-      <c r="X15" s="94"/>
-    </row>
-    <row r="16" spans="1:24" ht="15" customHeight="1">
+      <c r="R15" s="56"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="56"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="56"/>
+      <c r="X15" s="57"/>
+      <c r="Z15" s="126"/>
+      <c r="AA15" s="126"/>
+      <c r="AB15" s="126"/>
+      <c r="AC15" s="126"/>
+      <c r="AD15" s="126"/>
+      <c r="AF15" s="127"/>
+      <c r="AG15" s="127"/>
+      <c r="AH15" s="127"/>
+      <c r="AI15" s="127"/>
+      <c r="AJ15" s="127"/>
+      <c r="AK15" s="127"/>
+    </row>
+    <row r="16" spans="1:37" ht="15" customHeight="1">
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="101" t="s">
+      <c r="M16" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="101"/>
-      <c r="O16" s="102"/>
-      <c r="Q16" s="95"/>
-      <c r="R16" s="96"/>
-      <c r="S16" s="96"/>
-      <c r="T16" s="96"/>
-      <c r="U16" s="96"/>
-      <c r="V16" s="96"/>
-      <c r="W16" s="96"/>
-      <c r="X16" s="97"/>
-    </row>
-    <row r="17" spans="1:24" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="86" t="s">
+      <c r="N16" s="35"/>
+      <c r="O16" s="36"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="59"/>
+      <c r="S16" s="59"/>
+      <c r="T16" s="59"/>
+      <c r="U16" s="59"/>
+      <c r="V16" s="59"/>
+      <c r="W16" s="59"/>
+      <c r="X16" s="60"/>
+      <c r="Z16" s="126"/>
+      <c r="AA16" s="126"/>
+      <c r="AB16" s="126"/>
+      <c r="AC16" s="126"/>
+      <c r="AD16" s="126"/>
+      <c r="AF16" s="127"/>
+      <c r="AG16" s="127"/>
+      <c r="AH16" s="127"/>
+      <c r="AI16" s="127"/>
+      <c r="AJ16" s="127"/>
+      <c r="AK16" s="127"/>
+    </row>
+    <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
+      <c r="B17" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="87"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="105" t="s">
+      <c r="E17" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="107"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="68"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="103"/>
-      <c r="N17" s="103"/>
-      <c r="O17" s="104"/>
-      <c r="Q17" s="98"/>
-      <c r="R17" s="99"/>
-      <c r="S17" s="99"/>
-      <c r="T17" s="99"/>
-      <c r="U17" s="99"/>
-      <c r="V17" s="99"/>
-      <c r="W17" s="99"/>
-      <c r="X17" s="100"/>
-    </row>
-    <row r="18" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="89"/>
-      <c r="C18" s="90"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="65"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="62"/>
+      <c r="W17" s="62"/>
+      <c r="X17" s="63"/>
+      <c r="Z17" s="126"/>
+      <c r="AA17" s="126"/>
+      <c r="AB17" s="126"/>
+      <c r="AC17" s="126"/>
+      <c r="AD17" s="126"/>
+      <c r="AF17" s="127"/>
+      <c r="AG17" s="127"/>
+      <c r="AH17" s="127"/>
+      <c r="AI17" s="127"/>
+      <c r="AJ17" s="127"/>
+      <c r="AK17" s="127"/>
+    </row>
+    <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="73" t="s">
+      <c r="L18" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="74"/>
+      <c r="M18" s="70"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -2544,227 +2988,359 @@
       <c r="V18" s="8"/>
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
-    </row>
-    <row r="19" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="108" t="s">
+      <c r="Z18" s="126"/>
+      <c r="AA18" s="126"/>
+      <c r="AB18" s="126"/>
+      <c r="AC18" s="126"/>
+      <c r="AD18" s="126"/>
+      <c r="AF18" s="127"/>
+      <c r="AG18" s="127"/>
+      <c r="AH18" s="127"/>
+      <c r="AI18" s="127"/>
+      <c r="AJ18" s="127"/>
+      <c r="AK18" s="127"/>
+    </row>
+    <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B19" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="102"/>
+      <c r="C19" s="36"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="74"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="70"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="111" t="s">
+      <c r="Q19" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="112"/>
-      <c r="S19" s="112"/>
-      <c r="T19" s="112"/>
-      <c r="U19" s="112"/>
-      <c r="V19" s="112"/>
-      <c r="W19" s="112"/>
-      <c r="X19" s="113"/>
-    </row>
-    <row r="20" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="109"/>
-      <c r="C20" s="110"/>
-      <c r="F20" s="114" t="s">
+      <c r="R19" s="72"/>
+      <c r="S19" s="72"/>
+      <c r="T19" s="72"/>
+      <c r="U19" s="72"/>
+      <c r="V19" s="72"/>
+      <c r="W19" s="72"/>
+      <c r="X19" s="73"/>
+      <c r="Z19" s="126"/>
+      <c r="AA19" s="126"/>
+      <c r="AB19" s="126"/>
+      <c r="AC19" s="126"/>
+      <c r="AD19" s="126"/>
+      <c r="AF19" s="127"/>
+      <c r="AG19" s="127"/>
+      <c r="AH19" s="127"/>
+      <c r="AI19" s="127"/>
+      <c r="AJ19" s="127"/>
+      <c r="AK19" s="127"/>
+    </row>
+    <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B20" s="37"/>
+      <c r="C20" s="39"/>
+      <c r="F20" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="115"/>
+      <c r="G20" s="75"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="73" t="s">
+      <c r="L20" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="74"/>
+      <c r="M20" s="70"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="40" t="s">
+      <c r="Q20" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="41"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
-      <c r="U20" s="41"/>
-      <c r="V20" s="41"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="49"/>
-    </row>
-    <row r="21" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="R20" s="79"/>
+      <c r="S20" s="79"/>
+      <c r="T20" s="79"/>
+      <c r="U20" s="79"/>
+      <c r="V20" s="79"/>
+      <c r="W20" s="79"/>
+      <c r="X20" s="80"/>
+      <c r="Z20" s="126"/>
+      <c r="AA20" s="126"/>
+      <c r="AB20" s="126"/>
+      <c r="AC20" s="126"/>
+      <c r="AD20" s="126"/>
+      <c r="AF20" s="127"/>
+      <c r="AG20" s="127"/>
+      <c r="AH20" s="127"/>
+      <c r="AI20" s="127"/>
+      <c r="AJ20" s="127"/>
+      <c r="AK20" s="127"/>
+    </row>
+    <row r="21" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="116"/>
-      <c r="G21" s="117"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="74"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="70"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="70" t="s">
+      <c r="Q21" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="71"/>
-      <c r="S21" s="71"/>
-      <c r="T21" s="71"/>
-      <c r="U21" s="71"/>
-      <c r="V21" s="71"/>
-      <c r="W21" s="71"/>
-      <c r="X21" s="72"/>
-    </row>
-    <row r="22" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="R21" s="82"/>
+      <c r="S21" s="82"/>
+      <c r="T21" s="82"/>
+      <c r="U21" s="82"/>
+      <c r="V21" s="82"/>
+      <c r="W21" s="82"/>
+      <c r="X21" s="83"/>
+      <c r="Z21" s="126"/>
+      <c r="AA21" s="126"/>
+      <c r="AB21" s="126"/>
+      <c r="AC21" s="126"/>
+      <c r="AD21" s="126"/>
+      <c r="AF21" s="127"/>
+      <c r="AG21" s="127"/>
+      <c r="AH21" s="127"/>
+      <c r="AI21" s="127"/>
+      <c r="AJ21" s="127"/>
+      <c r="AK21" s="127"/>
+    </row>
+    <row r="22" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="73" t="s">
+      <c r="L22" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="74"/>
+      <c r="M22" s="70"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
-    </row>
-    <row r="23" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Z22" s="126"/>
+      <c r="AA22" s="126"/>
+      <c r="AB22" s="126"/>
+      <c r="AC22" s="126"/>
+      <c r="AD22" s="126"/>
+      <c r="AF22" s="127"/>
+      <c r="AG22" s="127"/>
+      <c r="AH22" s="127"/>
+      <c r="AI22" s="127"/>
+      <c r="AJ22" s="127"/>
+      <c r="AK22" s="127"/>
+    </row>
+    <row r="23" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="42"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="84"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="74"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="75" t="s">
+      <c r="Q23" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="76"/>
-      <c r="S23" s="76"/>
-      <c r="T23" s="76"/>
-      <c r="U23" s="76"/>
-      <c r="V23" s="76"/>
-      <c r="W23" s="76"/>
-      <c r="X23" s="77"/>
-    </row>
-    <row r="24" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="R23" s="86"/>
+      <c r="S23" s="86"/>
+      <c r="T23" s="86"/>
+      <c r="U23" s="86"/>
+      <c r="V23" s="86"/>
+      <c r="W23" s="86"/>
+      <c r="X23" s="87"/>
+      <c r="Z23" s="126"/>
+      <c r="AA23" s="126"/>
+      <c r="AB23" s="126"/>
+      <c r="AC23" s="126"/>
+      <c r="AD23" s="126"/>
+      <c r="AF23" s="127"/>
+      <c r="AG23" s="127"/>
+      <c r="AH23" s="127"/>
+      <c r="AI23" s="127"/>
+      <c r="AJ23" s="127"/>
+      <c r="AK23" s="127"/>
+    </row>
+    <row r="24" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="73" t="s">
+      <c r="L24" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="74"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="79"/>
-      <c r="T24" s="79"/>
-      <c r="U24" s="79"/>
-      <c r="V24" s="79"/>
-      <c r="W24" s="79"/>
-      <c r="X24" s="80"/>
-    </row>
-    <row r="25" spans="1:24" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="Q24" s="88"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="89"/>
+      <c r="T24" s="89"/>
+      <c r="U24" s="89"/>
+      <c r="V24" s="89"/>
+      <c r="W24" s="89"/>
+      <c r="X24" s="90"/>
+      <c r="Z24" s="126"/>
+      <c r="AA24" s="126"/>
+      <c r="AB24" s="126"/>
+      <c r="AC24" s="126"/>
+      <c r="AD24" s="126"/>
+      <c r="AF24" s="127"/>
+      <c r="AG24" s="127"/>
+      <c r="AH24" s="127"/>
+      <c r="AI24" s="127"/>
+      <c r="AJ24" s="127"/>
+      <c r="AK24" s="127"/>
+    </row>
+    <row r="25" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="74"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="70"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="81"/>
-      <c r="R25" s="82"/>
-      <c r="S25" s="82"/>
-      <c r="T25" s="82"/>
-      <c r="U25" s="82"/>
-      <c r="V25" s="82"/>
-      <c r="W25" s="82"/>
-      <c r="X25" s="83"/>
-    </row>
-    <row r="26" spans="1:24" ht="15" customHeight="1" thickTop="1">
+      <c r="Q25" s="91"/>
+      <c r="R25" s="92"/>
+      <c r="S25" s="92"/>
+      <c r="T25" s="92"/>
+      <c r="U25" s="92"/>
+      <c r="V25" s="92"/>
+      <c r="W25" s="92"/>
+      <c r="X25" s="93"/>
+      <c r="Z25" s="126"/>
+      <c r="AA25" s="126"/>
+      <c r="AB25" s="126"/>
+      <c r="AC25" s="126"/>
+      <c r="AD25" s="126"/>
+      <c r="AF25" s="127"/>
+      <c r="AG25" s="127"/>
+      <c r="AH25" s="127"/>
+      <c r="AI25" s="127"/>
+      <c r="AJ25" s="127"/>
+      <c r="AK25" s="127"/>
+    </row>
+    <row r="26" spans="1:37" ht="15" customHeight="1" thickTop="1">
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="42"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="84"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="43" t="s">
+      <c r="Q26" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="44"/>
-      <c r="V26" s="44"/>
-      <c r="W26" s="44"/>
-      <c r="X26" s="45"/>
-    </row>
-    <row r="27" spans="1:24" ht="15" customHeight="1">
+      <c r="R26" s="101"/>
+      <c r="S26" s="101"/>
+      <c r="T26" s="101"/>
+      <c r="U26" s="101"/>
+      <c r="V26" s="101"/>
+      <c r="W26" s="101"/>
+      <c r="X26" s="102"/>
+      <c r="Z26" s="126"/>
+      <c r="AA26" s="126"/>
+      <c r="AB26" s="126"/>
+      <c r="AC26" s="126"/>
+      <c r="AD26" s="126"/>
+      <c r="AF26" s="126"/>
+      <c r="AG26" s="126"/>
+      <c r="AH26" s="126"/>
+      <c r="AI26" s="126"/>
+      <c r="AJ26" s="126"/>
+      <c r="AK26" s="126"/>
+    </row>
+    <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="47"/>
-      <c r="S27" s="47"/>
-      <c r="T27" s="47"/>
-      <c r="U27" s="47"/>
-      <c r="V27" s="47"/>
-      <c r="W27" s="47"/>
-      <c r="X27" s="48"/>
-    </row>
-    <row r="28" spans="1:24" ht="15" customHeight="1">
+      <c r="Q27" s="103"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="104"/>
+      <c r="T27" s="104"/>
+      <c r="U27" s="104"/>
+      <c r="V27" s="104"/>
+      <c r="W27" s="104"/>
+      <c r="X27" s="105"/>
+      <c r="Z27" s="126"/>
+      <c r="AA27" s="126"/>
+      <c r="AB27" s="126"/>
+      <c r="AC27" s="126"/>
+      <c r="AD27" s="126"/>
+      <c r="AF27" s="126"/>
+      <c r="AG27" s="126"/>
+      <c r="AH27" s="126"/>
+      <c r="AI27" s="126"/>
+      <c r="AJ27" s="126"/>
+      <c r="AK27" s="126"/>
+    </row>
+    <row r="28" spans="1:37" ht="15" customHeight="1">
       <c r="N28" s="12"/>
       <c r="O28" s="14"/>
       <c r="X28" s="13"/>
-    </row>
-    <row r="29" spans="1:24" ht="15" customHeight="1">
+      <c r="Z28" s="126"/>
+      <c r="AA28" s="126"/>
+      <c r="AB28" s="126"/>
+      <c r="AC28" s="126"/>
+      <c r="AD28" s="126"/>
+      <c r="AF28" s="126"/>
+      <c r="AG28" s="126"/>
+      <c r="AH28" s="126"/>
+      <c r="AI28" s="126"/>
+      <c r="AJ28" s="126"/>
+      <c r="AK28" s="126"/>
+    </row>
+    <row r="29" spans="1:37" ht="15" customHeight="1">
       <c r="N29" s="12"/>
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="40" t="s">
+      <c r="Q29" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="41"/>
-      <c r="V29" s="41"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="49"/>
-    </row>
-    <row r="30" spans="1:24" ht="15" customHeight="1">
+      <c r="R29" s="79"/>
+      <c r="S29" s="79"/>
+      <c r="T29" s="79"/>
+      <c r="U29" s="79"/>
+      <c r="V29" s="79"/>
+      <c r="W29" s="79"/>
+      <c r="X29" s="80"/>
+      <c r="Z29" s="126"/>
+      <c r="AA29" s="126"/>
+      <c r="AB29" s="126"/>
+      <c r="AC29" s="126"/>
+      <c r="AD29" s="126"/>
+      <c r="AF29" s="126"/>
+      <c r="AG29" s="126"/>
+      <c r="AH29" s="126"/>
+      <c r="AI29" s="126"/>
+      <c r="AJ29" s="126"/>
+      <c r="AK29" s="126"/>
+    </row>
+    <row r="30" spans="1:37" ht="15" customHeight="1">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2779,62 +3355,95 @@
       <c r="N30" s="12"/>
       <c r="O30" s="14"/>
       <c r="X30" s="13"/>
-    </row>
-    <row r="31" spans="1:24" ht="15" customHeight="1">
-      <c r="A31" s="50" t="s">
+      <c r="Z30" s="126"/>
+      <c r="AA30" s="126"/>
+      <c r="AB30" s="126"/>
+      <c r="AC30" s="126"/>
+      <c r="AD30" s="126"/>
+      <c r="AF30" s="126"/>
+      <c r="AG30" s="126"/>
+      <c r="AH30" s="126"/>
+      <c r="AI30" s="126"/>
+      <c r="AJ30" s="126"/>
+      <c r="AK30" s="126"/>
+    </row>
+    <row r="31" spans="1:37" ht="15" customHeight="1">
+      <c r="A31" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
+      <c r="B31" s="106"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="106"/>
+      <c r="J31" s="106"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="51" t="s">
+      <c r="P31" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="52"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="52"/>
-      <c r="W31" s="53"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="108"/>
+      <c r="S31" s="108"/>
+      <c r="T31" s="108"/>
+      <c r="U31" s="108"/>
+      <c r="V31" s="108"/>
+      <c r="W31" s="109"/>
       <c r="X31" s="13"/>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1">
-      <c r="A32" s="50"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
+      <c r="Z31" s="126"/>
+      <c r="AA31" s="126"/>
+      <c r="AB31" s="126"/>
+      <c r="AC31" s="126"/>
+      <c r="AD31" s="126"/>
+      <c r="AF31" s="126"/>
+      <c r="AG31" s="126"/>
+      <c r="AH31" s="126"/>
+      <c r="AI31" s="126"/>
+      <c r="AJ31" s="126"/>
+      <c r="AK31" s="126"/>
+    </row>
+    <row r="32" spans="1:37" ht="15" customHeight="1">
+      <c r="A32" s="106"/>
+      <c r="B32" s="106"/>
+      <c r="C32" s="106"/>
+      <c r="D32" s="106"/>
+      <c r="E32" s="106"/>
+      <c r="F32" s="106"/>
+      <c r="G32" s="106"/>
+      <c r="H32" s="106"/>
+      <c r="I32" s="106"/>
+      <c r="J32" s="106"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="54"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="55"/>
-      <c r="T32" s="55"/>
-      <c r="U32" s="55"/>
-      <c r="V32" s="55"/>
-      <c r="W32" s="56"/>
+      <c r="P32" s="110"/>
+      <c r="Q32" s="111"/>
+      <c r="R32" s="111"/>
+      <c r="S32" s="111"/>
+      <c r="T32" s="111"/>
+      <c r="U32" s="111"/>
+      <c r="V32" s="111"/>
+      <c r="W32" s="112"/>
       <c r="X32" s="13"/>
-    </row>
-    <row r="33" spans="1:25" ht="15" customHeight="1">
+      <c r="Z32" s="126"/>
+      <c r="AA32" s="126"/>
+      <c r="AB32" s="126"/>
+      <c r="AC32" s="126"/>
+      <c r="AD32" s="126"/>
+      <c r="AF32" s="126"/>
+      <c r="AG32" s="126"/>
+      <c r="AH32" s="126"/>
+      <c r="AI32" s="126"/>
+      <c r="AJ32" s="126"/>
+      <c r="AK32" s="126"/>
+    </row>
+    <row r="33" spans="1:37" ht="15" customHeight="1">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2849,140 +3458,184 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="54"/>
-      <c r="Q33" s="55"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="55"/>
-      <c r="T33" s="55"/>
-      <c r="U33" s="55"/>
-      <c r="V33" s="55"/>
-      <c r="W33" s="56"/>
+      <c r="P33" s="110"/>
+      <c r="Q33" s="111"/>
+      <c r="R33" s="111"/>
+      <c r="S33" s="111"/>
+      <c r="T33" s="111"/>
+      <c r="U33" s="111"/>
+      <c r="V33" s="111"/>
+      <c r="W33" s="112"/>
       <c r="X33" s="13"/>
-    </row>
-    <row r="34" spans="1:25" ht="15" customHeight="1">
+      <c r="Z33" s="126"/>
+      <c r="AA33" s="126"/>
+      <c r="AB33" s="126"/>
+      <c r="AC33" s="126"/>
+      <c r="AD33" s="126"/>
+      <c r="AF33" s="126"/>
+      <c r="AG33" s="126"/>
+      <c r="AH33" s="126"/>
+      <c r="AI33" s="126"/>
+      <c r="AJ33" s="126"/>
+      <c r="AK33" s="126"/>
+    </row>
+    <row r="34" spans="1:37" ht="15" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="60"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="116"/>
+      <c r="J34" s="116"/>
+      <c r="K34" s="116"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="54"/>
-      <c r="Q34" s="55"/>
-      <c r="R34" s="55"/>
-      <c r="S34" s="55"/>
-      <c r="T34" s="55"/>
-      <c r="U34" s="55"/>
-      <c r="V34" s="55"/>
-      <c r="W34" s="56"/>
+      <c r="P34" s="110"/>
+      <c r="Q34" s="111"/>
+      <c r="R34" s="111"/>
+      <c r="S34" s="111"/>
+      <c r="T34" s="111"/>
+      <c r="U34" s="111"/>
+      <c r="V34" s="111"/>
+      <c r="W34" s="112"/>
       <c r="X34" s="13"/>
-    </row>
-    <row r="35" spans="1:25" ht="15" customHeight="1">
-      <c r="A35" s="60" t="s">
+      <c r="Z34" s="126"/>
+      <c r="AA34" s="126"/>
+      <c r="AB34" s="126"/>
+      <c r="AC34" s="126"/>
+      <c r="AD34" s="126"/>
+      <c r="AF34" s="126"/>
+      <c r="AG34" s="126"/>
+      <c r="AH34" s="126"/>
+      <c r="AI34" s="126"/>
+      <c r="AJ34" s="126"/>
+      <c r="AK34" s="126"/>
+    </row>
+    <row r="35" spans="1:37" ht="15" customHeight="1">
+      <c r="A35" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="63"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="118"/>
+      <c r="K35" s="119"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="54"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="55"/>
-      <c r="T35" s="55"/>
-      <c r="U35" s="55"/>
-      <c r="V35" s="55"/>
-      <c r="W35" s="56"/>
+      <c r="P35" s="110"/>
+      <c r="Q35" s="111"/>
+      <c r="R35" s="111"/>
+      <c r="S35" s="111"/>
+      <c r="T35" s="111"/>
+      <c r="U35" s="111"/>
+      <c r="V35" s="111"/>
+      <c r="W35" s="112"/>
       <c r="X35" s="13"/>
-    </row>
-    <row r="36" spans="1:25" ht="15" customHeight="1">
-      <c r="A36" s="60"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="66"/>
+      <c r="Z35" s="126"/>
+      <c r="AA35" s="126"/>
+      <c r="AB35" s="126"/>
+      <c r="AC35" s="126"/>
+      <c r="AD35" s="126"/>
+      <c r="AF35" s="126"/>
+      <c r="AG35" s="126"/>
+      <c r="AH35" s="126"/>
+      <c r="AI35" s="126"/>
+      <c r="AJ35" s="126"/>
+      <c r="AK35" s="126"/>
+    </row>
+    <row r="36" spans="1:37" ht="15" customHeight="1">
+      <c r="A36" s="116"/>
+      <c r="B36" s="120"/>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="121"/>
+      <c r="G36" s="121"/>
+      <c r="H36" s="121"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="121"/>
+      <c r="K36" s="122"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="54"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="55"/>
-      <c r="T36" s="55"/>
-      <c r="U36" s="55"/>
-      <c r="V36" s="55"/>
-      <c r="W36" s="56"/>
+      <c r="P36" s="110"/>
+      <c r="Q36" s="111"/>
+      <c r="R36" s="111"/>
+      <c r="S36" s="111"/>
+      <c r="T36" s="111"/>
+      <c r="U36" s="111"/>
+      <c r="V36" s="111"/>
+      <c r="W36" s="112"/>
       <c r="X36" s="13"/>
-    </row>
-    <row r="37" spans="1:25" ht="15" customHeight="1">
-      <c r="A37" s="60"/>
-      <c r="B37" s="67"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="69"/>
+      <c r="Z36" s="126"/>
+      <c r="AA36" s="126"/>
+      <c r="AB36" s="126"/>
+      <c r="AC36" s="126"/>
+      <c r="AD36" s="126"/>
+      <c r="AF36" s="126"/>
+      <c r="AG36" s="126"/>
+      <c r="AH36" s="126"/>
+      <c r="AI36" s="126"/>
+      <c r="AJ36" s="126"/>
+      <c r="AK36" s="126"/>
+    </row>
+    <row r="37" spans="1:37" ht="15" customHeight="1">
+      <c r="A37" s="116"/>
+      <c r="B37" s="123"/>
+      <c r="C37" s="124"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="124"/>
+      <c r="F37" s="124"/>
+      <c r="G37" s="124"/>
+      <c r="H37" s="124"/>
+      <c r="I37" s="124"/>
+      <c r="J37" s="124"/>
+      <c r="K37" s="125"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="57"/>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="58"/>
-      <c r="T37" s="58"/>
-      <c r="U37" s="58"/>
-      <c r="V37" s="58"/>
-      <c r="W37" s="59"/>
+      <c r="P37" s="113"/>
+      <c r="Q37" s="114"/>
+      <c r="R37" s="114"/>
+      <c r="S37" s="114"/>
+      <c r="T37" s="114"/>
+      <c r="U37" s="114"/>
+      <c r="V37" s="114"/>
+      <c r="W37" s="115"/>
       <c r="X37" s="13"/>
     </row>
-    <row r="38" spans="1:25" ht="15" customHeight="1" thickBot="1">
+    <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="36"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="98"/>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="98"/>
+      <c r="I38" s="98"/>
+      <c r="J38" s="98"/>
+      <c r="K38" s="99"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -2996,40 +3649,40 @@
       <c r="W38" s="10"/>
       <c r="X38" s="9"/>
     </row>
-    <row r="39" spans="1:25" ht="15" customHeight="1">
+    <row r="39" spans="1:37" ht="15" customHeight="1">
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="36"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="98"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="99"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:25" ht="15" customHeight="1">
+    <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="36"/>
+      <c r="C40" s="98"/>
+      <c r="D40" s="98"/>
+      <c r="E40" s="98"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="98"/>
+      <c r="H40" s="98"/>
+      <c r="I40" s="98"/>
+      <c r="J40" s="98"/>
+      <c r="K40" s="99"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -3044,80 +3697,80 @@
       <c r="W40" s="8"/>
       <c r="X40" s="8"/>
     </row>
-    <row r="41" spans="1:25" ht="15" customHeight="1">
+    <row r="41" spans="1:37" ht="15" customHeight="1">
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="36"/>
+      <c r="C41" s="98"/>
+      <c r="D41" s="98"/>
+      <c r="E41" s="98"/>
+      <c r="F41" s="98"/>
+      <c r="G41" s="98"/>
+      <c r="H41" s="98"/>
+      <c r="I41" s="98"/>
+      <c r="J41" s="98"/>
+      <c r="K41" s="99"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="37" t="s">
+      <c r="M41" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-      <c r="P41" s="38"/>
-      <c r="Q41" s="38"/>
-      <c r="R41" s="38"/>
-      <c r="S41" s="38"/>
-      <c r="T41" s="38"/>
-      <c r="U41" s="38"/>
-      <c r="V41" s="38"/>
-      <c r="W41" s="38"/>
-      <c r="X41" s="39"/>
+      <c r="N41" s="95"/>
+      <c r="O41" s="95"/>
+      <c r="P41" s="95"/>
+      <c r="Q41" s="95"/>
+      <c r="R41" s="95"/>
+      <c r="S41" s="95"/>
+      <c r="T41" s="95"/>
+      <c r="U41" s="95"/>
+      <c r="V41" s="95"/>
+      <c r="W41" s="95"/>
+      <c r="X41" s="96"/>
       <c r="Y41" s="4"/>
     </row>
-    <row r="42" spans="1:25" ht="15" customHeight="1">
+    <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="36"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="98"/>
+      <c r="D42" s="98"/>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="98"/>
+      <c r="H42" s="98"/>
+      <c r="I42" s="98"/>
+      <c r="J42" s="98"/>
+      <c r="K42" s="99"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="37" t="s">
+      <c r="M42" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="38"/>
-      <c r="O42" s="38"/>
-      <c r="P42" s="38"/>
-      <c r="Q42" s="38"/>
-      <c r="R42" s="38"/>
-      <c r="S42" s="38"/>
-      <c r="T42" s="38"/>
-      <c r="U42" s="38"/>
-      <c r="V42" s="38"/>
-      <c r="W42" s="38"/>
-      <c r="X42" s="39"/>
+      <c r="N42" s="95"/>
+      <c r="O42" s="95"/>
+      <c r="P42" s="95"/>
+      <c r="Q42" s="95"/>
+      <c r="R42" s="95"/>
+      <c r="S42" s="95"/>
+      <c r="T42" s="95"/>
+      <c r="U42" s="95"/>
+      <c r="V42" s="95"/>
+      <c r="W42" s="95"/>
+      <c r="X42" s="96"/>
       <c r="Y42" s="4"/>
     </row>
-    <row r="43" spans="1:25" ht="15" customHeight="1">
+    <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
-      <c r="K43" s="36"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="98"/>
+      <c r="D43" s="98"/>
+      <c r="E43" s="98"/>
+      <c r="F43" s="98"/>
+      <c r="G43" s="98"/>
+      <c r="H43" s="98"/>
+      <c r="I43" s="98"/>
+      <c r="J43" s="98"/>
+      <c r="K43" s="99"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -3133,18 +3786,18 @@
       <c r="X43" s="5"/>
       <c r="Y43" s="4"/>
     </row>
-    <row r="44" spans="1:25" ht="15" customHeight="1">
+    <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="36"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="98"/>
+      <c r="E44" s="98"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="98"/>
+      <c r="H44" s="98"/>
+      <c r="I44" s="98"/>
+      <c r="J44" s="98"/>
+      <c r="K44" s="99"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -3160,18 +3813,18 @@
       <c r="X44" s="5"/>
       <c r="Y44" s="4"/>
     </row>
-    <row r="45" spans="1:25" ht="15" customHeight="1">
+    <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="36"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="98"/>
+      <c r="D45" s="98"/>
+      <c r="E45" s="98"/>
+      <c r="F45" s="98"/>
+      <c r="G45" s="98"/>
+      <c r="H45" s="98"/>
+      <c r="I45" s="98"/>
+      <c r="J45" s="98"/>
+      <c r="K45" s="99"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -3187,18 +3840,18 @@
       <c r="X45" s="5"/>
       <c r="Y45" s="4"/>
     </row>
-    <row r="46" spans="1:25" ht="15" customHeight="1">
+    <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="36"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="98"/>
+      <c r="D46" s="98"/>
+      <c r="E46" s="98"/>
+      <c r="F46" s="98"/>
+      <c r="G46" s="98"/>
+      <c r="H46" s="98"/>
+      <c r="I46" s="98"/>
+      <c r="J46" s="98"/>
+      <c r="K46" s="99"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -3214,7 +3867,7 @@
       <c r="X46" s="5"/>
       <c r="Y46" s="4"/>
     </row>
-    <row r="47" spans="1:25" ht="15" customHeight="1">
+    <row r="47" spans="1:37" ht="15" customHeight="1">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3240,12 +3893,31 @@
       <c r="X47" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="J9:L10"/>
-    <mergeCell ref="B10:D10"/>
+  <mergeCells count="42">
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="M42:X42"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="Q26:X27"/>
+    <mergeCell ref="Q29:X29"/>
+    <mergeCell ref="A31:J32"/>
+    <mergeCell ref="P31:W37"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:K37"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="M41:X41"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="L12:S13"/>
     <mergeCell ref="Q15:X17"/>
@@ -3259,32 +3931,15 @@
     <mergeCell ref="L20:M21"/>
     <mergeCell ref="Q20:X20"/>
     <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="M41:X41"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="M42:X42"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="Q26:X27"/>
-    <mergeCell ref="Q29:X29"/>
-    <mergeCell ref="A31:J32"/>
-    <mergeCell ref="P31:W37"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:K37"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="J9:L10"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
been struggling with these architecture decisions for 2 week now need to do a course or read some stuff about structuring scripts developing in general
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -161,15 +161,9 @@
     <t>Comm Ports LR for eachShip LR</t>
   </si>
   <si>
-    <t>Player Setup Manager</t>
-  </si>
-  <si>
     <t>Game Scenario Setting, Or Allow Player Setup to Run Advanced Game Setup</t>
   </si>
   <si>
-    <t>GM</t>
-  </si>
-  <si>
     <t>Organiser Settings</t>
   </si>
   <si>
@@ -261,6 +255,12 @@
   </si>
   <si>
     <t>deactivate arrow, activate max bar big timer</t>
+  </si>
+  <si>
+    <t>Player Setup Manager - run interface trigger actions</t>
+  </si>
+  <si>
+    <t>GM - hold info</t>
   </si>
 </sst>
 </file>
@@ -1247,22 +1247,292 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1284,276 +1554,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -2025,66 +2025,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="6-Point Star 9"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6543674" y="4876800"/>
-          <a:ext cx="2009775" cy="1695450"/>
-        </a:xfrm>
-        <a:prstGeom prst="star6">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Could</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> use the animator to trigger the code use it as a timer</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>276226</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -2480,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL27" sqref="AL27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2491,182 +2431,182 @@
     <col min="28" max="28" width="30.85546875" style="1" customWidth="1"/>
     <col min="29" max="29" width="34.140625" style="1" customWidth="1"/>
     <col min="30" max="30" width="39.85546875" style="1" customWidth="1"/>
-    <col min="31" max="31" width="78.42578125" style="128" customWidth="1"/>
+    <col min="31" max="31" width="78.42578125" style="36" customWidth="1"/>
     <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="Y1" s="131" t="s">
+      <c r="Y1" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" s="40"/>
+    </row>
+    <row r="2" spans="1:37" ht="15" customHeight="1">
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="42"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+    </row>
+    <row r="3" spans="1:37" ht="15" customHeight="1">
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="34"/>
+      <c r="AB3" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC3" s="34"/>
+      <c r="AD3" s="34"/>
+      <c r="AE3" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF3" s="35"/>
+      <c r="AG3" s="35"/>
+      <c r="AH3" s="35"/>
+      <c r="AI3" s="35"/>
+      <c r="AJ3" s="35"/>
+      <c r="AK3" s="35"/>
+    </row>
+    <row r="4" spans="1:37" ht="15" customHeight="1">
+      <c r="B4" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="109"/>
+      <c r="D4" s="110"/>
+      <c r="G4" s="116" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="109"/>
+      <c r="I4" s="110"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="34"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="35"/>
+    </row>
+    <row r="5" spans="1:37" ht="15" customHeight="1">
+      <c r="B5" s="117"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="118"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="118"/>
+      <c r="Z5" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="35"/>
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+    </row>
+    <row r="6" spans="1:37" ht="15" customHeight="1">
+      <c r="Z6" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="Z1" s="132"/>
-    </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="Y2" s="133"/>
-      <c r="Z2" s="134"/>
-      <c r="AF2" s="127"/>
-      <c r="AG2" s="127"/>
-      <c r="AH2" s="127"/>
-      <c r="AI2" s="127"/>
-      <c r="AJ2" s="127"/>
-      <c r="AK2" s="127"/>
-    </row>
-    <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="136"/>
-      <c r="AA3" s="126"/>
-      <c r="AB3" s="130" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC3" s="126"/>
-      <c r="AD3" s="126"/>
-      <c r="AE3" s="129" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF3" s="127"/>
-      <c r="AG3" s="127"/>
-      <c r="AH3" s="127"/>
-      <c r="AI3" s="127"/>
-      <c r="AJ3" s="127"/>
-      <c r="AK3" s="127"/>
-    </row>
-    <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="34" t="s">
+      <c r="AA6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="G4" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
-      <c r="Z4" s="126"/>
-      <c r="AA4" s="126"/>
-      <c r="AB4" s="126"/>
-      <c r="AC4" s="126"/>
-      <c r="AD4" s="126"/>
-      <c r="AF4" s="127"/>
-      <c r="AG4" s="127"/>
-      <c r="AH4" s="127"/>
-      <c r="AI4" s="127"/>
-      <c r="AJ4" s="127"/>
-      <c r="AK4" s="127"/>
-    </row>
-    <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="39"/>
-      <c r="Z5" s="126" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA5" s="126"/>
-      <c r="AB5" s="126"/>
-      <c r="AC5" s="126"/>
-      <c r="AD5" s="126"/>
-      <c r="AF5" s="127"/>
-      <c r="AG5" s="127"/>
-      <c r="AH5" s="127"/>
-      <c r="AI5" s="127"/>
-      <c r="AJ5" s="127"/>
-      <c r="AK5" s="127"/>
-    </row>
-    <row r="6" spans="1:37" ht="15" customHeight="1">
-      <c r="Z6" s="126" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA6" s="126" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB6" s="126" t="s">
+      <c r="AB6" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC6" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="AC6" s="126" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD6" s="126" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE6" s="127" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF6" s="127"/>
-      <c r="AG6" s="127"/>
-      <c r="AH6" s="127"/>
-      <c r="AI6" s="127"/>
-      <c r="AJ6" s="127"/>
-      <c r="AK6" s="127"/>
+      <c r="AD6" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE6" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF6" s="35"/>
+      <c r="AG6" s="35"/>
+      <c r="AH6" s="35"/>
+      <c r="AI6" s="35"/>
+      <c r="AJ6" s="35"/>
+      <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
+      <c r="B7" s="130" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="132"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
-      <c r="Z7" s="126" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA7" s="126" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB7" s="126" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC7" s="126" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD7" s="126" t="s">
+      <c r="Z7" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA7" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC7" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="AE7" s="128" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF7" s="127"/>
-      <c r="AG7" s="127"/>
-      <c r="AH7" s="127"/>
-      <c r="AI7" s="127"/>
-      <c r="AJ7" s="127"/>
-      <c r="AK7" s="127"/>
+      <c r="AD7" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE7" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF7" s="35"/>
+      <c r="AG7" s="35"/>
+      <c r="AH7" s="35"/>
+      <c r="AI7" s="35"/>
+      <c r="AJ7" s="35"/>
+      <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="135"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
-      <c r="Z8" s="126">
+      <c r="Z8" s="34">
         <v>10</v>
       </c>
-      <c r="AA8" s="126" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB8" s="126" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC8" s="126" t="s">
+      <c r="AA8" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB8" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC8" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD8" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE8" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="AD8" s="126" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE8" s="128" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF8" s="127"/>
-      <c r="AG8" s="127"/>
-      <c r="AH8" s="127"/>
-      <c r="AI8" s="127"/>
-      <c r="AJ8" s="127"/>
-      <c r="AK8" s="127"/>
+      <c r="AF8" s="35"/>
+      <c r="AG8" s="35"/>
+      <c r="AH8" s="35"/>
+      <c r="AI8" s="35"/>
+      <c r="AJ8" s="35"/>
+      <c r="AK8" s="35"/>
     </row>
     <row r="9" spans="1:37" ht="15" customHeight="1">
       <c r="B9" s="32"/>
@@ -2676,75 +2616,87 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
-      <c r="Z9" s="126" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA9" s="126" t="s">
+      <c r="J9" s="116" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="110"/>
+      <c r="Z9" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA9" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB9" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="AB9" s="126" t="s">
+      <c r="AC9" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="AC9" s="126" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD9" s="126" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE9" s="128" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF9" s="127"/>
-      <c r="AG9" s="127"/>
-      <c r="AH9" s="127"/>
-      <c r="AI9" s="127"/>
-      <c r="AJ9" s="127"/>
-      <c r="AK9" s="127"/>
+      <c r="AD9" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE9" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF9" s="35"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="35"/>
+      <c r="AI9" s="35"/>
+      <c r="AJ9" s="35"/>
+      <c r="AK9" s="35"/>
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="136"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
-      <c r="Z10" s="126">
+      <c r="J10" s="117"/>
+      <c r="K10" s="129"/>
+      <c r="L10" s="129"/>
+      <c r="M10" s="129"/>
+      <c r="N10" s="129"/>
+      <c r="O10" s="129"/>
+      <c r="P10" s="129"/>
+      <c r="Q10" s="129"/>
+      <c r="R10" s="118"/>
+      <c r="Z10" s="34">
         <v>20</v>
       </c>
-      <c r="AA10" s="126" t="s">
+      <c r="AA10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="AB10" s="126" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC10" s="126" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD10" s="126" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE10" s="128" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF10" s="127"/>
-      <c r="AG10" s="127"/>
-      <c r="AH10" s="127"/>
-      <c r="AI10" s="127"/>
-      <c r="AJ10" s="127"/>
-      <c r="AK10" s="127"/>
+      <c r="AB10" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC10" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD10" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE10" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF10" s="35"/>
+      <c r="AG10" s="35"/>
+      <c r="AH10" s="35"/>
+      <c r="AI10" s="35"/>
+      <c r="AJ10" s="35"/>
+      <c r="AK10" s="35"/>
     </row>
     <row r="11" spans="1:37" ht="15" customHeight="1">
       <c r="A11" s="12"/>
@@ -2752,33 +2704,33 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="48"/>
+      <c r="H11" s="93"/>
       <c r="I11" s="28"/>
-      <c r="Z11" s="126">
+      <c r="Z11" s="34">
         <v>5</v>
       </c>
-      <c r="AA11" s="126" t="s">
+      <c r="AA11" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="AB11" s="126" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC11" s="126" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD11" s="126"/>
-      <c r="AE11" s="128" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF11" s="127"/>
-      <c r="AG11" s="127"/>
-      <c r="AH11" s="127"/>
-      <c r="AI11" s="127"/>
-      <c r="AJ11" s="127"/>
-      <c r="AK11" s="127"/>
+      <c r="AB11" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC11" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD11" s="34"/>
+      <c r="AE11" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF11" s="35"/>
+      <c r="AG11" s="35"/>
+      <c r="AH11" s="35"/>
+      <c r="AI11" s="35"/>
+      <c r="AJ11" s="35"/>
+      <c r="AK11" s="35"/>
     </row>
     <row r="12" spans="1:37" ht="15" customHeight="1">
       <c r="A12" s="12"/>
@@ -2791,27 +2743,27 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="49" t="s">
+      <c r="L12" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="51"/>
-      <c r="Z12" s="126"/>
-      <c r="AA12" s="126"/>
-      <c r="AB12" s="126"/>
-      <c r="AC12" s="126"/>
-      <c r="AD12" s="126"/>
-      <c r="AF12" s="127"/>
-      <c r="AG12" s="127"/>
-      <c r="AH12" s="127"/>
-      <c r="AI12" s="127"/>
-      <c r="AJ12" s="127"/>
-      <c r="AK12" s="127"/>
+      <c r="M12" s="95"/>
+      <c r="N12" s="95"/>
+      <c r="O12" s="95"/>
+      <c r="P12" s="95"/>
+      <c r="Q12" s="95"/>
+      <c r="R12" s="95"/>
+      <c r="S12" s="96"/>
+      <c r="Z12" s="34"/>
+      <c r="AA12" s="34"/>
+      <c r="AB12" s="34"/>
+      <c r="AC12" s="34"/>
+      <c r="AD12" s="34"/>
+      <c r="AF12" s="35"/>
+      <c r="AG12" s="35"/>
+      <c r="AH12" s="35"/>
+      <c r="AI12" s="35"/>
+      <c r="AJ12" s="35"/>
+      <c r="AK12" s="35"/>
     </row>
     <row r="13" spans="1:37" ht="15" customHeight="1">
       <c r="B13" s="30"/>
@@ -2823,25 +2775,25 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="53"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="54"/>
-      <c r="Z13" s="126"/>
-      <c r="AA13" s="126"/>
-      <c r="AB13" s="126"/>
-      <c r="AC13" s="126"/>
-      <c r="AD13" s="126"/>
-      <c r="AF13" s="127"/>
-      <c r="AG13" s="127"/>
-      <c r="AH13" s="127"/>
-      <c r="AI13" s="127"/>
-      <c r="AJ13" s="127"/>
-      <c r="AK13" s="127"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="98"/>
+      <c r="P13" s="98"/>
+      <c r="Q13" s="98"/>
+      <c r="R13" s="98"/>
+      <c r="S13" s="99"/>
+      <c r="Z13" s="34"/>
+      <c r="AA13" s="34"/>
+      <c r="AB13" s="34"/>
+      <c r="AC13" s="34"/>
+      <c r="AD13" s="34"/>
+      <c r="AF13" s="35"/>
+      <c r="AG13" s="35"/>
+      <c r="AH13" s="35"/>
+      <c r="AI13" s="35"/>
+      <c r="AJ13" s="35"/>
+      <c r="AK13" s="35"/>
     </row>
     <row r="14" spans="1:37" ht="15" customHeight="1">
       <c r="B14" s="29"/>
@@ -2852,17 +2804,17 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
-      <c r="Z14" s="126"/>
-      <c r="AA14" s="126"/>
-      <c r="AB14" s="126"/>
-      <c r="AC14" s="126"/>
-      <c r="AD14" s="126"/>
-      <c r="AF14" s="127"/>
-      <c r="AG14" s="127"/>
-      <c r="AH14" s="127"/>
-      <c r="AI14" s="127"/>
-      <c r="AJ14" s="127"/>
-      <c r="AK14" s="127"/>
+      <c r="Z14" s="34"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="34"/>
+      <c r="AC14" s="34"/>
+      <c r="AD14" s="34"/>
+      <c r="AF14" s="35"/>
+      <c r="AG14" s="35"/>
+      <c r="AH14" s="35"/>
+      <c r="AI14" s="35"/>
+      <c r="AJ14" s="35"/>
+      <c r="AK14" s="35"/>
     </row>
     <row r="15" spans="1:37" ht="15" customHeight="1">
       <c r="B15" s="29"/>
@@ -2874,109 +2826,109 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="55" t="s">
+      <c r="Q15" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="56"/>
-      <c r="V15" s="56"/>
-      <c r="W15" s="56"/>
-      <c r="X15" s="57"/>
-      <c r="Z15" s="126"/>
-      <c r="AA15" s="126"/>
-      <c r="AB15" s="126"/>
-      <c r="AC15" s="126"/>
-      <c r="AD15" s="126"/>
-      <c r="AF15" s="127"/>
-      <c r="AG15" s="127"/>
-      <c r="AH15" s="127"/>
-      <c r="AI15" s="127"/>
-      <c r="AJ15" s="127"/>
-      <c r="AK15" s="127"/>
+      <c r="R15" s="101"/>
+      <c r="S15" s="101"/>
+      <c r="T15" s="101"/>
+      <c r="U15" s="101"/>
+      <c r="V15" s="101"/>
+      <c r="W15" s="101"/>
+      <c r="X15" s="102"/>
+      <c r="Z15" s="34"/>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="34"/>
+      <c r="AC15" s="34"/>
+      <c r="AD15" s="34"/>
+      <c r="AF15" s="35"/>
+      <c r="AG15" s="35"/>
+      <c r="AH15" s="35"/>
+      <c r="AI15" s="35"/>
+      <c r="AJ15" s="35"/>
+      <c r="AK15" s="35"/>
     </row>
     <row r="16" spans="1:37" ht="15" customHeight="1">
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="35" t="s">
+      <c r="M16" s="109" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="35"/>
-      <c r="O16" s="36"/>
-      <c r="Q16" s="58"/>
-      <c r="R16" s="59"/>
-      <c r="S16" s="59"/>
-      <c r="T16" s="59"/>
-      <c r="U16" s="59"/>
-      <c r="V16" s="59"/>
-      <c r="W16" s="59"/>
-      <c r="X16" s="60"/>
-      <c r="Z16" s="126"/>
-      <c r="AA16" s="126"/>
-      <c r="AB16" s="126"/>
-      <c r="AC16" s="126"/>
-      <c r="AD16" s="126"/>
-      <c r="AF16" s="127"/>
-      <c r="AG16" s="127"/>
-      <c r="AH16" s="127"/>
-      <c r="AI16" s="127"/>
-      <c r="AJ16" s="127"/>
-      <c r="AK16" s="127"/>
+      <c r="N16" s="109"/>
+      <c r="O16" s="110"/>
+      <c r="Q16" s="103"/>
+      <c r="R16" s="104"/>
+      <c r="S16" s="104"/>
+      <c r="T16" s="104"/>
+      <c r="U16" s="104"/>
+      <c r="V16" s="104"/>
+      <c r="W16" s="104"/>
+      <c r="X16" s="105"/>
+      <c r="Z16" s="34"/>
+      <c r="AA16" s="34"/>
+      <c r="AB16" s="34"/>
+      <c r="AC16" s="34"/>
+      <c r="AD16" s="34"/>
+      <c r="AF16" s="35"/>
+      <c r="AG16" s="35"/>
+      <c r="AH16" s="35"/>
+      <c r="AI16" s="35"/>
+      <c r="AJ16" s="35"/>
+      <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="50"/>
+      <c r="C17" s="95"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="66" t="s">
+      <c r="E17" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="68"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="115"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="64"/>
-      <c r="N17" s="64"/>
-      <c r="O17" s="65"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="62"/>
-      <c r="V17" s="62"/>
-      <c r="W17" s="62"/>
-      <c r="X17" s="63"/>
-      <c r="Z17" s="126"/>
-      <c r="AA17" s="126"/>
-      <c r="AB17" s="126"/>
-      <c r="AC17" s="126"/>
-      <c r="AD17" s="126"/>
-      <c r="AF17" s="127"/>
-      <c r="AG17" s="127"/>
-      <c r="AH17" s="127"/>
-      <c r="AI17" s="127"/>
-      <c r="AJ17" s="127"/>
-      <c r="AK17" s="127"/>
+      <c r="M17" s="111"/>
+      <c r="N17" s="111"/>
+      <c r="O17" s="112"/>
+      <c r="Q17" s="106"/>
+      <c r="R17" s="107"/>
+      <c r="S17" s="107"/>
+      <c r="T17" s="107"/>
+      <c r="U17" s="107"/>
+      <c r="V17" s="107"/>
+      <c r="W17" s="107"/>
+      <c r="X17" s="108"/>
+      <c r="Z17" s="34"/>
+      <c r="AA17" s="34"/>
+      <c r="AB17" s="34"/>
+      <c r="AC17" s="34"/>
+      <c r="AD17" s="34"/>
+      <c r="AF17" s="35"/>
+      <c r="AG17" s="35"/>
+      <c r="AH17" s="35"/>
+      <c r="AI17" s="35"/>
+      <c r="AJ17" s="35"/>
+      <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="52"/>
-      <c r="C18" s="53"/>
+      <c r="B18" s="97"/>
+      <c r="C18" s="98"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="69" t="s">
+      <c r="L18" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="70"/>
+      <c r="M18" s="82"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -2988,357 +2940,357 @@
       <c r="V18" s="8"/>
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
-      <c r="Z18" s="126"/>
-      <c r="AA18" s="126"/>
-      <c r="AB18" s="126"/>
-      <c r="AC18" s="126"/>
-      <c r="AD18" s="126"/>
-      <c r="AF18" s="127"/>
-      <c r="AG18" s="127"/>
-      <c r="AH18" s="127"/>
-      <c r="AI18" s="127"/>
-      <c r="AJ18" s="127"/>
-      <c r="AK18" s="127"/>
+      <c r="Z18" s="34"/>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="34"/>
+      <c r="AC18" s="34"/>
+      <c r="AD18" s="34"/>
+      <c r="AF18" s="35"/>
+      <c r="AG18" s="35"/>
+      <c r="AH18" s="35"/>
+      <c r="AI18" s="35"/>
+      <c r="AJ18" s="35"/>
+      <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="110"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="70"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="82"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="71" t="s">
+      <c r="Q19" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="72"/>
-      <c r="S19" s="72"/>
-      <c r="T19" s="72"/>
-      <c r="U19" s="72"/>
-      <c r="V19" s="72"/>
-      <c r="W19" s="72"/>
-      <c r="X19" s="73"/>
-      <c r="Z19" s="126"/>
-      <c r="AA19" s="126"/>
-      <c r="AB19" s="126"/>
-      <c r="AC19" s="126"/>
-      <c r="AD19" s="126"/>
-      <c r="AF19" s="127"/>
-      <c r="AG19" s="127"/>
-      <c r="AH19" s="127"/>
-      <c r="AI19" s="127"/>
-      <c r="AJ19" s="127"/>
-      <c r="AK19" s="127"/>
+      <c r="R19" s="120"/>
+      <c r="S19" s="120"/>
+      <c r="T19" s="120"/>
+      <c r="U19" s="120"/>
+      <c r="V19" s="120"/>
+      <c r="W19" s="120"/>
+      <c r="X19" s="121"/>
+      <c r="Z19" s="34"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34"/>
+      <c r="AC19" s="34"/>
+      <c r="AD19" s="34"/>
+      <c r="AF19" s="35"/>
+      <c r="AG19" s="35"/>
+      <c r="AH19" s="35"/>
+      <c r="AI19" s="35"/>
+      <c r="AJ19" s="35"/>
+      <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="37"/>
-      <c r="C20" s="39"/>
-      <c r="F20" s="74" t="s">
+      <c r="B20" s="117"/>
+      <c r="C20" s="118"/>
+      <c r="F20" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="75"/>
+      <c r="G20" s="123"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="69" t="s">
+      <c r="L20" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="70"/>
+      <c r="M20" s="82"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="78" t="s">
+      <c r="Q20" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="79"/>
-      <c r="S20" s="79"/>
-      <c r="T20" s="79"/>
-      <c r="U20" s="79"/>
-      <c r="V20" s="79"/>
-      <c r="W20" s="79"/>
-      <c r="X20" s="80"/>
-      <c r="Z20" s="126"/>
-      <c r="AA20" s="126"/>
-      <c r="AB20" s="126"/>
-      <c r="AC20" s="126"/>
-      <c r="AD20" s="126"/>
-      <c r="AF20" s="127"/>
-      <c r="AG20" s="127"/>
-      <c r="AH20" s="127"/>
-      <c r="AI20" s="127"/>
-      <c r="AJ20" s="127"/>
-      <c r="AK20" s="127"/>
+      <c r="R20" s="52"/>
+      <c r="S20" s="52"/>
+      <c r="T20" s="52"/>
+      <c r="U20" s="52"/>
+      <c r="V20" s="52"/>
+      <c r="W20" s="52"/>
+      <c r="X20" s="60"/>
+      <c r="Z20" s="34"/>
+      <c r="AA20" s="34"/>
+      <c r="AB20" s="34"/>
+      <c r="AC20" s="34"/>
+      <c r="AD20" s="34"/>
+      <c r="AF20" s="35"/>
+      <c r="AG20" s="35"/>
+      <c r="AH20" s="35"/>
+      <c r="AI20" s="35"/>
+      <c r="AJ20" s="35"/>
+      <c r="AK20" s="35"/>
     </row>
     <row r="21" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="77"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="125"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="70"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="82"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="81" t="s">
+      <c r="Q21" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="82"/>
-      <c r="S21" s="82"/>
-      <c r="T21" s="82"/>
-      <c r="U21" s="82"/>
-      <c r="V21" s="82"/>
-      <c r="W21" s="82"/>
-      <c r="X21" s="83"/>
-      <c r="Z21" s="126"/>
-      <c r="AA21" s="126"/>
-      <c r="AB21" s="126"/>
-      <c r="AC21" s="126"/>
-      <c r="AD21" s="126"/>
-      <c r="AF21" s="127"/>
-      <c r="AG21" s="127"/>
-      <c r="AH21" s="127"/>
-      <c r="AI21" s="127"/>
-      <c r="AJ21" s="127"/>
-      <c r="AK21" s="127"/>
+      <c r="R21" s="127"/>
+      <c r="S21" s="127"/>
+      <c r="T21" s="127"/>
+      <c r="U21" s="127"/>
+      <c r="V21" s="127"/>
+      <c r="W21" s="127"/>
+      <c r="X21" s="128"/>
+      <c r="Z21" s="34"/>
+      <c r="AA21" s="34"/>
+      <c r="AB21" s="34"/>
+      <c r="AC21" s="34"/>
+      <c r="AD21" s="34"/>
+      <c r="AF21" s="35"/>
+      <c r="AG21" s="35"/>
+      <c r="AH21" s="35"/>
+      <c r="AI21" s="35"/>
+      <c r="AJ21" s="35"/>
+      <c r="AK21" s="35"/>
     </row>
     <row r="22" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="69" t="s">
+      <c r="L22" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="70"/>
+      <c r="M22" s="82"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
-      <c r="Z22" s="126"/>
-      <c r="AA22" s="126"/>
-      <c r="AB22" s="126"/>
-      <c r="AC22" s="126"/>
-      <c r="AD22" s="126"/>
-      <c r="AF22" s="127"/>
-      <c r="AG22" s="127"/>
-      <c r="AH22" s="127"/>
-      <c r="AI22" s="127"/>
-      <c r="AJ22" s="127"/>
-      <c r="AK22" s="127"/>
+      <c r="Z22" s="34"/>
+      <c r="AA22" s="34"/>
+      <c r="AB22" s="34"/>
+      <c r="AC22" s="34"/>
+      <c r="AD22" s="34"/>
+      <c r="AF22" s="35"/>
+      <c r="AG22" s="35"/>
+      <c r="AH22" s="35"/>
+      <c r="AI22" s="35"/>
+      <c r="AJ22" s="35"/>
+      <c r="AK22" s="35"/>
     </row>
     <row r="23" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="78" t="s">
+      <c r="E23" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="79"/>
-      <c r="G23" s="84"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="53"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="70"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="82"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="85" t="s">
+      <c r="Q23" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="86"/>
-      <c r="S23" s="86"/>
-      <c r="T23" s="86"/>
-      <c r="U23" s="86"/>
-      <c r="V23" s="86"/>
-      <c r="W23" s="86"/>
-      <c r="X23" s="87"/>
-      <c r="Z23" s="126"/>
-      <c r="AA23" s="126"/>
-      <c r="AB23" s="126"/>
-      <c r="AC23" s="126"/>
-      <c r="AD23" s="126"/>
-      <c r="AF23" s="127"/>
-      <c r="AG23" s="127"/>
-      <c r="AH23" s="127"/>
-      <c r="AI23" s="127"/>
-      <c r="AJ23" s="127"/>
-      <c r="AK23" s="127"/>
+      <c r="R23" s="84"/>
+      <c r="S23" s="84"/>
+      <c r="T23" s="84"/>
+      <c r="U23" s="84"/>
+      <c r="V23" s="84"/>
+      <c r="W23" s="84"/>
+      <c r="X23" s="85"/>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="34"/>
+      <c r="AB23" s="34"/>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="34"/>
+      <c r="AF23" s="35"/>
+      <c r="AG23" s="35"/>
+      <c r="AH23" s="35"/>
+      <c r="AI23" s="35"/>
+      <c r="AJ23" s="35"/>
+      <c r="AK23" s="35"/>
     </row>
     <row r="24" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="69" t="s">
+      <c r="L24" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="70"/>
+      <c r="M24" s="82"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="88"/>
-      <c r="R24" s="89"/>
-      <c r="S24" s="89"/>
-      <c r="T24" s="89"/>
-      <c r="U24" s="89"/>
-      <c r="V24" s="89"/>
-      <c r="W24" s="89"/>
-      <c r="X24" s="90"/>
-      <c r="Z24" s="126"/>
-      <c r="AA24" s="126"/>
-      <c r="AB24" s="126"/>
-      <c r="AC24" s="126"/>
-      <c r="AD24" s="126"/>
-      <c r="AF24" s="127"/>
-      <c r="AG24" s="127"/>
-      <c r="AH24" s="127"/>
-      <c r="AI24" s="127"/>
-      <c r="AJ24" s="127"/>
-      <c r="AK24" s="127"/>
+      <c r="Q24" s="86"/>
+      <c r="R24" s="87"/>
+      <c r="S24" s="87"/>
+      <c r="T24" s="87"/>
+      <c r="U24" s="87"/>
+      <c r="V24" s="87"/>
+      <c r="W24" s="87"/>
+      <c r="X24" s="88"/>
+      <c r="Z24" s="34"/>
+      <c r="AA24" s="34"/>
+      <c r="AB24" s="34"/>
+      <c r="AC24" s="34"/>
+      <c r="AD24" s="34"/>
+      <c r="AF24" s="35"/>
+      <c r="AG24" s="35"/>
+      <c r="AH24" s="35"/>
+      <c r="AI24" s="35"/>
+      <c r="AJ24" s="35"/>
+      <c r="AK24" s="35"/>
     </row>
     <row r="25" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="L25" s="81"/>
+      <c r="M25" s="82"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="91"/>
-      <c r="R25" s="92"/>
-      <c r="S25" s="92"/>
-      <c r="T25" s="92"/>
-      <c r="U25" s="92"/>
-      <c r="V25" s="92"/>
-      <c r="W25" s="92"/>
-      <c r="X25" s="93"/>
-      <c r="Z25" s="126"/>
-      <c r="AA25" s="126"/>
-      <c r="AB25" s="126"/>
-      <c r="AC25" s="126"/>
-      <c r="AD25" s="126"/>
-      <c r="AF25" s="127"/>
-      <c r="AG25" s="127"/>
-      <c r="AH25" s="127"/>
-      <c r="AI25" s="127"/>
-      <c r="AJ25" s="127"/>
-      <c r="AK25" s="127"/>
+      <c r="Q25" s="89"/>
+      <c r="R25" s="90"/>
+      <c r="S25" s="90"/>
+      <c r="T25" s="90"/>
+      <c r="U25" s="90"/>
+      <c r="V25" s="90"/>
+      <c r="W25" s="90"/>
+      <c r="X25" s="91"/>
+      <c r="Z25" s="34"/>
+      <c r="AA25" s="34"/>
+      <c r="AB25" s="34"/>
+      <c r="AC25" s="34"/>
+      <c r="AD25" s="34"/>
+      <c r="AF25" s="35"/>
+      <c r="AG25" s="35"/>
+      <c r="AH25" s="35"/>
+      <c r="AI25" s="35"/>
+      <c r="AJ25" s="35"/>
+      <c r="AK25" s="35"/>
     </row>
     <row r="26" spans="1:37" ht="15" customHeight="1" thickTop="1">
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="79"/>
-      <c r="J26" s="79"/>
-      <c r="K26" s="84"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="53"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="100" t="s">
+      <c r="Q26" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="101"/>
-      <c r="S26" s="101"/>
-      <c r="T26" s="101"/>
-      <c r="U26" s="101"/>
-      <c r="V26" s="101"/>
-      <c r="W26" s="101"/>
-      <c r="X26" s="102"/>
-      <c r="Z26" s="126"/>
-      <c r="AA26" s="126"/>
-      <c r="AB26" s="126"/>
-      <c r="AC26" s="126"/>
-      <c r="AD26" s="126"/>
-      <c r="AF26" s="126"/>
-      <c r="AG26" s="126"/>
-      <c r="AH26" s="126"/>
-      <c r="AI26" s="126"/>
-      <c r="AJ26" s="126"/>
-      <c r="AK26" s="126"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="56"/>
+      <c r="Z26" s="34"/>
+      <c r="AA26" s="34"/>
+      <c r="AB26" s="34"/>
+      <c r="AC26" s="34"/>
+      <c r="AD26" s="34"/>
+      <c r="AF26" s="34"/>
+      <c r="AG26" s="34"/>
+      <c r="AH26" s="34"/>
+      <c r="AI26" s="34"/>
+      <c r="AJ26" s="34"/>
+      <c r="AK26" s="34"/>
     </row>
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="103"/>
-      <c r="R27" s="104"/>
-      <c r="S27" s="104"/>
-      <c r="T27" s="104"/>
-      <c r="U27" s="104"/>
-      <c r="V27" s="104"/>
-      <c r="W27" s="104"/>
-      <c r="X27" s="105"/>
-      <c r="Z27" s="126"/>
-      <c r="AA27" s="126"/>
-      <c r="AB27" s="126"/>
-      <c r="AC27" s="126"/>
-      <c r="AD27" s="126"/>
-      <c r="AF27" s="126"/>
-      <c r="AG27" s="126"/>
-      <c r="AH27" s="126"/>
-      <c r="AI27" s="126"/>
-      <c r="AJ27" s="126"/>
-      <c r="AK27" s="126"/>
+      <c r="Q27" s="57"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="59"/>
+      <c r="Z27" s="34"/>
+      <c r="AA27" s="34"/>
+      <c r="AB27" s="34"/>
+      <c r="AC27" s="34"/>
+      <c r="AD27" s="34"/>
+      <c r="AF27" s="34"/>
+      <c r="AG27" s="34"/>
+      <c r="AH27" s="34"/>
+      <c r="AI27" s="34"/>
+      <c r="AJ27" s="34"/>
+      <c r="AK27" s="34"/>
     </row>
     <row r="28" spans="1:37" ht="15" customHeight="1">
       <c r="N28" s="12"/>
       <c r="O28" s="14"/>
       <c r="X28" s="13"/>
-      <c r="Z28" s="126"/>
-      <c r="AA28" s="126"/>
-      <c r="AB28" s="126"/>
-      <c r="AC28" s="126"/>
-      <c r="AD28" s="126"/>
-      <c r="AF28" s="126"/>
-      <c r="AG28" s="126"/>
-      <c r="AH28" s="126"/>
-      <c r="AI28" s="126"/>
-      <c r="AJ28" s="126"/>
-      <c r="AK28" s="126"/>
+      <c r="Z28" s="34"/>
+      <c r="AA28" s="34"/>
+      <c r="AB28" s="34"/>
+      <c r="AC28" s="34"/>
+      <c r="AD28" s="34"/>
+      <c r="AF28" s="34"/>
+      <c r="AG28" s="34"/>
+      <c r="AH28" s="34"/>
+      <c r="AI28" s="34"/>
+      <c r="AJ28" s="34"/>
+      <c r="AK28" s="34"/>
     </row>
     <row r="29" spans="1:37" ht="15" customHeight="1">
       <c r="N29" s="12"/>
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="78" t="s">
+      <c r="Q29" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="79"/>
-      <c r="S29" s="79"/>
-      <c r="T29" s="79"/>
-      <c r="U29" s="79"/>
-      <c r="V29" s="79"/>
-      <c r="W29" s="79"/>
-      <c r="X29" s="80"/>
-      <c r="Z29" s="126"/>
-      <c r="AA29" s="126"/>
-      <c r="AB29" s="126"/>
-      <c r="AC29" s="126"/>
-      <c r="AD29" s="126"/>
-      <c r="AF29" s="126"/>
-      <c r="AG29" s="126"/>
-      <c r="AH29" s="126"/>
-      <c r="AI29" s="126"/>
-      <c r="AJ29" s="126"/>
-      <c r="AK29" s="126"/>
+      <c r="R29" s="52"/>
+      <c r="S29" s="52"/>
+      <c r="T29" s="52"/>
+      <c r="U29" s="52"/>
+      <c r="V29" s="52"/>
+      <c r="W29" s="52"/>
+      <c r="X29" s="60"/>
+      <c r="Z29" s="34"/>
+      <c r="AA29" s="34"/>
+      <c r="AB29" s="34"/>
+      <c r="AC29" s="34"/>
+      <c r="AD29" s="34"/>
+      <c r="AF29" s="34"/>
+      <c r="AG29" s="34"/>
+      <c r="AH29" s="34"/>
+      <c r="AI29" s="34"/>
+      <c r="AJ29" s="34"/>
+      <c r="AK29" s="34"/>
     </row>
     <row r="30" spans="1:37" ht="15" customHeight="1">
       <c r="A30" s="8"/>
@@ -3355,93 +3307,93 @@
       <c r="N30" s="12"/>
       <c r="O30" s="14"/>
       <c r="X30" s="13"/>
-      <c r="Z30" s="126"/>
-      <c r="AA30" s="126"/>
-      <c r="AB30" s="126"/>
-      <c r="AC30" s="126"/>
-      <c r="AD30" s="126"/>
-      <c r="AF30" s="126"/>
-      <c r="AG30" s="126"/>
-      <c r="AH30" s="126"/>
-      <c r="AI30" s="126"/>
-      <c r="AJ30" s="126"/>
-      <c r="AK30" s="126"/>
+      <c r="Z30" s="34"/>
+      <c r="AA30" s="34"/>
+      <c r="AB30" s="34"/>
+      <c r="AC30" s="34"/>
+      <c r="AD30" s="34"/>
+      <c r="AF30" s="34"/>
+      <c r="AG30" s="34"/>
+      <c r="AH30" s="34"/>
+      <c r="AI30" s="34"/>
+      <c r="AJ30" s="34"/>
+      <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="106" t="s">
+      <c r="A31" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="106"/>
-      <c r="C31" s="106"/>
-      <c r="D31" s="106"/>
-      <c r="E31" s="106"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="106"/>
-      <c r="H31" s="106"/>
-      <c r="I31" s="106"/>
-      <c r="J31" s="106"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="107" t="s">
+      <c r="P31" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="108"/>
-      <c r="R31" s="108"/>
-      <c r="S31" s="108"/>
-      <c r="T31" s="108"/>
-      <c r="U31" s="108"/>
-      <c r="V31" s="108"/>
-      <c r="W31" s="109"/>
+      <c r="Q31" s="63"/>
+      <c r="R31" s="63"/>
+      <c r="S31" s="63"/>
+      <c r="T31" s="63"/>
+      <c r="U31" s="63"/>
+      <c r="V31" s="63"/>
+      <c r="W31" s="64"/>
       <c r="X31" s="13"/>
-      <c r="Z31" s="126"/>
-      <c r="AA31" s="126"/>
-      <c r="AB31" s="126"/>
-      <c r="AC31" s="126"/>
-      <c r="AD31" s="126"/>
-      <c r="AF31" s="126"/>
-      <c r="AG31" s="126"/>
-      <c r="AH31" s="126"/>
-      <c r="AI31" s="126"/>
-      <c r="AJ31" s="126"/>
-      <c r="AK31" s="126"/>
+      <c r="Z31" s="34"/>
+      <c r="AA31" s="34"/>
+      <c r="AB31" s="34"/>
+      <c r="AC31" s="34"/>
+      <c r="AD31" s="34"/>
+      <c r="AF31" s="34"/>
+      <c r="AG31" s="34"/>
+      <c r="AH31" s="34"/>
+      <c r="AI31" s="34"/>
+      <c r="AJ31" s="34"/>
+      <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="106"/>
-      <c r="B32" s="106"/>
-      <c r="C32" s="106"/>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="106"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="106"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="110"/>
-      <c r="Q32" s="111"/>
-      <c r="R32" s="111"/>
-      <c r="S32" s="111"/>
-      <c r="T32" s="111"/>
-      <c r="U32" s="111"/>
-      <c r="V32" s="111"/>
-      <c r="W32" s="112"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="66"/>
+      <c r="R32" s="66"/>
+      <c r="S32" s="66"/>
+      <c r="T32" s="66"/>
+      <c r="U32" s="66"/>
+      <c r="V32" s="66"/>
+      <c r="W32" s="67"/>
       <c r="X32" s="13"/>
-      <c r="Z32" s="126"/>
-      <c r="AA32" s="126"/>
-      <c r="AB32" s="126"/>
-      <c r="AC32" s="126"/>
-      <c r="AD32" s="126"/>
-      <c r="AF32" s="126"/>
-      <c r="AG32" s="126"/>
-      <c r="AH32" s="126"/>
-      <c r="AI32" s="126"/>
-      <c r="AJ32" s="126"/>
-      <c r="AK32" s="126"/>
+      <c r="Z32" s="34"/>
+      <c r="AA32" s="34"/>
+      <c r="AB32" s="34"/>
+      <c r="AC32" s="34"/>
+      <c r="AD32" s="34"/>
+      <c r="AF32" s="34"/>
+      <c r="AG32" s="34"/>
+      <c r="AH32" s="34"/>
+      <c r="AI32" s="34"/>
+      <c r="AJ32" s="34"/>
+      <c r="AK32" s="34"/>
     </row>
     <row r="33" spans="1:37" ht="15" customHeight="1">
       <c r="A33" s="15"/>
@@ -3458,184 +3410,184 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="110"/>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="111"/>
-      <c r="S33" s="111"/>
-      <c r="T33" s="111"/>
-      <c r="U33" s="111"/>
-      <c r="V33" s="111"/>
-      <c r="W33" s="112"/>
+      <c r="P33" s="65"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="66"/>
+      <c r="S33" s="66"/>
+      <c r="T33" s="66"/>
+      <c r="U33" s="66"/>
+      <c r="V33" s="66"/>
+      <c r="W33" s="67"/>
       <c r="X33" s="13"/>
-      <c r="Z33" s="126"/>
-      <c r="AA33" s="126"/>
-      <c r="AB33" s="126"/>
-      <c r="AC33" s="126"/>
-      <c r="AD33" s="126"/>
-      <c r="AF33" s="126"/>
-      <c r="AG33" s="126"/>
-      <c r="AH33" s="126"/>
-      <c r="AI33" s="126"/>
-      <c r="AJ33" s="126"/>
-      <c r="AK33" s="126"/>
+      <c r="Z33" s="34"/>
+      <c r="AA33" s="34"/>
+      <c r="AB33" s="34"/>
+      <c r="AC33" s="34"/>
+      <c r="AD33" s="34"/>
+      <c r="AF33" s="34"/>
+      <c r="AG33" s="34"/>
+      <c r="AH33" s="34"/>
+      <c r="AI33" s="34"/>
+      <c r="AJ33" s="34"/>
+      <c r="AK33" s="34"/>
     </row>
     <row r="34" spans="1:37" ht="15" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="116"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="71"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="110"/>
-      <c r="Q34" s="111"/>
-      <c r="R34" s="111"/>
-      <c r="S34" s="111"/>
-      <c r="T34" s="111"/>
-      <c r="U34" s="111"/>
-      <c r="V34" s="111"/>
-      <c r="W34" s="112"/>
+      <c r="P34" s="65"/>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="66"/>
+      <c r="S34" s="66"/>
+      <c r="T34" s="66"/>
+      <c r="U34" s="66"/>
+      <c r="V34" s="66"/>
+      <c r="W34" s="67"/>
       <c r="X34" s="13"/>
-      <c r="Z34" s="126"/>
-      <c r="AA34" s="126"/>
-      <c r="AB34" s="126"/>
-      <c r="AC34" s="126"/>
-      <c r="AD34" s="126"/>
-      <c r="AF34" s="126"/>
-      <c r="AG34" s="126"/>
-      <c r="AH34" s="126"/>
-      <c r="AI34" s="126"/>
-      <c r="AJ34" s="126"/>
-      <c r="AK34" s="126"/>
+      <c r="Z34" s="34"/>
+      <c r="AA34" s="34"/>
+      <c r="AB34" s="34"/>
+      <c r="AC34" s="34"/>
+      <c r="AD34" s="34"/>
+      <c r="AF34" s="34"/>
+      <c r="AG34" s="34"/>
+      <c r="AH34" s="34"/>
+      <c r="AI34" s="34"/>
+      <c r="AJ34" s="34"/>
+      <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="116" t="s">
+      <c r="A35" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="117" t="s">
+      <c r="B35" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="118"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="118"/>
-      <c r="J35" s="118"/>
-      <c r="K35" s="119"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="74"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="110"/>
-      <c r="Q35" s="111"/>
-      <c r="R35" s="111"/>
-      <c r="S35" s="111"/>
-      <c r="T35" s="111"/>
-      <c r="U35" s="111"/>
-      <c r="V35" s="111"/>
-      <c r="W35" s="112"/>
+      <c r="P35" s="65"/>
+      <c r="Q35" s="66"/>
+      <c r="R35" s="66"/>
+      <c r="S35" s="66"/>
+      <c r="T35" s="66"/>
+      <c r="U35" s="66"/>
+      <c r="V35" s="66"/>
+      <c r="W35" s="67"/>
       <c r="X35" s="13"/>
-      <c r="Z35" s="126"/>
-      <c r="AA35" s="126"/>
-      <c r="AB35" s="126"/>
-      <c r="AC35" s="126"/>
-      <c r="AD35" s="126"/>
-      <c r="AF35" s="126"/>
-      <c r="AG35" s="126"/>
-      <c r="AH35" s="126"/>
-      <c r="AI35" s="126"/>
-      <c r="AJ35" s="126"/>
-      <c r="AK35" s="126"/>
+      <c r="Z35" s="34"/>
+      <c r="AA35" s="34"/>
+      <c r="AB35" s="34"/>
+      <c r="AC35" s="34"/>
+      <c r="AD35" s="34"/>
+      <c r="AF35" s="34"/>
+      <c r="AG35" s="34"/>
+      <c r="AH35" s="34"/>
+      <c r="AI35" s="34"/>
+      <c r="AJ35" s="34"/>
+      <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="116"/>
-      <c r="B36" s="120"/>
-      <c r="C36" s="121"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="121"/>
-      <c r="F36" s="121"/>
-      <c r="G36" s="121"/>
-      <c r="H36" s="121"/>
-      <c r="I36" s="121"/>
-      <c r="J36" s="121"/>
-      <c r="K36" s="122"/>
+      <c r="A36" s="71"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="77"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="110"/>
-      <c r="Q36" s="111"/>
-      <c r="R36" s="111"/>
-      <c r="S36" s="111"/>
-      <c r="T36" s="111"/>
-      <c r="U36" s="111"/>
-      <c r="V36" s="111"/>
-      <c r="W36" s="112"/>
+      <c r="P36" s="65"/>
+      <c r="Q36" s="66"/>
+      <c r="R36" s="66"/>
+      <c r="S36" s="66"/>
+      <c r="T36" s="66"/>
+      <c r="U36" s="66"/>
+      <c r="V36" s="66"/>
+      <c r="W36" s="67"/>
       <c r="X36" s="13"/>
-      <c r="Z36" s="126"/>
-      <c r="AA36" s="126"/>
-      <c r="AB36" s="126"/>
-      <c r="AC36" s="126"/>
-      <c r="AD36" s="126"/>
-      <c r="AF36" s="126"/>
-      <c r="AG36" s="126"/>
-      <c r="AH36" s="126"/>
-      <c r="AI36" s="126"/>
-      <c r="AJ36" s="126"/>
-      <c r="AK36" s="126"/>
+      <c r="Z36" s="34"/>
+      <c r="AA36" s="34"/>
+      <c r="AB36" s="34"/>
+      <c r="AC36" s="34"/>
+      <c r="AD36" s="34"/>
+      <c r="AF36" s="34"/>
+      <c r="AG36" s="34"/>
+      <c r="AH36" s="34"/>
+      <c r="AI36" s="34"/>
+      <c r="AJ36" s="34"/>
+      <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="116"/>
-      <c r="B37" s="123"/>
-      <c r="C37" s="124"/>
-      <c r="D37" s="124"/>
-      <c r="E37" s="124"/>
-      <c r="F37" s="124"/>
-      <c r="G37" s="124"/>
-      <c r="H37" s="124"/>
-      <c r="I37" s="124"/>
-      <c r="J37" s="124"/>
-      <c r="K37" s="125"/>
+      <c r="A37" s="71"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="79"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="80"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="113"/>
-      <c r="Q37" s="114"/>
-      <c r="R37" s="114"/>
-      <c r="S37" s="114"/>
-      <c r="T37" s="114"/>
-      <c r="U37" s="114"/>
-      <c r="V37" s="114"/>
-      <c r="W37" s="115"/>
+      <c r="P37" s="68"/>
+      <c r="Q37" s="69"/>
+      <c r="R37" s="69"/>
+      <c r="S37" s="69"/>
+      <c r="T37" s="69"/>
+      <c r="U37" s="69"/>
+      <c r="V37" s="69"/>
+      <c r="W37" s="70"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="97" t="s">
+      <c r="B38" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="98"/>
-      <c r="D38" s="98"/>
-      <c r="E38" s="98"/>
-      <c r="F38" s="98"/>
-      <c r="G38" s="98"/>
-      <c r="H38" s="98"/>
-      <c r="I38" s="98"/>
-      <c r="J38" s="98"/>
-      <c r="K38" s="99"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="47"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3653,36 +3605,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="97" t="s">
+      <c r="B39" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="98"/>
-      <c r="D39" s="98"/>
-      <c r="E39" s="98"/>
-      <c r="F39" s="98"/>
-      <c r="G39" s="98"/>
-      <c r="H39" s="98"/>
-      <c r="I39" s="98"/>
-      <c r="J39" s="98"/>
-      <c r="K39" s="99"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="47"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="97" t="s">
+      <c r="B40" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="98"/>
-      <c r="D40" s="98"/>
-      <c r="E40" s="98"/>
-      <c r="F40" s="98"/>
-      <c r="G40" s="98"/>
-      <c r="H40" s="98"/>
-      <c r="I40" s="98"/>
-      <c r="J40" s="98"/>
-      <c r="K40" s="99"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="47"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -3701,76 +3653,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="97" t="s">
+      <c r="B41" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="98"/>
-      <c r="D41" s="98"/>
-      <c r="E41" s="98"/>
-      <c r="F41" s="98"/>
-      <c r="G41" s="98"/>
-      <c r="H41" s="98"/>
-      <c r="I41" s="98"/>
-      <c r="J41" s="98"/>
-      <c r="K41" s="99"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="47"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="94" t="s">
+      <c r="M41" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="95"/>
-      <c r="O41" s="95"/>
-      <c r="P41" s="95"/>
-      <c r="Q41" s="95"/>
-      <c r="R41" s="95"/>
-      <c r="S41" s="95"/>
-      <c r="T41" s="95"/>
-      <c r="U41" s="95"/>
-      <c r="V41" s="95"/>
-      <c r="W41" s="95"/>
-      <c r="X41" s="96"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="49"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="49"/>
+      <c r="U41" s="49"/>
+      <c r="V41" s="49"/>
+      <c r="W41" s="49"/>
+      <c r="X41" s="50"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="97"/>
-      <c r="C42" s="98"/>
-      <c r="D42" s="98"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="98"/>
-      <c r="G42" s="98"/>
-      <c r="H42" s="98"/>
-      <c r="I42" s="98"/>
-      <c r="J42" s="98"/>
-      <c r="K42" s="99"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="47"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="94" t="s">
+      <c r="M42" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="95"/>
-      <c r="O42" s="95"/>
-      <c r="P42" s="95"/>
-      <c r="Q42" s="95"/>
-      <c r="R42" s="95"/>
-      <c r="S42" s="95"/>
-      <c r="T42" s="95"/>
-      <c r="U42" s="95"/>
-      <c r="V42" s="95"/>
-      <c r="W42" s="95"/>
-      <c r="X42" s="96"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="49"/>
+      <c r="U42" s="49"/>
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="50"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="97"/>
-      <c r="C43" s="98"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="98"/>
-      <c r="H43" s="98"/>
-      <c r="I43" s="98"/>
-      <c r="J43" s="98"/>
-      <c r="K43" s="99"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="47"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -3788,16 +3740,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="98"/>
-      <c r="G44" s="98"/>
-      <c r="H44" s="98"/>
-      <c r="I44" s="98"/>
-      <c r="J44" s="98"/>
-      <c r="K44" s="99"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="47"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -3815,16 +3767,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="97"/>
-      <c r="C45" s="98"/>
-      <c r="D45" s="98"/>
-      <c r="E45" s="98"/>
-      <c r="F45" s="98"/>
-      <c r="G45" s="98"/>
-      <c r="H45" s="98"/>
-      <c r="I45" s="98"/>
-      <c r="J45" s="98"/>
-      <c r="K45" s="99"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="47"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -3842,16 +3794,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="97"/>
-      <c r="C46" s="98"/>
-      <c r="D46" s="98"/>
-      <c r="E46" s="98"/>
-      <c r="F46" s="98"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="98"/>
-      <c r="I46" s="98"/>
-      <c r="J46" s="98"/>
-      <c r="K46" s="99"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="47"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -3894,6 +3846,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:R10"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="Q19:X19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="M41:X41"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:K37"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
     <mergeCell ref="Y1:Z3"/>
     <mergeCell ref="B43:K43"/>
     <mergeCell ref="B44:K44"/>
@@ -3910,32 +3888,6 @@
     <mergeCell ref="Q29:X29"/>
     <mergeCell ref="A31:J32"/>
     <mergeCell ref="P31:W37"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:K37"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="M41:X41"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="Q19:X19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="J9:L10"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
lots to do do but working make a laptop functional copy tommorrow ready for testing with new board at woodys
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="-240" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="9360" yWindow="-240" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Design peddle pirotS! (2)" sheetId="4" r:id="rId1"/>
+    <sheet name="To do" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -261,6 +262,147 @@
   </si>
   <si>
     <t>GM - hold info</t>
+  </si>
+  <si>
+    <t>make rects worked out at the end so if ppl drop out dont get wrong devision of screen</t>
+  </si>
+  <si>
+    <t>play test speeds of player and get right numbers</t>
+  </si>
+  <si>
+    <t>set all tags on boats</t>
+  </si>
+  <si>
+    <t>lights need to turn off during day</t>
+  </si>
+  <si>
+    <t>cannon ball needs to be parented to spawning transform</t>
+  </si>
+  <si>
+    <t>tactical cam off bow sides</t>
+  </si>
+  <si>
+    <t>do green the yellow orange red blue white is it necessary - pink get playtest feed back give them experience of two options</t>
+  </si>
+  <si>
+    <t>redo land so dont get stuck going forward maybe lots of bounce or some kind of current push</t>
+  </si>
+  <si>
+    <t>find solution to display health - flag damage using a material layer?</t>
+  </si>
+  <si>
+    <t>setup option attack only humans</t>
+  </si>
+  <si>
+    <t>stop coroutine fire, stop friendly targetting, stop shooting when an enemy falls</t>
+  </si>
+  <si>
+    <t>replace tags sorting layers</t>
+  </si>
+  <si>
+    <t>box around drop boxes and tick box or colour code panel behind so clear what tick box for</t>
+  </si>
+  <si>
+    <t>check right side player guns</t>
+  </si>
+  <si>
+    <t>bigger more visable cannon balls</t>
+  </si>
+  <si>
+    <t>on death top down view or and pirate flag over screen</t>
+  </si>
+  <si>
+    <t>reset the thisplayersetting</t>
+  </si>
+  <si>
+    <t>reset the setup if everyone drops out</t>
+  </si>
+  <si>
+    <t>player prefs so that can skip team set up stage and set max</t>
+  </si>
+  <si>
+    <t>option for constant respawn constant play so anyone can jump on play jump off</t>
+  </si>
+  <si>
+    <t>esc to return to setup</t>
+  </si>
+  <si>
+    <t>daycycle starts at game start</t>
+  </si>
+  <si>
+    <t>check count ships</t>
+  </si>
+  <si>
+    <t>check max bar working properly saught text</t>
+  </si>
+  <si>
+    <t>put arduino code into the pedal pirates file</t>
+  </si>
+  <si>
+    <t>read through notes made so far in notes document</t>
+  </si>
+  <si>
+    <t>angle change of boat or spray as turn or lean so feel the turn</t>
+  </si>
+  <si>
+    <t>laptop version for Wednesday and optomise</t>
+  </si>
+  <si>
+    <t>check why returns true for wrong baudrate on arduino</t>
+  </si>
+  <si>
+    <t>error handler spelling changed with anduino version and uncomment in arduino code - is this why getting odd results at times</t>
+  </si>
+  <si>
+    <t>do ai bump?</t>
+  </si>
+  <si>
+    <t>playerscript for ai make ai as similar to player as possible to make more options easier to code so ai has as much shared functionality as possible</t>
+  </si>
+  <si>
+    <t>shorten win screen visual</t>
+  </si>
+  <si>
+    <t>redo pirate text</t>
+  </si>
+  <si>
+    <t>android monitor on bike and button to divert power to shooting</t>
+  </si>
+  <si>
+    <t>sfx</t>
+  </si>
+  <si>
+    <t>ram damage ram script and black flags when ai go to ram made</t>
+  </si>
+  <si>
+    <t>check bow damage</t>
+  </si>
+  <si>
+    <t>win conditions in setup, last one standing inc ex ai, race - winner has most health and loads health drop so collection race</t>
+  </si>
+  <si>
+    <t>alternate map for racing linear start end start port end port</t>
+  </si>
+  <si>
+    <t>health drop reverse ship damage</t>
+  </si>
+  <si>
+    <t>hi graphic and low graphic mode</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>family mode kid bike and adut bikes drop fdown volt max range</t>
+  </si>
+  <si>
+    <t>explosion graphic</t>
+  </si>
+  <si>
+    <t>do something with team names etc</t>
+  </si>
+  <si>
+    <t>individual win screns in middle screen countdown to next game</t>
   </si>
 </sst>
 </file>
@@ -418,7 +560,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,6 +610,84 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="56">
     <border>
@@ -1146,7 +1366,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1262,6 +1482,225 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1287,24 +1726,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1325,9 +1746,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1358,204 +1776,19 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -1568,6 +1801,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -2130,6 +2368,91 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7886699" cy="3800474"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2590800" y="1809751"/>
+          <a:ext cx="7886699" cy="3800474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="9600" b="1" cap="none" spc="0">
+              <a:ln w="10541" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:shade val="88000"/>
+                    <a:satMod val="110000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="40000"/>
+                      <a:satMod val="250000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="9000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="52000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="20000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="79000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="52000"/>
+                      <a:satMod val="300000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:tint val="40000"/>
+                      <a:satMod val="250000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000"/>
+              </a:gradFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>old redo</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2420,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2436,14 +2759,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="Y1" s="39" t="s">
+      <c r="Y1" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="40"/>
+      <c r="Z1" s="113"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="42"/>
+      <c r="Y2" s="114"/>
+      <c r="Z2" s="115"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
       <c r="AH2" s="35"/>
@@ -2452,8 +2775,8 @@
       <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="44"/>
+      <c r="Y3" s="116"/>
+      <c r="Z3" s="117"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="38" t="s">
         <v>58</v>
@@ -2471,16 +2794,16 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="109"/>
-      <c r="D4" s="110"/>
-      <c r="G4" s="116" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="41"/>
+      <c r="G4" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="109"/>
-      <c r="I4" s="110"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
       <c r="Z4" s="34"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
@@ -2494,12 +2817,12 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="117"/>
-      <c r="C5" s="129"/>
-      <c r="D5" s="118"/>
-      <c r="G5" s="117"/>
-      <c r="H5" s="129"/>
-      <c r="I5" s="118"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
       <c r="Z5" s="34" t="s">
         <v>50</v>
       </c>
@@ -2541,12 +2864,12 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="131"/>
-      <c r="D7" s="131"/>
-      <c r="E7" s="132"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -2576,10 +2899,10 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="133"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="135"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2616,17 +2939,17 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="116" t="s">
+      <c r="J9" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="109"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
-      <c r="O9" s="109"/>
-      <c r="P9" s="109"/>
-      <c r="Q9" s="109"/>
-      <c r="R9" s="110"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="41"/>
       <c r="Z9" s="34" t="s">
         <v>69</v>
       </c>
@@ -2654,25 +2977,25 @@
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="136" t="s">
+      <c r="B10" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="136"/>
-      <c r="D10" s="136"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="129"/>
-      <c r="L10" s="129"/>
-      <c r="M10" s="129"/>
-      <c r="N10" s="129"/>
-      <c r="O10" s="129"/>
-      <c r="P10" s="129"/>
-      <c r="Q10" s="129"/>
-      <c r="R10" s="118"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="44"/>
       <c r="Z10" s="34">
         <v>20</v>
       </c>
@@ -2704,10 +3027,10 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="92" t="s">
+      <c r="G11" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="93"/>
+      <c r="H11" s="87"/>
       <c r="I11" s="28"/>
       <c r="Z11" s="34">
         <v>5</v>
@@ -2743,16 +3066,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="94" t="s">
+      <c r="L12" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="95"/>
-      <c r="N12" s="95"/>
-      <c r="O12" s="95"/>
-      <c r="P12" s="95"/>
-      <c r="Q12" s="95"/>
-      <c r="R12" s="95"/>
-      <c r="S12" s="96"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="53"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="88"/>
       <c r="Z12" s="34"/>
       <c r="AA12" s="34"/>
       <c r="AB12" s="34"/>
@@ -2775,14 +3098,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="98"/>
-      <c r="Q13" s="98"/>
-      <c r="R13" s="98"/>
-      <c r="S13" s="99"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="89"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -2826,16 +3149,16 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="100" t="s">
+      <c r="Q15" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="101"/>
-      <c r="S15" s="101"/>
-      <c r="T15" s="101"/>
-      <c r="U15" s="101"/>
-      <c r="V15" s="101"/>
-      <c r="W15" s="101"/>
-      <c r="X15" s="102"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="91"/>
+      <c r="X15" s="92"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -2853,19 +3176,19 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="109" t="s">
+      <c r="M16" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="109"/>
-      <c r="O16" s="110"/>
-      <c r="Q16" s="103"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="104"/>
-      <c r="U16" s="104"/>
-      <c r="V16" s="104"/>
-      <c r="W16" s="104"/>
-      <c r="X16" s="105"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="41"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="94"/>
+      <c r="S16" s="94"/>
+      <c r="T16" s="94"/>
+      <c r="U16" s="94"/>
+      <c r="V16" s="94"/>
+      <c r="W16" s="94"/>
+      <c r="X16" s="95"/>
       <c r="Z16" s="34"/>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
@@ -2879,31 +3202,31 @@
       <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="95"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="113" t="s">
+      <c r="E17" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="114"/>
-      <c r="G17" s="115"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="111"/>
-      <c r="N17" s="111"/>
-      <c r="O17" s="112"/>
-      <c r="Q17" s="106"/>
-      <c r="R17" s="107"/>
-      <c r="S17" s="107"/>
-      <c r="T17" s="107"/>
-      <c r="U17" s="107"/>
-      <c r="V17" s="107"/>
-      <c r="W17" s="107"/>
-      <c r="X17" s="108"/>
+      <c r="M17" s="99"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="100"/>
+      <c r="Q17" s="96"/>
+      <c r="R17" s="97"/>
+      <c r="S17" s="97"/>
+      <c r="T17" s="97"/>
+      <c r="U17" s="97"/>
+      <c r="V17" s="97"/>
+      <c r="W17" s="97"/>
+      <c r="X17" s="98"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -2917,18 +3240,18 @@
       <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="97"/>
-      <c r="C18" s="98"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="81" t="s">
+      <c r="L18" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="82"/>
+      <c r="M18" s="60"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -2953,32 +3276,32 @@
       <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="110"/>
+      <c r="C19" s="41"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="82"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="60"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="119" t="s">
+      <c r="Q19" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="120"/>
-      <c r="S19" s="120"/>
-      <c r="T19" s="120"/>
-      <c r="U19" s="120"/>
-      <c r="V19" s="120"/>
-      <c r="W19" s="120"/>
-      <c r="X19" s="121"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="62"/>
+      <c r="U19" s="62"/>
+      <c r="V19" s="62"/>
+      <c r="W19" s="62"/>
+      <c r="X19" s="63"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -2992,32 +3315,32 @@
       <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
-      <c r="F20" s="122" t="s">
+      <c r="B20" s="42"/>
+      <c r="C20" s="44"/>
+      <c r="F20" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="123"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="81" t="s">
+      <c r="L20" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="82"/>
+      <c r="M20" s="60"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="51" t="s">
+      <c r="Q20" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="52"/>
-      <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
-      <c r="U20" s="52"/>
-      <c r="V20" s="52"/>
-      <c r="W20" s="52"/>
-      <c r="X20" s="60"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="69"/>
+      <c r="T20" s="69"/>
+      <c r="U20" s="69"/>
+      <c r="V20" s="69"/>
+      <c r="W20" s="69"/>
+      <c r="X20" s="70"/>
       <c r="Z20" s="34"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
@@ -3034,28 +3357,28 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="125"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="82"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="60"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="126" t="s">
+      <c r="Q21" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="127"/>
-      <c r="S21" s="127"/>
-      <c r="T21" s="127"/>
-      <c r="U21" s="127"/>
-      <c r="V21" s="127"/>
-      <c r="W21" s="127"/>
-      <c r="X21" s="128"/>
+      <c r="R21" s="72"/>
+      <c r="S21" s="72"/>
+      <c r="T21" s="72"/>
+      <c r="U21" s="72"/>
+      <c r="V21" s="72"/>
+      <c r="W21" s="72"/>
+      <c r="X21" s="73"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -3073,10 +3396,10 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="81" t="s">
+      <c r="L22" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="82"/>
+      <c r="M22" s="60"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -3096,28 +3419,28 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="52"/>
-      <c r="G23" s="53"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="111"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="82"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="60"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="83" t="s">
+      <c r="Q23" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="84"/>
-      <c r="S23" s="84"/>
-      <c r="T23" s="84"/>
-      <c r="U23" s="84"/>
-      <c r="V23" s="84"/>
-      <c r="W23" s="84"/>
-      <c r="X23" s="85"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="75"/>
+      <c r="T23" s="75"/>
+      <c r="U23" s="75"/>
+      <c r="V23" s="75"/>
+      <c r="W23" s="75"/>
+      <c r="X23" s="76"/>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
@@ -3135,20 +3458,20 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="81" t="s">
+      <c r="L24" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="82"/>
+      <c r="M24" s="60"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="86"/>
-      <c r="R24" s="87"/>
-      <c r="S24" s="87"/>
-      <c r="T24" s="87"/>
-      <c r="U24" s="87"/>
-      <c r="V24" s="87"/>
-      <c r="W24" s="87"/>
-      <c r="X24" s="88"/>
+      <c r="Q24" s="77"/>
+      <c r="R24" s="78"/>
+      <c r="S24" s="78"/>
+      <c r="T24" s="78"/>
+      <c r="U24" s="78"/>
+      <c r="V24" s="78"/>
+      <c r="W24" s="78"/>
+      <c r="X24" s="79"/>
       <c r="Z24" s="34"/>
       <c r="AA24" s="34"/>
       <c r="AB24" s="34"/>
@@ -3166,18 +3489,18 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="81"/>
-      <c r="M25" s="82"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="60"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="89"/>
-      <c r="R25" s="90"/>
-      <c r="S25" s="90"/>
-      <c r="T25" s="90"/>
-      <c r="U25" s="90"/>
-      <c r="V25" s="90"/>
-      <c r="W25" s="90"/>
-      <c r="X25" s="91"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="81"/>
+      <c r="S25" s="81"/>
+      <c r="T25" s="81"/>
+      <c r="U25" s="81"/>
+      <c r="V25" s="81"/>
+      <c r="W25" s="81"/>
+      <c r="X25" s="82"/>
       <c r="Z25" s="34"/>
       <c r="AA25" s="34"/>
       <c r="AB25" s="34"/>
@@ -3194,26 +3517,26 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="53"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="111"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="54" t="s">
+      <c r="Q26" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="55"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="55"/>
-      <c r="U26" s="55"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="56"/>
+      <c r="R26" s="122"/>
+      <c r="S26" s="122"/>
+      <c r="T26" s="122"/>
+      <c r="U26" s="122"/>
+      <c r="V26" s="122"/>
+      <c r="W26" s="122"/>
+      <c r="X26" s="123"/>
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
       <c r="AB26" s="34"/>
@@ -3229,14 +3552,14 @@
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="57"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
-      <c r="T27" s="58"/>
-      <c r="U27" s="58"/>
-      <c r="V27" s="58"/>
-      <c r="W27" s="58"/>
-      <c r="X27" s="59"/>
+      <c r="Q27" s="124"/>
+      <c r="R27" s="125"/>
+      <c r="S27" s="125"/>
+      <c r="T27" s="125"/>
+      <c r="U27" s="125"/>
+      <c r="V27" s="125"/>
+      <c r="W27" s="125"/>
+      <c r="X27" s="126"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -3270,16 +3593,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="51" t="s">
+      <c r="Q29" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="52"/>
-      <c r="S29" s="52"/>
-      <c r="T29" s="52"/>
-      <c r="U29" s="52"/>
-      <c r="V29" s="52"/>
-      <c r="W29" s="52"/>
-      <c r="X29" s="60"/>
+      <c r="R29" s="69"/>
+      <c r="S29" s="69"/>
+      <c r="T29" s="69"/>
+      <c r="U29" s="69"/>
+      <c r="V29" s="69"/>
+      <c r="W29" s="69"/>
+      <c r="X29" s="70"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -3320,32 +3643,32 @@
       <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="61" t="s">
+      <c r="A31" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
+      <c r="B31" s="127"/>
+      <c r="C31" s="127"/>
+      <c r="D31" s="127"/>
+      <c r="E31" s="127"/>
+      <c r="F31" s="127"/>
+      <c r="G31" s="127"/>
+      <c r="H31" s="127"/>
+      <c r="I31" s="127"/>
+      <c r="J31" s="127"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="62" t="s">
+      <c r="P31" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="63"/>
-      <c r="S31" s="63"/>
-      <c r="T31" s="63"/>
-      <c r="U31" s="63"/>
-      <c r="V31" s="63"/>
-      <c r="W31" s="64"/>
+      <c r="Q31" s="129"/>
+      <c r="R31" s="129"/>
+      <c r="S31" s="129"/>
+      <c r="T31" s="129"/>
+      <c r="U31" s="129"/>
+      <c r="V31" s="129"/>
+      <c r="W31" s="130"/>
       <c r="X31" s="13"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
@@ -3360,28 +3683,28 @@
       <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="61"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
+      <c r="A32" s="127"/>
+      <c r="B32" s="127"/>
+      <c r="C32" s="127"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="127"/>
+      <c r="F32" s="127"/>
+      <c r="G32" s="127"/>
+      <c r="H32" s="127"/>
+      <c r="I32" s="127"/>
+      <c r="J32" s="127"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="65"/>
-      <c r="Q32" s="66"/>
-      <c r="R32" s="66"/>
-      <c r="S32" s="66"/>
-      <c r="T32" s="66"/>
-      <c r="U32" s="66"/>
-      <c r="V32" s="66"/>
-      <c r="W32" s="67"/>
+      <c r="P32" s="131"/>
+      <c r="Q32" s="132"/>
+      <c r="R32" s="132"/>
+      <c r="S32" s="132"/>
+      <c r="T32" s="132"/>
+      <c r="U32" s="132"/>
+      <c r="V32" s="132"/>
+      <c r="W32" s="133"/>
       <c r="X32" s="13"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
@@ -3410,14 +3733,14 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="65"/>
-      <c r="Q33" s="66"/>
-      <c r="R33" s="66"/>
-      <c r="S33" s="66"/>
-      <c r="T33" s="66"/>
-      <c r="U33" s="66"/>
-      <c r="V33" s="66"/>
-      <c r="W33" s="67"/>
+      <c r="P33" s="131"/>
+      <c r="Q33" s="132"/>
+      <c r="R33" s="132"/>
+      <c r="S33" s="132"/>
+      <c r="T33" s="132"/>
+      <c r="U33" s="132"/>
+      <c r="V33" s="132"/>
+      <c r="W33" s="133"/>
       <c r="X33" s="13"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="34"/>
@@ -3435,29 +3758,29 @@
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="71"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
+      <c r="K34" s="101"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="65"/>
-      <c r="Q34" s="66"/>
-      <c r="R34" s="66"/>
-      <c r="S34" s="66"/>
-      <c r="T34" s="66"/>
-      <c r="U34" s="66"/>
-      <c r="V34" s="66"/>
-      <c r="W34" s="67"/>
+      <c r="P34" s="131"/>
+      <c r="Q34" s="132"/>
+      <c r="R34" s="132"/>
+      <c r="S34" s="132"/>
+      <c r="T34" s="132"/>
+      <c r="U34" s="132"/>
+      <c r="V34" s="132"/>
+      <c r="W34" s="133"/>
       <c r="X34" s="13"/>
       <c r="Z34" s="34"/>
       <c r="AA34" s="34"/>
@@ -3472,32 +3795,32 @@
       <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="71" t="s">
+      <c r="A35" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="72" t="s">
+      <c r="B35" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="74"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="103"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="103"/>
+      <c r="H35" s="103"/>
+      <c r="I35" s="103"/>
+      <c r="J35" s="103"/>
+      <c r="K35" s="104"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="65"/>
-      <c r="Q35" s="66"/>
-      <c r="R35" s="66"/>
-      <c r="S35" s="66"/>
-      <c r="T35" s="66"/>
-      <c r="U35" s="66"/>
-      <c r="V35" s="66"/>
-      <c r="W35" s="67"/>
+      <c r="P35" s="131"/>
+      <c r="Q35" s="132"/>
+      <c r="R35" s="132"/>
+      <c r="S35" s="132"/>
+      <c r="T35" s="132"/>
+      <c r="U35" s="132"/>
+      <c r="V35" s="132"/>
+      <c r="W35" s="133"/>
       <c r="X35" s="13"/>
       <c r="Z35" s="34"/>
       <c r="AA35" s="34"/>
@@ -3512,28 +3835,28 @@
       <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="71"/>
-      <c r="B36" s="75"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="76"/>
-      <c r="K36" s="77"/>
+      <c r="A36" s="101"/>
+      <c r="B36" s="105"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="106"/>
+      <c r="G36" s="106"/>
+      <c r="H36" s="106"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="106"/>
+      <c r="K36" s="107"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="65"/>
-      <c r="Q36" s="66"/>
-      <c r="R36" s="66"/>
-      <c r="S36" s="66"/>
-      <c r="T36" s="66"/>
-      <c r="U36" s="66"/>
-      <c r="V36" s="66"/>
-      <c r="W36" s="67"/>
+      <c r="P36" s="131"/>
+      <c r="Q36" s="132"/>
+      <c r="R36" s="132"/>
+      <c r="S36" s="132"/>
+      <c r="T36" s="132"/>
+      <c r="U36" s="132"/>
+      <c r="V36" s="132"/>
+      <c r="W36" s="133"/>
       <c r="X36" s="13"/>
       <c r="Z36" s="34"/>
       <c r="AA36" s="34"/>
@@ -3548,46 +3871,46 @@
       <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="71"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="80"/>
+      <c r="A37" s="101"/>
+      <c r="B37" s="108"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="109"/>
+      <c r="E37" s="109"/>
+      <c r="F37" s="109"/>
+      <c r="G37" s="109"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="109"/>
+      <c r="J37" s="109"/>
+      <c r="K37" s="110"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="68"/>
-      <c r="Q37" s="69"/>
-      <c r="R37" s="69"/>
-      <c r="S37" s="69"/>
-      <c r="T37" s="69"/>
-      <c r="U37" s="69"/>
-      <c r="V37" s="69"/>
-      <c r="W37" s="70"/>
+      <c r="P37" s="134"/>
+      <c r="Q37" s="135"/>
+      <c r="R37" s="135"/>
+      <c r="S37" s="135"/>
+      <c r="T37" s="135"/>
+      <c r="U37" s="135"/>
+      <c r="V37" s="135"/>
+      <c r="W37" s="136"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
-      <c r="K38" s="47"/>
+      <c r="C38" s="119"/>
+      <c r="D38" s="119"/>
+      <c r="E38" s="119"/>
+      <c r="F38" s="119"/>
+      <c r="G38" s="119"/>
+      <c r="H38" s="119"/>
+      <c r="I38" s="119"/>
+      <c r="J38" s="119"/>
+      <c r="K38" s="120"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3605,36 +3928,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="46"/>
-      <c r="K39" s="47"/>
+      <c r="C39" s="119"/>
+      <c r="D39" s="119"/>
+      <c r="E39" s="119"/>
+      <c r="F39" s="119"/>
+      <c r="G39" s="119"/>
+      <c r="H39" s="119"/>
+      <c r="I39" s="119"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="120"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
-      <c r="K40" s="47"/>
+      <c r="C40" s="119"/>
+      <c r="D40" s="119"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="119"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="119"/>
+      <c r="J40" s="119"/>
+      <c r="K40" s="120"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -3653,76 +3976,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="47"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="119"/>
+      <c r="F41" s="119"/>
+      <c r="G41" s="119"/>
+      <c r="H41" s="119"/>
+      <c r="I41" s="119"/>
+      <c r="J41" s="119"/>
+      <c r="K41" s="120"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="48" t="s">
+      <c r="M41" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="49"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
-      <c r="S41" s="49"/>
-      <c r="T41" s="49"/>
-      <c r="U41" s="49"/>
-      <c r="V41" s="49"/>
-      <c r="W41" s="49"/>
-      <c r="X41" s="50"/>
+      <c r="N41" s="84"/>
+      <c r="O41" s="84"/>
+      <c r="P41" s="84"/>
+      <c r="Q41" s="84"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="84"/>
+      <c r="T41" s="84"/>
+      <c r="U41" s="84"/>
+      <c r="V41" s="84"/>
+      <c r="W41" s="84"/>
+      <c r="X41" s="85"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="47"/>
+      <c r="B42" s="118"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="119"/>
+      <c r="E42" s="119"/>
+      <c r="F42" s="119"/>
+      <c r="G42" s="119"/>
+      <c r="H42" s="119"/>
+      <c r="I42" s="119"/>
+      <c r="J42" s="119"/>
+      <c r="K42" s="120"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="48" t="s">
+      <c r="M42" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="49"/>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="49"/>
-      <c r="S42" s="49"/>
-      <c r="T42" s="49"/>
-      <c r="U42" s="49"/>
-      <c r="V42" s="49"/>
-      <c r="W42" s="49"/>
-      <c r="X42" s="50"/>
+      <c r="N42" s="84"/>
+      <c r="O42" s="84"/>
+      <c r="P42" s="84"/>
+      <c r="Q42" s="84"/>
+      <c r="R42" s="84"/>
+      <c r="S42" s="84"/>
+      <c r="T42" s="84"/>
+      <c r="U42" s="84"/>
+      <c r="V42" s="84"/>
+      <c r="W42" s="84"/>
+      <c r="X42" s="85"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46"/>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
-      <c r="K43" s="47"/>
+      <c r="B43" s="118"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="119"/>
+      <c r="E43" s="119"/>
+      <c r="F43" s="119"/>
+      <c r="G43" s="119"/>
+      <c r="H43" s="119"/>
+      <c r="I43" s="119"/>
+      <c r="J43" s="119"/>
+      <c r="K43" s="120"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -3740,16 +4063,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="47"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="119"/>
+      <c r="E44" s="119"/>
+      <c r="F44" s="119"/>
+      <c r="G44" s="119"/>
+      <c r="H44" s="119"/>
+      <c r="I44" s="119"/>
+      <c r="J44" s="119"/>
+      <c r="K44" s="120"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -3767,16 +4090,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="47"/>
+      <c r="B45" s="118"/>
+      <c r="C45" s="119"/>
+      <c r="D45" s="119"/>
+      <c r="E45" s="119"/>
+      <c r="F45" s="119"/>
+      <c r="G45" s="119"/>
+      <c r="H45" s="119"/>
+      <c r="I45" s="119"/>
+      <c r="J45" s="119"/>
+      <c r="K45" s="120"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -3794,16 +4117,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="47"/>
+      <c r="B46" s="118"/>
+      <c r="C46" s="119"/>
+      <c r="D46" s="119"/>
+      <c r="E46" s="119"/>
+      <c r="F46" s="119"/>
+      <c r="G46" s="119"/>
+      <c r="H46" s="119"/>
+      <c r="I46" s="119"/>
+      <c r="J46" s="119"/>
+      <c r="K46" s="120"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -3846,11 +4169,34 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="J9:R10"/>
+    <mergeCell ref="M42:X42"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="Q26:X27"/>
+    <mergeCell ref="Q29:X29"/>
+    <mergeCell ref="A31:J32"/>
+    <mergeCell ref="P31:W37"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:K37"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="M41:X41"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="B34:K34"/>
     <mergeCell ref="B17:C18"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="L18:M19"/>
@@ -3860,38 +4206,269 @@
     <mergeCell ref="L20:M21"/>
     <mergeCell ref="Q20:X20"/>
     <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="M41:X41"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:K37"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Y1:Z3"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="M42:X42"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="Q26:X27"/>
-    <mergeCell ref="Q29:X29"/>
-    <mergeCell ref="A31:J32"/>
-    <mergeCell ref="P31:W37"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="146.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="139" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="137" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="140" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="139" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="144" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="140" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="140" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="139" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="141" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="138" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="141" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="145" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="141" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="141" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="142" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="140" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="137" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="140" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="138" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="141" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="143" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="148" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="148" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="149" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="146" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="146" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="146" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="147" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
trying stops ships falling over no concavities in terrain etc
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="136">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -276,9 +276,6 @@
     <t>lights need to turn off during day</t>
   </si>
   <si>
-    <t>cannon ball needs to be parented to spawning transform</t>
-  </si>
-  <si>
     <t>tactical cam off bow sides</t>
   </si>
   <si>
@@ -336,27 +333,18 @@
     <t>check max bar working properly saught text</t>
   </si>
   <si>
-    <t>put arduino code into the pedal pirates file</t>
-  </si>
-  <si>
     <t>read through notes made so far in notes document</t>
   </si>
   <si>
     <t>angle change of boat or spray as turn or lean so feel the turn</t>
   </si>
   <si>
-    <t>laptop version for Wednesday and optomise</t>
-  </si>
-  <si>
     <t>check why returns true for wrong baudrate on arduino</t>
   </si>
   <si>
     <t>error handler spelling changed with anduino version and uncomment in arduino code - is this why getting odd results at times</t>
   </si>
   <si>
-    <t>do ai bump?</t>
-  </si>
-  <si>
     <t>playerscript for ai make ai as similar to player as possible to make more options easier to code so ai has as much shared functionality as possible</t>
   </si>
   <si>
@@ -403,6 +391,63 @@
   </si>
   <si>
     <t>individual win screns in middle screen countdown to next game</t>
+  </si>
+  <si>
+    <t>laptop version to pc</t>
+  </si>
+  <si>
+    <t>put arduino code into the pedal pirates file - update with new library</t>
+  </si>
+  <si>
+    <t>auto find comms preset baud</t>
+  </si>
+  <si>
+    <t>improve code to arduino so if open then close, then reopen on the open option as with crashes etc stays open we reopen and cause error</t>
+  </si>
+  <si>
+    <t>research how to run faster over xmas and tweak on laptop for play</t>
+  </si>
+  <si>
+    <t>canon ball smoke impact explosion etc</t>
+  </si>
+  <si>
+    <t>cannon ball needs to be parented to spawning transform, cannon larger, colour of team, low firate damage, lower health, visible (maybe do particle effects same time)</t>
+  </si>
+  <si>
+    <t>experiment and read about camera views</t>
+  </si>
+  <si>
+    <t>have playerSetup mode - which is current game mode with selectors for ai behaviour etc, then have noSetup mode which games on maybe specific maps where just pedal to start new game teams preset, have constant play mode with constant spawning and player respawning</t>
+  </si>
+  <si>
+    <t>its actually really hard to hit so maybe boat damage, sail damage and bow damage will need new strategy for chosing between colliders, cube colliders for each sail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add text 60x for bow damage 4x for hull damage 1x for sail damage and you can fire - if all cannons hit hull that 20 damage or sails 5 </t>
+  </si>
+  <si>
+    <t>addindicator strip for ideal damage</t>
+  </si>
+  <si>
+    <t>teraain thickness and bounce</t>
+  </si>
+  <si>
+    <t>on die get rid all colliders inc new box ones</t>
+  </si>
+  <si>
+    <t>put coloured pannels below toggles for stting the bikes</t>
+  </si>
+  <si>
+    <t>check skinned renders not receiving shadows for lite version</t>
+  </si>
+  <si>
+    <t>new terrain</t>
+  </si>
+  <si>
+    <t>check if boats falling over! YEP! When run aground fixed?</t>
+  </si>
+  <si>
+    <t>make power bars visible and large and less transparent - was working check</t>
   </si>
 </sst>
 </file>
@@ -560,7 +605,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -688,6 +733,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="56">
     <border>
@@ -1366,7 +1423,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1481,300 +1538,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
@@ -1789,6 +1552,303 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -2759,14 +2819,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="Y1" s="112" t="s">
+      <c r="Y1" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="113"/>
+      <c r="Z1" s="91"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="Y2" s="114"/>
-      <c r="Z2" s="115"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="93"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
       <c r="AH2" s="35"/>
@@ -2775,8 +2835,8 @@
       <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="Y3" s="116"/>
-      <c r="Z3" s="117"/>
+      <c r="Y3" s="94"/>
+      <c r="Z3" s="95"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="38" t="s">
         <v>58</v>
@@ -2794,16 +2854,16 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41"/>
-      <c r="G4" s="39" t="s">
+      <c r="C4" s="122"/>
+      <c r="D4" s="123"/>
+      <c r="G4" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="123"/>
       <c r="Z4" s="34"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
@@ -2817,12 +2877,12 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="42"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="131"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="131"/>
       <c r="Z5" s="34" t="s">
         <v>50</v>
       </c>
@@ -2864,12 +2924,12 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="47"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="145"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -2899,10 +2959,10 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="148"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2939,17 +2999,17 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="41"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="122"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="122"/>
+      <c r="O9" s="122"/>
+      <c r="P9" s="122"/>
+      <c r="Q9" s="122"/>
+      <c r="R9" s="123"/>
       <c r="Z9" s="34" t="s">
         <v>69</v>
       </c>
@@ -2977,25 +3037,25 @@
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="149"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="44"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="142"/>
+      <c r="Q10" s="142"/>
+      <c r="R10" s="131"/>
       <c r="Z10" s="34">
         <v>20</v>
       </c>
@@ -3027,10 +3087,10 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="86" t="s">
+      <c r="G11" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="87"/>
+      <c r="H11" s="106"/>
       <c r="I11" s="28"/>
       <c r="Z11" s="34">
         <v>5</v>
@@ -3066,16 +3126,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="52" t="s">
+      <c r="L12" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="88"/>
+      <c r="M12" s="108"/>
+      <c r="N12" s="108"/>
+      <c r="O12" s="108"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="109"/>
       <c r="Z12" s="34"/>
       <c r="AA12" s="34"/>
       <c r="AB12" s="34"/>
@@ -3098,14 +3158,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="89"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="111"/>
+      <c r="S13" s="112"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -3149,16 +3209,16 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="90" t="s">
+      <c r="Q15" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="91"/>
-      <c r="S15" s="91"/>
-      <c r="T15" s="91"/>
-      <c r="U15" s="91"/>
-      <c r="V15" s="91"/>
-      <c r="W15" s="91"/>
-      <c r="X15" s="92"/>
+      <c r="R15" s="114"/>
+      <c r="S15" s="114"/>
+      <c r="T15" s="114"/>
+      <c r="U15" s="114"/>
+      <c r="V15" s="114"/>
+      <c r="W15" s="114"/>
+      <c r="X15" s="115"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -3176,19 +3236,19 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="40" t="s">
+      <c r="M16" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="40"/>
-      <c r="O16" s="41"/>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="94"/>
-      <c r="S16" s="94"/>
-      <c r="T16" s="94"/>
-      <c r="U16" s="94"/>
-      <c r="V16" s="94"/>
-      <c r="W16" s="94"/>
-      <c r="X16" s="95"/>
+      <c r="N16" s="122"/>
+      <c r="O16" s="123"/>
+      <c r="Q16" s="116"/>
+      <c r="R16" s="117"/>
+      <c r="S16" s="117"/>
+      <c r="T16" s="117"/>
+      <c r="U16" s="117"/>
+      <c r="V16" s="117"/>
+      <c r="W16" s="117"/>
+      <c r="X16" s="118"/>
       <c r="Z16" s="34"/>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
@@ -3202,31 +3262,31 @@
       <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="53"/>
+      <c r="C17" s="108"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="128"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="99"/>
-      <c r="N17" s="99"/>
-      <c r="O17" s="100"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="97"/>
-      <c r="S17" s="97"/>
-      <c r="T17" s="97"/>
-      <c r="U17" s="97"/>
-      <c r="V17" s="97"/>
-      <c r="W17" s="97"/>
-      <c r="X17" s="98"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="124"/>
+      <c r="O17" s="125"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="120"/>
+      <c r="S17" s="120"/>
+      <c r="T17" s="120"/>
+      <c r="U17" s="120"/>
+      <c r="V17" s="120"/>
+      <c r="W17" s="120"/>
+      <c r="X17" s="121"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -3240,18 +3300,18 @@
       <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="111"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="59" t="s">
+      <c r="L18" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="60"/>
+      <c r="M18" s="89"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3276,32 +3336,32 @@
       <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="41"/>
+      <c r="C19" s="123"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="60"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="89"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="61" t="s">
+      <c r="Q19" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="62"/>
-      <c r="S19" s="62"/>
-      <c r="T19" s="62"/>
-      <c r="U19" s="62"/>
-      <c r="V19" s="62"/>
-      <c r="W19" s="62"/>
-      <c r="X19" s="63"/>
+      <c r="R19" s="133"/>
+      <c r="S19" s="133"/>
+      <c r="T19" s="133"/>
+      <c r="U19" s="133"/>
+      <c r="V19" s="133"/>
+      <c r="W19" s="133"/>
+      <c r="X19" s="134"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -3315,32 +3375,32 @@
       <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="42"/>
-      <c r="C20" s="44"/>
-      <c r="F20" s="64" t="s">
+      <c r="B20" s="130"/>
+      <c r="C20" s="131"/>
+      <c r="F20" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="65"/>
+      <c r="G20" s="136"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="59" t="s">
+      <c r="L20" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="60"/>
+      <c r="M20" s="89"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="68" t="s">
+      <c r="Q20" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="69"/>
-      <c r="S20" s="69"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="69"/>
-      <c r="W20" s="69"/>
-      <c r="X20" s="70"/>
+      <c r="R20" s="56"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="56"/>
+      <c r="U20" s="56"/>
+      <c r="V20" s="56"/>
+      <c r="W20" s="56"/>
+      <c r="X20" s="64"/>
       <c r="Z20" s="34"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
@@ -3357,28 +3417,28 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="67"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="138"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="60"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="89"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="71" t="s">
+      <c r="Q21" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="72"/>
-      <c r="S21" s="72"/>
-      <c r="T21" s="72"/>
-      <c r="U21" s="72"/>
-      <c r="V21" s="72"/>
-      <c r="W21" s="72"/>
-      <c r="X21" s="73"/>
+      <c r="R21" s="140"/>
+      <c r="S21" s="140"/>
+      <c r="T21" s="140"/>
+      <c r="U21" s="140"/>
+      <c r="V21" s="140"/>
+      <c r="W21" s="140"/>
+      <c r="X21" s="141"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -3396,10 +3456,10 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="59" t="s">
+      <c r="L22" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="60"/>
+      <c r="M22" s="89"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -3419,28 +3479,28 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="68" t="s">
+      <c r="E23" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="69"/>
-      <c r="G23" s="111"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="57"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="60"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="89"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="74" t="s">
+      <c r="Q23" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="75"/>
-      <c r="S23" s="75"/>
-      <c r="T23" s="75"/>
-      <c r="U23" s="75"/>
-      <c r="V23" s="75"/>
-      <c r="W23" s="75"/>
-      <c r="X23" s="76"/>
+      <c r="R23" s="97"/>
+      <c r="S23" s="97"/>
+      <c r="T23" s="97"/>
+      <c r="U23" s="97"/>
+      <c r="V23" s="97"/>
+      <c r="W23" s="97"/>
+      <c r="X23" s="98"/>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
@@ -3458,20 +3518,20 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="59" t="s">
+      <c r="L24" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="60"/>
+      <c r="M24" s="89"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="77"/>
-      <c r="R24" s="78"/>
-      <c r="S24" s="78"/>
-      <c r="T24" s="78"/>
-      <c r="U24" s="78"/>
-      <c r="V24" s="78"/>
-      <c r="W24" s="78"/>
-      <c r="X24" s="79"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
+      <c r="S24" s="100"/>
+      <c r="T24" s="100"/>
+      <c r="U24" s="100"/>
+      <c r="V24" s="100"/>
+      <c r="W24" s="100"/>
+      <c r="X24" s="101"/>
       <c r="Z24" s="34"/>
       <c r="AA24" s="34"/>
       <c r="AB24" s="34"/>
@@ -3489,18 +3549,18 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="60"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="89"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="80"/>
-      <c r="R25" s="81"/>
-      <c r="S25" s="81"/>
-      <c r="T25" s="81"/>
-      <c r="U25" s="81"/>
-      <c r="V25" s="81"/>
-      <c r="W25" s="81"/>
-      <c r="X25" s="82"/>
+      <c r="Q25" s="102"/>
+      <c r="R25" s="103"/>
+      <c r="S25" s="103"/>
+      <c r="T25" s="103"/>
+      <c r="U25" s="103"/>
+      <c r="V25" s="103"/>
+      <c r="W25" s="103"/>
+      <c r="X25" s="104"/>
       <c r="Z25" s="34"/>
       <c r="AA25" s="34"/>
       <c r="AB25" s="34"/>
@@ -3517,26 +3577,26 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="111"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="57"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="121" t="s">
+      <c r="Q26" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="122"/>
-      <c r="S26" s="122"/>
-      <c r="T26" s="122"/>
-      <c r="U26" s="122"/>
-      <c r="V26" s="122"/>
-      <c r="W26" s="122"/>
-      <c r="X26" s="123"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="60"/>
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
       <c r="AB26" s="34"/>
@@ -3552,14 +3612,14 @@
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="124"/>
-      <c r="R27" s="125"/>
-      <c r="S27" s="125"/>
-      <c r="T27" s="125"/>
-      <c r="U27" s="125"/>
-      <c r="V27" s="125"/>
-      <c r="W27" s="125"/>
-      <c r="X27" s="126"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="63"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -3593,16 +3653,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="68" t="s">
+      <c r="Q29" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="69"/>
-      <c r="S29" s="69"/>
-      <c r="T29" s="69"/>
-      <c r="U29" s="69"/>
-      <c r="V29" s="69"/>
-      <c r="W29" s="69"/>
-      <c r="X29" s="70"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
+      <c r="X29" s="64"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -3643,32 +3703,32 @@
       <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="127" t="s">
+      <c r="A31" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="127"/>
-      <c r="C31" s="127"/>
-      <c r="D31" s="127"/>
-      <c r="E31" s="127"/>
-      <c r="F31" s="127"/>
-      <c r="G31" s="127"/>
-      <c r="H31" s="127"/>
-      <c r="I31" s="127"/>
-      <c r="J31" s="127"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="128" t="s">
+      <c r="P31" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="129"/>
-      <c r="R31" s="129"/>
-      <c r="S31" s="129"/>
-      <c r="T31" s="129"/>
-      <c r="U31" s="129"/>
-      <c r="V31" s="129"/>
-      <c r="W31" s="130"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="67"/>
+      <c r="T31" s="67"/>
+      <c r="U31" s="67"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="68"/>
       <c r="X31" s="13"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
@@ -3683,28 +3743,28 @@
       <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="127"/>
-      <c r="B32" s="127"/>
-      <c r="C32" s="127"/>
-      <c r="D32" s="127"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="127"/>
-      <c r="G32" s="127"/>
-      <c r="H32" s="127"/>
-      <c r="I32" s="127"/>
-      <c r="J32" s="127"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="131"/>
-      <c r="Q32" s="132"/>
-      <c r="R32" s="132"/>
-      <c r="S32" s="132"/>
-      <c r="T32" s="132"/>
-      <c r="U32" s="132"/>
-      <c r="V32" s="132"/>
-      <c r="W32" s="133"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="70"/>
+      <c r="R32" s="70"/>
+      <c r="S32" s="70"/>
+      <c r="T32" s="70"/>
+      <c r="U32" s="70"/>
+      <c r="V32" s="70"/>
+      <c r="W32" s="71"/>
       <c r="X32" s="13"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
@@ -3733,14 +3793,14 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="131"/>
-      <c r="Q33" s="132"/>
-      <c r="R33" s="132"/>
-      <c r="S33" s="132"/>
-      <c r="T33" s="132"/>
-      <c r="U33" s="132"/>
-      <c r="V33" s="132"/>
-      <c r="W33" s="133"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="70"/>
+      <c r="R33" s="70"/>
+      <c r="S33" s="70"/>
+      <c r="T33" s="70"/>
+      <c r="U33" s="70"/>
+      <c r="V33" s="70"/>
+      <c r="W33" s="71"/>
       <c r="X33" s="13"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="34"/>
@@ -3758,29 +3818,29 @@
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="101" t="s">
+      <c r="B34" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="101"/>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
-      <c r="H34" s="101"/>
-      <c r="I34" s="101"/>
-      <c r="J34" s="101"/>
-      <c r="K34" s="101"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="78"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="131"/>
-      <c r="Q34" s="132"/>
-      <c r="R34" s="132"/>
-      <c r="S34" s="132"/>
-      <c r="T34" s="132"/>
-      <c r="U34" s="132"/>
-      <c r="V34" s="132"/>
-      <c r="W34" s="133"/>
+      <c r="P34" s="69"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="70"/>
+      <c r="W34" s="71"/>
       <c r="X34" s="13"/>
       <c r="Z34" s="34"/>
       <c r="AA34" s="34"/>
@@ -3795,32 +3855,32 @@
       <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="101" t="s">
+      <c r="A35" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="102" t="s">
+      <c r="B35" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="103"/>
-      <c r="D35" s="103"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="103"/>
-      <c r="H35" s="103"/>
-      <c r="I35" s="103"/>
-      <c r="J35" s="103"/>
-      <c r="K35" s="104"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="81"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="131"/>
-      <c r="Q35" s="132"/>
-      <c r="R35" s="132"/>
-      <c r="S35" s="132"/>
-      <c r="T35" s="132"/>
-      <c r="U35" s="132"/>
-      <c r="V35" s="132"/>
-      <c r="W35" s="133"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="70"/>
+      <c r="R35" s="70"/>
+      <c r="S35" s="70"/>
+      <c r="T35" s="70"/>
+      <c r="U35" s="70"/>
+      <c r="V35" s="70"/>
+      <c r="W35" s="71"/>
       <c r="X35" s="13"/>
       <c r="Z35" s="34"/>
       <c r="AA35" s="34"/>
@@ -3835,28 +3895,28 @@
       <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="101"/>
-      <c r="B36" s="105"/>
-      <c r="C36" s="106"/>
-      <c r="D36" s="106"/>
-      <c r="E36" s="106"/>
-      <c r="F36" s="106"/>
-      <c r="G36" s="106"/>
-      <c r="H36" s="106"/>
-      <c r="I36" s="106"/>
-      <c r="J36" s="106"/>
-      <c r="K36" s="107"/>
+      <c r="A36" s="78"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="83"/>
+      <c r="J36" s="83"/>
+      <c r="K36" s="84"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="131"/>
-      <c r="Q36" s="132"/>
-      <c r="R36" s="132"/>
-      <c r="S36" s="132"/>
-      <c r="T36" s="132"/>
-      <c r="U36" s="132"/>
-      <c r="V36" s="132"/>
-      <c r="W36" s="133"/>
+      <c r="P36" s="69"/>
+      <c r="Q36" s="70"/>
+      <c r="R36" s="70"/>
+      <c r="S36" s="70"/>
+      <c r="T36" s="70"/>
+      <c r="U36" s="70"/>
+      <c r="V36" s="70"/>
+      <c r="W36" s="71"/>
       <c r="X36" s="13"/>
       <c r="Z36" s="34"/>
       <c r="AA36" s="34"/>
@@ -3871,46 +3931,46 @@
       <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="101"/>
-      <c r="B37" s="108"/>
-      <c r="C37" s="109"/>
-      <c r="D37" s="109"/>
-      <c r="E37" s="109"/>
-      <c r="F37" s="109"/>
-      <c r="G37" s="109"/>
-      <c r="H37" s="109"/>
-      <c r="I37" s="109"/>
-      <c r="J37" s="109"/>
-      <c r="K37" s="110"/>
+      <c r="A37" s="78"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
+      <c r="H37" s="86"/>
+      <c r="I37" s="86"/>
+      <c r="J37" s="86"/>
+      <c r="K37" s="87"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="134"/>
-      <c r="Q37" s="135"/>
-      <c r="R37" s="135"/>
-      <c r="S37" s="135"/>
-      <c r="T37" s="135"/>
-      <c r="U37" s="135"/>
-      <c r="V37" s="135"/>
-      <c r="W37" s="136"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="73"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="73"/>
+      <c r="V37" s="73"/>
+      <c r="W37" s="74"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="118" t="s">
+      <c r="B38" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="119"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="119"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="119"/>
-      <c r="H38" s="119"/>
-      <c r="I38" s="119"/>
-      <c r="J38" s="119"/>
-      <c r="K38" s="120"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="76"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="77"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3928,36 +3988,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="118" t="s">
+      <c r="B39" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="119"/>
-      <c r="D39" s="119"/>
-      <c r="E39" s="119"/>
-      <c r="F39" s="119"/>
-      <c r="G39" s="119"/>
-      <c r="H39" s="119"/>
-      <c r="I39" s="119"/>
-      <c r="J39" s="119"/>
-      <c r="K39" s="120"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="77"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="118" t="s">
+      <c r="B40" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="119"/>
-      <c r="D40" s="119"/>
-      <c r="E40" s="119"/>
-      <c r="F40" s="119"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="119"/>
-      <c r="I40" s="119"/>
-      <c r="J40" s="119"/>
-      <c r="K40" s="120"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="76"/>
+      <c r="I40" s="76"/>
+      <c r="J40" s="76"/>
+      <c r="K40" s="77"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -3976,76 +4036,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="118" t="s">
+      <c r="B41" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="119"/>
-      <c r="D41" s="119"/>
-      <c r="E41" s="119"/>
-      <c r="F41" s="119"/>
-      <c r="G41" s="119"/>
-      <c r="H41" s="119"/>
-      <c r="I41" s="119"/>
-      <c r="J41" s="119"/>
-      <c r="K41" s="120"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="77"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="83" t="s">
+      <c r="M41" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="84"/>
-      <c r="O41" s="84"/>
-      <c r="P41" s="84"/>
-      <c r="Q41" s="84"/>
-      <c r="R41" s="84"/>
-      <c r="S41" s="84"/>
-      <c r="T41" s="84"/>
-      <c r="U41" s="84"/>
-      <c r="V41" s="84"/>
-      <c r="W41" s="84"/>
-      <c r="X41" s="85"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="54"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="118"/>
-      <c r="C42" s="119"/>
-      <c r="D42" s="119"/>
-      <c r="E42" s="119"/>
-      <c r="F42" s="119"/>
-      <c r="G42" s="119"/>
-      <c r="H42" s="119"/>
-      <c r="I42" s="119"/>
-      <c r="J42" s="119"/>
-      <c r="K42" s="120"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="77"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="83" t="s">
+      <c r="M42" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="84"/>
-      <c r="O42" s="84"/>
-      <c r="P42" s="84"/>
-      <c r="Q42" s="84"/>
-      <c r="R42" s="84"/>
-      <c r="S42" s="84"/>
-      <c r="T42" s="84"/>
-      <c r="U42" s="84"/>
-      <c r="V42" s="84"/>
-      <c r="W42" s="84"/>
-      <c r="X42" s="85"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="53"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="54"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="118"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="119"/>
-      <c r="F43" s="119"/>
-      <c r="G43" s="119"/>
-      <c r="H43" s="119"/>
-      <c r="I43" s="119"/>
-      <c r="J43" s="119"/>
-      <c r="K43" s="120"/>
+      <c r="B43" s="75"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+      <c r="J43" s="76"/>
+      <c r="K43" s="77"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -4063,16 +4123,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="118"/>
-      <c r="C44" s="119"/>
-      <c r="D44" s="119"/>
-      <c r="E44" s="119"/>
-      <c r="F44" s="119"/>
-      <c r="G44" s="119"/>
-      <c r="H44" s="119"/>
-      <c r="I44" s="119"/>
-      <c r="J44" s="119"/>
-      <c r="K44" s="120"/>
+      <c r="B44" s="75"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="77"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -4090,16 +4150,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="118"/>
-      <c r="C45" s="119"/>
-      <c r="D45" s="119"/>
-      <c r="E45" s="119"/>
-      <c r="F45" s="119"/>
-      <c r="G45" s="119"/>
-      <c r="H45" s="119"/>
-      <c r="I45" s="119"/>
-      <c r="J45" s="119"/>
-      <c r="K45" s="120"/>
+      <c r="B45" s="75"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="77"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -4117,16 +4177,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="118"/>
-      <c r="C46" s="119"/>
-      <c r="D46" s="119"/>
-      <c r="E46" s="119"/>
-      <c r="F46" s="119"/>
-      <c r="G46" s="119"/>
-      <c r="H46" s="119"/>
-      <c r="I46" s="119"/>
-      <c r="J46" s="119"/>
-      <c r="K46" s="120"/>
+      <c r="B46" s="75"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="76"/>
+      <c r="I46" s="76"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="77"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -4169,12 +4229,29 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="M42:X42"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="Q26:X27"/>
-    <mergeCell ref="Q29:X29"/>
-    <mergeCell ref="A31:J32"/>
-    <mergeCell ref="P31:W37"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:R10"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="Q19:X19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
     <mergeCell ref="B43:K43"/>
     <mergeCell ref="B44:K44"/>
     <mergeCell ref="B45:K45"/>
@@ -4184,33 +4261,16 @@
     <mergeCell ref="B40:K40"/>
     <mergeCell ref="B41:K41"/>
     <mergeCell ref="B42:K42"/>
+    <mergeCell ref="M42:X42"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="Q26:X27"/>
+    <mergeCell ref="Q29:X29"/>
+    <mergeCell ref="A31:J32"/>
+    <mergeCell ref="P31:W37"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:K37"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Y1:Z3"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
     <mergeCell ref="M41:X41"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
     <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="Q19:X19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="J9:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4221,10 +4281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A47"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4234,16 +4294,16 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="41" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="39" t="s">
         <v>75</v>
       </c>
     </row>
@@ -4253,218 +4313,293 @@
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="140" t="s">
+      <c r="A5" s="42" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="139" t="s">
+      <c r="A6" s="151" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="46" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="144" t="s">
-        <v>79</v>
-      </c>
-    </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="140" t="s">
-        <v>81</v>
+      <c r="A8" s="42" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="42" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="140" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="41" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="139" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="141" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" s="40" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="138" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="43" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="141" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="47" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="145" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="43" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="141" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="43" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="141" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" s="44" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="142" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" s="42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="140" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" s="39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="42" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="137" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="140" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="138" t="s">
-        <v>101</v>
+      <c r="A28" s="40" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="141" t="s">
-        <v>102</v>
+      <c r="A29" s="43" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="143" t="s">
-        <v>114</v>
+      <c r="A33" s="45" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="148" t="s">
-        <v>106</v>
+      <c r="A34" s="50" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="148" t="s">
-        <v>107</v>
+      <c r="A35" s="50" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="149" t="s">
-        <v>109</v>
+      <c r="A37" s="51" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="146" t="s">
-        <v>111</v>
+      <c r="A39" s="48" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="146" t="s">
-        <v>116</v>
+      <c r="A43" s="48" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="146" t="s">
-        <v>118</v>
+      <c r="A45" s="48" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="50" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="147" t="s">
+    <row r="49" spans="1:1">
+      <c r="A49" s="40" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="150" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="152" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="44" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert to a different naff terrain will do all the terrain renders and things when only got a day or two left and the interface slickness can wait as i will do that the game play is the focus for a few days
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -327,9 +327,6 @@
     <t>daycycle starts at game start</t>
   </si>
   <si>
-    <t>check count ships</t>
-  </si>
-  <si>
     <t>check max bar working properly saught text</t>
   </si>
   <si>
@@ -441,13 +438,19 @@
     <t>check skinned renders not receiving shadows for lite version</t>
   </si>
   <si>
-    <t>new terrain</t>
-  </si>
-  <si>
     <t>check if boats falling over! YEP! When run aground fixed?</t>
   </si>
   <si>
-    <t>make power bars visible and large and less transparent - was working check</t>
+    <t>new terrain when do on laptop, no light details etc small get rid all files dont us make it light, try turning off scripts to see what slows it</t>
+  </si>
+  <si>
+    <t>gizmo jumps</t>
+  </si>
+  <si>
+    <t>ai need health and cannon scripts disabling on death</t>
+  </si>
+  <si>
+    <t>cannons not stopping firing as count things inand out change to just when triggered with cool down</t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -705,12 +708,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1423,7 +1420,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1552,6 +1549,215 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1559,15 +1765,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1588,9 +1785,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1621,15 +1815,6 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1660,195 +1845,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -2854,16 +2850,16 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="122"/>
-      <c r="D4" s="123"/>
-      <c r="G4" s="129" t="s">
+      <c r="C4" s="55"/>
+      <c r="D4" s="56"/>
+      <c r="G4" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="122"/>
-      <c r="I4" s="123"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="56"/>
       <c r="Z4" s="34"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
@@ -2877,12 +2873,12 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="130"/>
-      <c r="C5" s="142"/>
-      <c r="D5" s="131"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="142"/>
-      <c r="I5" s="131"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="59"/>
       <c r="Z5" s="34" t="s">
         <v>50</v>
       </c>
@@ -2924,12 +2920,12 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="144"/>
-      <c r="D7" s="144"/>
-      <c r="E7" s="145"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="62"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -2959,10 +2955,10 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="146"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
-      <c r="E8" s="148"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2999,17 +2995,17 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="129" t="s">
+      <c r="J9" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="122"/>
-      <c r="L9" s="122"/>
-      <c r="M9" s="122"/>
-      <c r="N9" s="122"/>
-      <c r="O9" s="122"/>
-      <c r="P9" s="122"/>
-      <c r="Q9" s="122"/>
-      <c r="R9" s="123"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="56"/>
       <c r="Z9" s="34" t="s">
         <v>69</v>
       </c>
@@ -3037,25 +3033,25 @@
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="149" t="s">
+      <c r="B10" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="149"/>
-      <c r="D10" s="149"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="142"/>
-      <c r="L10" s="142"/>
-      <c r="M10" s="142"/>
-      <c r="N10" s="142"/>
-      <c r="O10" s="142"/>
-      <c r="P10" s="142"/>
-      <c r="Q10" s="142"/>
-      <c r="R10" s="131"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="59"/>
       <c r="Z10" s="34">
         <v>20</v>
       </c>
@@ -3126,16 +3122,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="107" t="s">
+      <c r="L12" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="108"/>
-      <c r="N12" s="108"/>
-      <c r="O12" s="108"/>
-      <c r="P12" s="108"/>
-      <c r="Q12" s="108"/>
-      <c r="R12" s="108"/>
-      <c r="S12" s="109"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="68"/>
+      <c r="Q12" s="68"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="107"/>
       <c r="Z12" s="34"/>
       <c r="AA12" s="34"/>
       <c r="AB12" s="34"/>
@@ -3158,14 +3154,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="110"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="111"/>
-      <c r="Q13" s="111"/>
-      <c r="R13" s="111"/>
-      <c r="S13" s="112"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="70"/>
+      <c r="P13" s="70"/>
+      <c r="Q13" s="70"/>
+      <c r="R13" s="70"/>
+      <c r="S13" s="108"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -3209,16 +3205,16 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="113" t="s">
+      <c r="Q15" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="114"/>
-      <c r="S15" s="114"/>
-      <c r="T15" s="114"/>
-      <c r="U15" s="114"/>
-      <c r="V15" s="114"/>
-      <c r="W15" s="114"/>
-      <c r="X15" s="115"/>
+      <c r="R15" s="110"/>
+      <c r="S15" s="110"/>
+      <c r="T15" s="110"/>
+      <c r="U15" s="110"/>
+      <c r="V15" s="110"/>
+      <c r="W15" s="110"/>
+      <c r="X15" s="111"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -3236,19 +3232,19 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="122" t="s">
+      <c r="M16" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="122"/>
-      <c r="O16" s="123"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="117"/>
-      <c r="S16" s="117"/>
-      <c r="T16" s="117"/>
-      <c r="U16" s="117"/>
-      <c r="V16" s="117"/>
-      <c r="W16" s="117"/>
-      <c r="X16" s="118"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="56"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="113"/>
+      <c r="S16" s="113"/>
+      <c r="T16" s="113"/>
+      <c r="U16" s="113"/>
+      <c r="V16" s="113"/>
+      <c r="W16" s="113"/>
+      <c r="X16" s="114"/>
       <c r="Z16" s="34"/>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
@@ -3262,31 +3258,31 @@
       <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="108"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="126" t="s">
+      <c r="E17" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="127"/>
-      <c r="G17" s="128"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="73"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="124"/>
-      <c r="N17" s="124"/>
-      <c r="O17" s="125"/>
-      <c r="Q17" s="119"/>
-      <c r="R17" s="120"/>
-      <c r="S17" s="120"/>
-      <c r="T17" s="120"/>
-      <c r="U17" s="120"/>
-      <c r="V17" s="120"/>
-      <c r="W17" s="120"/>
-      <c r="X17" s="121"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="118"/>
+      <c r="O17" s="119"/>
+      <c r="Q17" s="115"/>
+      <c r="R17" s="116"/>
+      <c r="S17" s="116"/>
+      <c r="T17" s="116"/>
+      <c r="U17" s="116"/>
+      <c r="V17" s="116"/>
+      <c r="W17" s="116"/>
+      <c r="X17" s="117"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -3300,18 +3296,18 @@
       <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="110"/>
-      <c r="C18" s="111"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="70"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="88" t="s">
+      <c r="L18" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="89"/>
+      <c r="M18" s="75"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3336,32 +3332,32 @@
       <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="129" t="s">
+      <c r="B19" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="123"/>
+      <c r="C19" s="56"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="89"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="75"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="132" t="s">
+      <c r="Q19" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="133"/>
-      <c r="S19" s="133"/>
-      <c r="T19" s="133"/>
-      <c r="U19" s="133"/>
-      <c r="V19" s="133"/>
-      <c r="W19" s="133"/>
-      <c r="X19" s="134"/>
+      <c r="R19" s="77"/>
+      <c r="S19" s="77"/>
+      <c r="T19" s="77"/>
+      <c r="U19" s="77"/>
+      <c r="V19" s="77"/>
+      <c r="W19" s="77"/>
+      <c r="X19" s="78"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -3375,32 +3371,32 @@
       <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="130"/>
-      <c r="C20" s="131"/>
-      <c r="F20" s="135" t="s">
+      <c r="B20" s="57"/>
+      <c r="C20" s="59"/>
+      <c r="F20" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="136"/>
+      <c r="G20" s="80"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="88" t="s">
+      <c r="L20" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="89"/>
+      <c r="M20" s="75"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="55" t="s">
+      <c r="Q20" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="64"/>
+      <c r="R20" s="84"/>
+      <c r="S20" s="84"/>
+      <c r="T20" s="84"/>
+      <c r="U20" s="84"/>
+      <c r="V20" s="84"/>
+      <c r="W20" s="84"/>
+      <c r="X20" s="85"/>
       <c r="Z20" s="34"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
@@ -3417,28 +3413,28 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="138"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="82"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="89"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="75"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="139" t="s">
+      <c r="Q21" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="140"/>
-      <c r="S21" s="140"/>
-      <c r="T21" s="140"/>
-      <c r="U21" s="140"/>
-      <c r="V21" s="140"/>
-      <c r="W21" s="140"/>
-      <c r="X21" s="141"/>
+      <c r="R21" s="87"/>
+      <c r="S21" s="87"/>
+      <c r="T21" s="87"/>
+      <c r="U21" s="87"/>
+      <c r="V21" s="87"/>
+      <c r="W21" s="87"/>
+      <c r="X21" s="88"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -3456,10 +3452,10 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="88" t="s">
+      <c r="L22" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="89"/>
+      <c r="M22" s="75"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -3479,14 +3475,14 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="57"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="89"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="89"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="75"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
@@ -3518,10 +3514,10 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="88" t="s">
+      <c r="L24" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="89"/>
+      <c r="M24" s="75"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
       <c r="Q24" s="99"/>
@@ -3549,8 +3545,8 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="88"/>
-      <c r="M25" s="89"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="75"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
       <c r="Q25" s="102"/>
@@ -3577,26 +3573,26 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="57"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="84"/>
+      <c r="J26" s="84"/>
+      <c r="K26" s="89"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="58" t="s">
+      <c r="Q26" s="126" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59"/>
-      <c r="T26" s="59"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="59"/>
-      <c r="W26" s="59"/>
-      <c r="X26" s="60"/>
+      <c r="R26" s="127"/>
+      <c r="S26" s="127"/>
+      <c r="T26" s="127"/>
+      <c r="U26" s="127"/>
+      <c r="V26" s="127"/>
+      <c r="W26" s="127"/>
+      <c r="X26" s="128"/>
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
       <c r="AB26" s="34"/>
@@ -3612,14 +3608,14 @@
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="62"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="62"/>
-      <c r="V27" s="62"/>
-      <c r="W27" s="62"/>
-      <c r="X27" s="63"/>
+      <c r="Q27" s="129"/>
+      <c r="R27" s="130"/>
+      <c r="S27" s="130"/>
+      <c r="T27" s="130"/>
+      <c r="U27" s="130"/>
+      <c r="V27" s="130"/>
+      <c r="W27" s="130"/>
+      <c r="X27" s="131"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -3653,16 +3649,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="55" t="s">
+      <c r="Q29" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
-      <c r="X29" s="64"/>
+      <c r="R29" s="84"/>
+      <c r="S29" s="84"/>
+      <c r="T29" s="84"/>
+      <c r="U29" s="84"/>
+      <c r="V29" s="84"/>
+      <c r="W29" s="84"/>
+      <c r="X29" s="85"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -3703,32 +3699,32 @@
       <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
+      <c r="B31" s="132"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="132"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="132"/>
+      <c r="G31" s="132"/>
+      <c r="H31" s="132"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="132"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="66" t="s">
+      <c r="P31" s="133" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="67"/>
-      <c r="S31" s="67"/>
-      <c r="T31" s="67"/>
-      <c r="U31" s="67"/>
-      <c r="V31" s="67"/>
-      <c r="W31" s="68"/>
+      <c r="Q31" s="134"/>
+      <c r="R31" s="134"/>
+      <c r="S31" s="134"/>
+      <c r="T31" s="134"/>
+      <c r="U31" s="134"/>
+      <c r="V31" s="134"/>
+      <c r="W31" s="135"/>
       <c r="X31" s="13"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
@@ -3743,28 +3739,28 @@
       <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="65"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
+      <c r="A32" s="132"/>
+      <c r="B32" s="132"/>
+      <c r="C32" s="132"/>
+      <c r="D32" s="132"/>
+      <c r="E32" s="132"/>
+      <c r="F32" s="132"/>
+      <c r="G32" s="132"/>
+      <c r="H32" s="132"/>
+      <c r="I32" s="132"/>
+      <c r="J32" s="132"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="70"/>
-      <c r="R32" s="70"/>
-      <c r="S32" s="70"/>
-      <c r="T32" s="70"/>
-      <c r="U32" s="70"/>
-      <c r="V32" s="70"/>
-      <c r="W32" s="71"/>
+      <c r="P32" s="136"/>
+      <c r="Q32" s="137"/>
+      <c r="R32" s="137"/>
+      <c r="S32" s="137"/>
+      <c r="T32" s="137"/>
+      <c r="U32" s="137"/>
+      <c r="V32" s="137"/>
+      <c r="W32" s="138"/>
       <c r="X32" s="13"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
@@ -3793,14 +3789,14 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="70"/>
-      <c r="R33" s="70"/>
-      <c r="S33" s="70"/>
-      <c r="T33" s="70"/>
-      <c r="U33" s="70"/>
-      <c r="V33" s="70"/>
-      <c r="W33" s="71"/>
+      <c r="P33" s="136"/>
+      <c r="Q33" s="137"/>
+      <c r="R33" s="137"/>
+      <c r="S33" s="137"/>
+      <c r="T33" s="137"/>
+      <c r="U33" s="137"/>
+      <c r="V33" s="137"/>
+      <c r="W33" s="138"/>
       <c r="X33" s="13"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="34"/>
@@ -3818,29 +3814,29 @@
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
+      <c r="C34" s="142"/>
+      <c r="D34" s="142"/>
+      <c r="E34" s="142"/>
+      <c r="F34" s="142"/>
+      <c r="G34" s="142"/>
+      <c r="H34" s="142"/>
+      <c r="I34" s="142"/>
+      <c r="J34" s="142"/>
+      <c r="K34" s="142"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="70"/>
-      <c r="T34" s="70"/>
-      <c r="U34" s="70"/>
-      <c r="V34" s="70"/>
-      <c r="W34" s="71"/>
+      <c r="P34" s="136"/>
+      <c r="Q34" s="137"/>
+      <c r="R34" s="137"/>
+      <c r="S34" s="137"/>
+      <c r="T34" s="137"/>
+      <c r="U34" s="137"/>
+      <c r="V34" s="137"/>
+      <c r="W34" s="138"/>
       <c r="X34" s="13"/>
       <c r="Z34" s="34"/>
       <c r="AA34" s="34"/>
@@ -3855,32 +3851,32 @@
       <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="142" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="81"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="144"/>
+      <c r="E35" s="144"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="144"/>
+      <c r="H35" s="144"/>
+      <c r="I35" s="144"/>
+      <c r="J35" s="144"/>
+      <c r="K35" s="145"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="70"/>
-      <c r="R35" s="70"/>
-      <c r="S35" s="70"/>
-      <c r="T35" s="70"/>
-      <c r="U35" s="70"/>
-      <c r="V35" s="70"/>
-      <c r="W35" s="71"/>
+      <c r="P35" s="136"/>
+      <c r="Q35" s="137"/>
+      <c r="R35" s="137"/>
+      <c r="S35" s="137"/>
+      <c r="T35" s="137"/>
+      <c r="U35" s="137"/>
+      <c r="V35" s="137"/>
+      <c r="W35" s="138"/>
       <c r="X35" s="13"/>
       <c r="Z35" s="34"/>
       <c r="AA35" s="34"/>
@@ -3895,28 +3891,28 @@
       <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="78"/>
-      <c r="B36" s="82"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="84"/>
+      <c r="A36" s="142"/>
+      <c r="B36" s="146"/>
+      <c r="C36" s="147"/>
+      <c r="D36" s="147"/>
+      <c r="E36" s="147"/>
+      <c r="F36" s="147"/>
+      <c r="G36" s="147"/>
+      <c r="H36" s="147"/>
+      <c r="I36" s="147"/>
+      <c r="J36" s="147"/>
+      <c r="K36" s="148"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="69"/>
-      <c r="Q36" s="70"/>
-      <c r="R36" s="70"/>
-      <c r="S36" s="70"/>
-      <c r="T36" s="70"/>
-      <c r="U36" s="70"/>
-      <c r="V36" s="70"/>
-      <c r="W36" s="71"/>
+      <c r="P36" s="136"/>
+      <c r="Q36" s="137"/>
+      <c r="R36" s="137"/>
+      <c r="S36" s="137"/>
+      <c r="T36" s="137"/>
+      <c r="U36" s="137"/>
+      <c r="V36" s="137"/>
+      <c r="W36" s="138"/>
       <c r="X36" s="13"/>
       <c r="Z36" s="34"/>
       <c r="AA36" s="34"/>
@@ -3931,46 +3927,46 @@
       <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="78"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="87"/>
+      <c r="A37" s="142"/>
+      <c r="B37" s="149"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="150"/>
+      <c r="E37" s="150"/>
+      <c r="F37" s="150"/>
+      <c r="G37" s="150"/>
+      <c r="H37" s="150"/>
+      <c r="I37" s="150"/>
+      <c r="J37" s="150"/>
+      <c r="K37" s="151"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="73"/>
-      <c r="R37" s="73"/>
-      <c r="S37" s="73"/>
-      <c r="T37" s="73"/>
-      <c r="U37" s="73"/>
-      <c r="V37" s="73"/>
-      <c r="W37" s="74"/>
+      <c r="P37" s="139"/>
+      <c r="Q37" s="140"/>
+      <c r="R37" s="140"/>
+      <c r="S37" s="140"/>
+      <c r="T37" s="140"/>
+      <c r="U37" s="140"/>
+      <c r="V37" s="140"/>
+      <c r="W37" s="141"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="76"/>
-      <c r="I38" s="76"/>
-      <c r="J38" s="76"/>
-      <c r="K38" s="77"/>
+      <c r="C38" s="121"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="121"/>
+      <c r="F38" s="121"/>
+      <c r="G38" s="121"/>
+      <c r="H38" s="121"/>
+      <c r="I38" s="121"/>
+      <c r="J38" s="121"/>
+      <c r="K38" s="122"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3988,36 +3984,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="76"/>
-      <c r="K39" s="77"/>
+      <c r="C39" s="121"/>
+      <c r="D39" s="121"/>
+      <c r="E39" s="121"/>
+      <c r="F39" s="121"/>
+      <c r="G39" s="121"/>
+      <c r="H39" s="121"/>
+      <c r="I39" s="121"/>
+      <c r="J39" s="121"/>
+      <c r="K39" s="122"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="76"/>
-      <c r="K40" s="77"/>
+      <c r="C40" s="121"/>
+      <c r="D40" s="121"/>
+      <c r="E40" s="121"/>
+      <c r="F40" s="121"/>
+      <c r="G40" s="121"/>
+      <c r="H40" s="121"/>
+      <c r="I40" s="121"/>
+      <c r="J40" s="121"/>
+      <c r="K40" s="122"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -4036,76 +4032,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="76"/>
-      <c r="K41" s="77"/>
+      <c r="C41" s="121"/>
+      <c r="D41" s="121"/>
+      <c r="E41" s="121"/>
+      <c r="F41" s="121"/>
+      <c r="G41" s="121"/>
+      <c r="H41" s="121"/>
+      <c r="I41" s="121"/>
+      <c r="J41" s="121"/>
+      <c r="K41" s="122"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="52" t="s">
+      <c r="M41" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="53"/>
-      <c r="O41" s="53"/>
-      <c r="P41" s="53"/>
-      <c r="Q41" s="53"/>
-      <c r="R41" s="53"/>
-      <c r="S41" s="53"/>
-      <c r="T41" s="53"/>
-      <c r="U41" s="53"/>
-      <c r="V41" s="53"/>
-      <c r="W41" s="53"/>
-      <c r="X41" s="54"/>
+      <c r="N41" s="124"/>
+      <c r="O41" s="124"/>
+      <c r="P41" s="124"/>
+      <c r="Q41" s="124"/>
+      <c r="R41" s="124"/>
+      <c r="S41" s="124"/>
+      <c r="T41" s="124"/>
+      <c r="U41" s="124"/>
+      <c r="V41" s="124"/>
+      <c r="W41" s="124"/>
+      <c r="X41" s="125"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="76"/>
-      <c r="K42" s="77"/>
+      <c r="B42" s="120"/>
+      <c r="C42" s="121"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="121"/>
+      <c r="F42" s="121"/>
+      <c r="G42" s="121"/>
+      <c r="H42" s="121"/>
+      <c r="I42" s="121"/>
+      <c r="J42" s="121"/>
+      <c r="K42" s="122"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="52" t="s">
+      <c r="M42" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="53"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
-      <c r="U42" s="53"/>
-      <c r="V42" s="53"/>
-      <c r="W42" s="53"/>
-      <c r="X42" s="54"/>
+      <c r="N42" s="124"/>
+      <c r="O42" s="124"/>
+      <c r="P42" s="124"/>
+      <c r="Q42" s="124"/>
+      <c r="R42" s="124"/>
+      <c r="S42" s="124"/>
+      <c r="T42" s="124"/>
+      <c r="U42" s="124"/>
+      <c r="V42" s="124"/>
+      <c r="W42" s="124"/>
+      <c r="X42" s="125"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="75"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
-      <c r="J43" s="76"/>
-      <c r="K43" s="77"/>
+      <c r="B43" s="120"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="121"/>
+      <c r="H43" s="121"/>
+      <c r="I43" s="121"/>
+      <c r="J43" s="121"/>
+      <c r="K43" s="122"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -4123,16 +4119,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="75"/>
-      <c r="C44" s="76"/>
-      <c r="D44" s="76"/>
-      <c r="E44" s="76"/>
-      <c r="F44" s="76"/>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76"/>
-      <c r="I44" s="76"/>
-      <c r="J44" s="76"/>
-      <c r="K44" s="77"/>
+      <c r="B44" s="120"/>
+      <c r="C44" s="121"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="121"/>
+      <c r="H44" s="121"/>
+      <c r="I44" s="121"/>
+      <c r="J44" s="121"/>
+      <c r="K44" s="122"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -4150,16 +4146,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="75"/>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="76"/>
-      <c r="F45" s="76"/>
-      <c r="G45" s="76"/>
-      <c r="H45" s="76"/>
-      <c r="I45" s="76"/>
-      <c r="J45" s="76"/>
-      <c r="K45" s="77"/>
+      <c r="B45" s="120"/>
+      <c r="C45" s="121"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="121"/>
+      <c r="F45" s="121"/>
+      <c r="G45" s="121"/>
+      <c r="H45" s="121"/>
+      <c r="I45" s="121"/>
+      <c r="J45" s="121"/>
+      <c r="K45" s="122"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -4177,16 +4173,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="75"/>
-      <c r="C46" s="76"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="76"/>
-      <c r="I46" s="76"/>
-      <c r="J46" s="76"/>
-      <c r="K46" s="77"/>
+      <c r="B46" s="120"/>
+      <c r="C46" s="121"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="121"/>
+      <c r="F46" s="121"/>
+      <c r="G46" s="121"/>
+      <c r="H46" s="121"/>
+      <c r="I46" s="121"/>
+      <c r="J46" s="121"/>
+      <c r="K46" s="122"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -4229,38 +4225,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="J9:R10"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="Q19:X19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Y1:Z3"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
-    <mergeCell ref="B42:K42"/>
     <mergeCell ref="M42:X42"/>
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="Q26:X27"/>
@@ -4271,6 +4235,38 @@
     <mergeCell ref="B35:K37"/>
     <mergeCell ref="M41:X41"/>
     <mergeCell ref="B34:K34"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="Q19:X19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4281,10 +4277,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4318,8 +4314,8 @@
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="151" t="s">
-        <v>123</v>
+      <c r="A6" s="52" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -4373,7 +4369,7 @@
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="44" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4403,82 +4399,82 @@
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="42" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="39" t="s">
-        <v>118</v>
-      </c>
-    </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="42" t="s">
+      <c r="A26" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="A27" s="44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="43" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="40" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="43" t="s">
+      <c r="A29" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" t="s">
+      <c r="A32" s="45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="49" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="45" t="s">
-        <v>110</v>
-      </c>
-    </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="50" t="s">
+      <c r="A34" s="49" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="50" t="s">
+      <c r="A35" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" t="s">
+      <c r="A36" s="50" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="51" t="s">
+      <c r="A37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" t="s">
+      <c r="A38" s="47" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="48" t="s">
+      <c r="A39" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4489,117 +4485,122 @@
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" t="s">
+      <c r="A42" s="47" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="48" t="s">
+      <c r="A43" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" t="s">
+      <c r="A44" s="47" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="48" t="s">
+      <c r="A45" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" t="s">
+      <c r="A46" s="48" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="49" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="50" t="s">
+      <c r="A48" s="40" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="40" t="s">
+      <c r="A49" s="44" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="42" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="42" t="s">
-        <v>122</v>
+      <c r="A51" s="51" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="150" t="s">
+      <c r="A52" s="53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="40" t="s">
-        <v>135</v>
-      </c>
-    </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="152" t="s">
-        <v>134</v>
+      <c r="A54" s="42" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="42" t="s">
-        <v>126</v>
+      <c r="A56" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>127</v>
+      <c r="A57" s="44" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="44" t="s">
-        <v>129</v>
+      <c r="A59" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>130</v>
+      <c r="A60" s="45" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>131</v>
+      <c r="A61" s="44" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="45" t="s">
-        <v>132</v>
+      <c r="A62" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="44" t="s">
-        <v>133</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="52" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dont want cannon changes so not hunked? them
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -1551,22 +1551,277 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1589,261 +1844,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2815,14 +2815,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="Y1" s="90" t="s">
+      <c r="Y1" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="91"/>
+      <c r="Z1" s="93"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="Y2" s="92"/>
-      <c r="Z2" s="93"/>
+      <c r="Y2" s="94"/>
+      <c r="Z2" s="95"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
       <c r="AH2" s="35"/>
@@ -2831,8 +2831,8 @@
       <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="Y3" s="94"/>
-      <c r="Z3" s="95"/>
+      <c r="Y3" s="96"/>
+      <c r="Z3" s="97"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="38" t="s">
         <v>58</v>
@@ -2850,16 +2850,16 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="G4" s="54" t="s">
+      <c r="C4" s="124"/>
+      <c r="D4" s="125"/>
+      <c r="G4" s="131" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="125"/>
       <c r="Z4" s="34"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
@@ -2873,12 +2873,12 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="57"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
+      <c r="B5" s="132"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="133"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="133"/>
       <c r="Z5" s="34" t="s">
         <v>50</v>
       </c>
@@ -2920,12 +2920,12 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="145" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="147"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -2955,10 +2955,10 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="63"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="65"/>
+      <c r="B8" s="148"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="149"/>
+      <c r="E8" s="150"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2995,17 +2995,17 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="131" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="56"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="124"/>
+      <c r="O9" s="124"/>
+      <c r="P9" s="124"/>
+      <c r="Q9" s="124"/>
+      <c r="R9" s="125"/>
       <c r="Z9" s="34" t="s">
         <v>69</v>
       </c>
@@ -3033,25 +3033,25 @@
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="151" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
+      <c r="C10" s="151"/>
+      <c r="D10" s="151"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="59"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="144"/>
+      <c r="L10" s="144"/>
+      <c r="M10" s="144"/>
+      <c r="N10" s="144"/>
+      <c r="O10" s="144"/>
+      <c r="P10" s="144"/>
+      <c r="Q10" s="144"/>
+      <c r="R10" s="133"/>
       <c r="Z10" s="34">
         <v>20</v>
       </c>
@@ -3083,10 +3083,10 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="105" t="s">
+      <c r="G11" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="106"/>
+      <c r="H11" s="108"/>
       <c r="I11" s="28"/>
       <c r="Z11" s="34">
         <v>5</v>
@@ -3122,16 +3122,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="67" t="s">
+      <c r="L12" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="107"/>
+      <c r="M12" s="110"/>
+      <c r="N12" s="110"/>
+      <c r="O12" s="110"/>
+      <c r="P12" s="110"/>
+      <c r="Q12" s="110"/>
+      <c r="R12" s="110"/>
+      <c r="S12" s="111"/>
       <c r="Z12" s="34"/>
       <c r="AA12" s="34"/>
       <c r="AB12" s="34"/>
@@ -3154,14 +3154,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="70"/>
-      <c r="O13" s="70"/>
-      <c r="P13" s="70"/>
-      <c r="Q13" s="70"/>
-      <c r="R13" s="70"/>
-      <c r="S13" s="108"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="113"/>
+      <c r="O13" s="113"/>
+      <c r="P13" s="113"/>
+      <c r="Q13" s="113"/>
+      <c r="R13" s="113"/>
+      <c r="S13" s="114"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -3205,16 +3205,16 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="109" t="s">
+      <c r="Q15" s="115" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="110"/>
-      <c r="S15" s="110"/>
-      <c r="T15" s="110"/>
-      <c r="U15" s="110"/>
-      <c r="V15" s="110"/>
-      <c r="W15" s="110"/>
-      <c r="X15" s="111"/>
+      <c r="R15" s="116"/>
+      <c r="S15" s="116"/>
+      <c r="T15" s="116"/>
+      <c r="U15" s="116"/>
+      <c r="V15" s="116"/>
+      <c r="W15" s="116"/>
+      <c r="X15" s="117"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -3232,19 +3232,19 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="55" t="s">
+      <c r="M16" s="124" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="55"/>
-      <c r="O16" s="56"/>
-      <c r="Q16" s="112"/>
-      <c r="R16" s="113"/>
-      <c r="S16" s="113"/>
-      <c r="T16" s="113"/>
-      <c r="U16" s="113"/>
-      <c r="V16" s="113"/>
-      <c r="W16" s="113"/>
-      <c r="X16" s="114"/>
+      <c r="N16" s="124"/>
+      <c r="O16" s="125"/>
+      <c r="Q16" s="118"/>
+      <c r="R16" s="119"/>
+      <c r="S16" s="119"/>
+      <c r="T16" s="119"/>
+      <c r="U16" s="119"/>
+      <c r="V16" s="119"/>
+      <c r="W16" s="119"/>
+      <c r="X16" s="120"/>
       <c r="Z16" s="34"/>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
@@ -3258,31 +3258,31 @@
       <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="110"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="71" t="s">
+      <c r="E17" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="72"/>
-      <c r="G17" s="73"/>
+      <c r="F17" s="129"/>
+      <c r="G17" s="130"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="119"/>
-      <c r="Q17" s="115"/>
-      <c r="R17" s="116"/>
-      <c r="S17" s="116"/>
-      <c r="T17" s="116"/>
-      <c r="U17" s="116"/>
-      <c r="V17" s="116"/>
-      <c r="W17" s="116"/>
-      <c r="X17" s="117"/>
+      <c r="M17" s="126"/>
+      <c r="N17" s="126"/>
+      <c r="O17" s="127"/>
+      <c r="Q17" s="121"/>
+      <c r="R17" s="122"/>
+      <c r="S17" s="122"/>
+      <c r="T17" s="122"/>
+      <c r="U17" s="122"/>
+      <c r="V17" s="122"/>
+      <c r="W17" s="122"/>
+      <c r="X17" s="123"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -3296,18 +3296,18 @@
       <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="69"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="113"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="74" t="s">
+      <c r="L18" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="75"/>
+      <c r="M18" s="91"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3332,32 +3332,32 @@
       <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="56"/>
+      <c r="C19" s="125"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="75"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="91"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="76" t="s">
+      <c r="Q19" s="134" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="77"/>
-      <c r="S19" s="77"/>
-      <c r="T19" s="77"/>
-      <c r="U19" s="77"/>
-      <c r="V19" s="77"/>
-      <c r="W19" s="77"/>
-      <c r="X19" s="78"/>
+      <c r="R19" s="135"/>
+      <c r="S19" s="135"/>
+      <c r="T19" s="135"/>
+      <c r="U19" s="135"/>
+      <c r="V19" s="135"/>
+      <c r="W19" s="135"/>
+      <c r="X19" s="136"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -3371,32 +3371,32 @@
       <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="57"/>
-      <c r="C20" s="59"/>
-      <c r="F20" s="79" t="s">
+      <c r="B20" s="132"/>
+      <c r="C20" s="133"/>
+      <c r="F20" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="80"/>
+      <c r="G20" s="138"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="74" t="s">
+      <c r="L20" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="75"/>
+      <c r="M20" s="91"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="83" t="s">
+      <c r="Q20" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="84"/>
-      <c r="S20" s="84"/>
-      <c r="T20" s="84"/>
-      <c r="U20" s="84"/>
-      <c r="V20" s="84"/>
-      <c r="W20" s="84"/>
-      <c r="X20" s="85"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
+      <c r="W20" s="58"/>
+      <c r="X20" s="66"/>
       <c r="Z20" s="34"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
@@ -3413,28 +3413,28 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="82"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="140"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="75"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="91"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="86" t="s">
+      <c r="Q21" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="87"/>
-      <c r="S21" s="87"/>
-      <c r="T21" s="87"/>
-      <c r="U21" s="87"/>
-      <c r="V21" s="87"/>
-      <c r="W21" s="87"/>
-      <c r="X21" s="88"/>
+      <c r="R21" s="142"/>
+      <c r="S21" s="142"/>
+      <c r="T21" s="142"/>
+      <c r="U21" s="142"/>
+      <c r="V21" s="142"/>
+      <c r="W21" s="142"/>
+      <c r="X21" s="143"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -3452,10 +3452,10 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="74" t="s">
+      <c r="L22" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="75"/>
+      <c r="M22" s="91"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -3475,28 +3475,28 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="83" t="s">
+      <c r="E23" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="84"/>
-      <c r="G23" s="89"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="59"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="75"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="91"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="96" t="s">
+      <c r="Q23" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="97"/>
-      <c r="S23" s="97"/>
-      <c r="T23" s="97"/>
-      <c r="U23" s="97"/>
-      <c r="V23" s="97"/>
-      <c r="W23" s="97"/>
-      <c r="X23" s="98"/>
+      <c r="R23" s="99"/>
+      <c r="S23" s="99"/>
+      <c r="T23" s="99"/>
+      <c r="U23" s="99"/>
+      <c r="V23" s="99"/>
+      <c r="W23" s="99"/>
+      <c r="X23" s="100"/>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
@@ -3514,20 +3514,20 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="74" t="s">
+      <c r="L24" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="75"/>
+      <c r="M24" s="91"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="99"/>
-      <c r="R24" s="100"/>
-      <c r="S24" s="100"/>
-      <c r="T24" s="100"/>
-      <c r="U24" s="100"/>
-      <c r="V24" s="100"/>
-      <c r="W24" s="100"/>
-      <c r="X24" s="101"/>
+      <c r="Q24" s="101"/>
+      <c r="R24" s="102"/>
+      <c r="S24" s="102"/>
+      <c r="T24" s="102"/>
+      <c r="U24" s="102"/>
+      <c r="V24" s="102"/>
+      <c r="W24" s="102"/>
+      <c r="X24" s="103"/>
       <c r="Z24" s="34"/>
       <c r="AA24" s="34"/>
       <c r="AB24" s="34"/>
@@ -3545,18 +3545,18 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="75"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="91"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="102"/>
-      <c r="R25" s="103"/>
-      <c r="S25" s="103"/>
-      <c r="T25" s="103"/>
-      <c r="U25" s="103"/>
-      <c r="V25" s="103"/>
-      <c r="W25" s="103"/>
-      <c r="X25" s="104"/>
+      <c r="Q25" s="104"/>
+      <c r="R25" s="105"/>
+      <c r="S25" s="105"/>
+      <c r="T25" s="105"/>
+      <c r="U25" s="105"/>
+      <c r="V25" s="105"/>
+      <c r="W25" s="105"/>
+      <c r="X25" s="106"/>
       <c r="Z25" s="34"/>
       <c r="AA25" s="34"/>
       <c r="AB25" s="34"/>
@@ -3573,26 +3573,26 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="83"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
-      <c r="K26" s="89"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="126" t="s">
+      <c r="Q26" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="127"/>
-      <c r="S26" s="127"/>
-      <c r="T26" s="127"/>
-      <c r="U26" s="127"/>
-      <c r="V26" s="127"/>
-      <c r="W26" s="127"/>
-      <c r="X26" s="128"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="61"/>
+      <c r="T26" s="61"/>
+      <c r="U26" s="61"/>
+      <c r="V26" s="61"/>
+      <c r="W26" s="61"/>
+      <c r="X26" s="62"/>
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
       <c r="AB26" s="34"/>
@@ -3608,14 +3608,14 @@
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="129"/>
-      <c r="R27" s="130"/>
-      <c r="S27" s="130"/>
-      <c r="T27" s="130"/>
-      <c r="U27" s="130"/>
-      <c r="V27" s="130"/>
-      <c r="W27" s="130"/>
-      <c r="X27" s="131"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="64"/>
+      <c r="S27" s="64"/>
+      <c r="T27" s="64"/>
+      <c r="U27" s="64"/>
+      <c r="V27" s="64"/>
+      <c r="W27" s="64"/>
+      <c r="X27" s="65"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -3649,16 +3649,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="83" t="s">
+      <c r="Q29" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="84"/>
-      <c r="S29" s="84"/>
-      <c r="T29" s="84"/>
-      <c r="U29" s="84"/>
-      <c r="V29" s="84"/>
-      <c r="W29" s="84"/>
-      <c r="X29" s="85"/>
+      <c r="R29" s="58"/>
+      <c r="S29" s="58"/>
+      <c r="T29" s="58"/>
+      <c r="U29" s="58"/>
+      <c r="V29" s="58"/>
+      <c r="W29" s="58"/>
+      <c r="X29" s="66"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -3699,32 +3699,32 @@
       <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="132" t="s">
+      <c r="A31" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="132"/>
-      <c r="C31" s="132"/>
-      <c r="D31" s="132"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="132"/>
-      <c r="G31" s="132"/>
-      <c r="H31" s="132"/>
-      <c r="I31" s="132"/>
-      <c r="J31" s="132"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="133" t="s">
+      <c r="P31" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="134"/>
-      <c r="R31" s="134"/>
-      <c r="S31" s="134"/>
-      <c r="T31" s="134"/>
-      <c r="U31" s="134"/>
-      <c r="V31" s="134"/>
-      <c r="W31" s="135"/>
+      <c r="Q31" s="69"/>
+      <c r="R31" s="69"/>
+      <c r="S31" s="69"/>
+      <c r="T31" s="69"/>
+      <c r="U31" s="69"/>
+      <c r="V31" s="69"/>
+      <c r="W31" s="70"/>
       <c r="X31" s="13"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
@@ -3739,28 +3739,28 @@
       <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="132"/>
-      <c r="B32" s="132"/>
-      <c r="C32" s="132"/>
-      <c r="D32" s="132"/>
-      <c r="E32" s="132"/>
-      <c r="F32" s="132"/>
-      <c r="G32" s="132"/>
-      <c r="H32" s="132"/>
-      <c r="I32" s="132"/>
-      <c r="J32" s="132"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="136"/>
-      <c r="Q32" s="137"/>
-      <c r="R32" s="137"/>
-      <c r="S32" s="137"/>
-      <c r="T32" s="137"/>
-      <c r="U32" s="137"/>
-      <c r="V32" s="137"/>
-      <c r="W32" s="138"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="72"/>
+      <c r="R32" s="72"/>
+      <c r="S32" s="72"/>
+      <c r="T32" s="72"/>
+      <c r="U32" s="72"/>
+      <c r="V32" s="72"/>
+      <c r="W32" s="73"/>
       <c r="X32" s="13"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
@@ -3789,14 +3789,14 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="136"/>
-      <c r="Q33" s="137"/>
-      <c r="R33" s="137"/>
-      <c r="S33" s="137"/>
-      <c r="T33" s="137"/>
-      <c r="U33" s="137"/>
-      <c r="V33" s="137"/>
-      <c r="W33" s="138"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="72"/>
+      <c r="R33" s="72"/>
+      <c r="S33" s="72"/>
+      <c r="T33" s="72"/>
+      <c r="U33" s="72"/>
+      <c r="V33" s="72"/>
+      <c r="W33" s="73"/>
       <c r="X33" s="13"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="34"/>
@@ -3814,29 +3814,29 @@
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="142" t="s">
+      <c r="B34" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="142"/>
-      <c r="D34" s="142"/>
-      <c r="E34" s="142"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="142"/>
-      <c r="H34" s="142"/>
-      <c r="I34" s="142"/>
-      <c r="J34" s="142"/>
-      <c r="K34" s="142"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="136"/>
-      <c r="Q34" s="137"/>
-      <c r="R34" s="137"/>
-      <c r="S34" s="137"/>
-      <c r="T34" s="137"/>
-      <c r="U34" s="137"/>
-      <c r="V34" s="137"/>
-      <c r="W34" s="138"/>
+      <c r="P34" s="71"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="72"/>
+      <c r="S34" s="72"/>
+      <c r="T34" s="72"/>
+      <c r="U34" s="72"/>
+      <c r="V34" s="72"/>
+      <c r="W34" s="73"/>
       <c r="X34" s="13"/>
       <c r="Z34" s="34"/>
       <c r="AA34" s="34"/>
@@ -3851,32 +3851,32 @@
       <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="142" t="s">
+      <c r="A35" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="143" t="s">
+      <c r="B35" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
-      <c r="H35" s="144"/>
-      <c r="I35" s="144"/>
-      <c r="J35" s="144"/>
-      <c r="K35" s="145"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="80"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="136"/>
-      <c r="Q35" s="137"/>
-      <c r="R35" s="137"/>
-      <c r="S35" s="137"/>
-      <c r="T35" s="137"/>
-      <c r="U35" s="137"/>
-      <c r="V35" s="137"/>
-      <c r="W35" s="138"/>
+      <c r="P35" s="71"/>
+      <c r="Q35" s="72"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="72"/>
+      <c r="T35" s="72"/>
+      <c r="U35" s="72"/>
+      <c r="V35" s="72"/>
+      <c r="W35" s="73"/>
       <c r="X35" s="13"/>
       <c r="Z35" s="34"/>
       <c r="AA35" s="34"/>
@@ -3891,28 +3891,28 @@
       <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="142"/>
-      <c r="B36" s="146"/>
-      <c r="C36" s="147"/>
-      <c r="D36" s="147"/>
-      <c r="E36" s="147"/>
-      <c r="F36" s="147"/>
-      <c r="G36" s="147"/>
-      <c r="H36" s="147"/>
-      <c r="I36" s="147"/>
-      <c r="J36" s="147"/>
-      <c r="K36" s="148"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="81"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="83"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="136"/>
-      <c r="Q36" s="137"/>
-      <c r="R36" s="137"/>
-      <c r="S36" s="137"/>
-      <c r="T36" s="137"/>
-      <c r="U36" s="137"/>
-      <c r="V36" s="137"/>
-      <c r="W36" s="138"/>
+      <c r="P36" s="71"/>
+      <c r="Q36" s="72"/>
+      <c r="R36" s="72"/>
+      <c r="S36" s="72"/>
+      <c r="T36" s="72"/>
+      <c r="U36" s="72"/>
+      <c r="V36" s="72"/>
+      <c r="W36" s="73"/>
       <c r="X36" s="13"/>
       <c r="Z36" s="34"/>
       <c r="AA36" s="34"/>
@@ -3927,46 +3927,46 @@
       <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="142"/>
-      <c r="B37" s="149"/>
-      <c r="C37" s="150"/>
-      <c r="D37" s="150"/>
-      <c r="E37" s="150"/>
-      <c r="F37" s="150"/>
-      <c r="G37" s="150"/>
-      <c r="H37" s="150"/>
-      <c r="I37" s="150"/>
-      <c r="J37" s="150"/>
-      <c r="K37" s="151"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="86"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="139"/>
-      <c r="Q37" s="140"/>
-      <c r="R37" s="140"/>
-      <c r="S37" s="140"/>
-      <c r="T37" s="140"/>
-      <c r="U37" s="140"/>
-      <c r="V37" s="140"/>
-      <c r="W37" s="141"/>
+      <c r="P37" s="74"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="75"/>
+      <c r="S37" s="75"/>
+      <c r="T37" s="75"/>
+      <c r="U37" s="75"/>
+      <c r="V37" s="75"/>
+      <c r="W37" s="76"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="120" t="s">
+      <c r="B38" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="121"/>
-      <c r="D38" s="121"/>
-      <c r="E38" s="121"/>
-      <c r="F38" s="121"/>
-      <c r="G38" s="121"/>
-      <c r="H38" s="121"/>
-      <c r="I38" s="121"/>
-      <c r="J38" s="121"/>
-      <c r="K38" s="122"/>
+      <c r="C38" s="88"/>
+      <c r="D38" s="88"/>
+      <c r="E38" s="88"/>
+      <c r="F38" s="88"/>
+      <c r="G38" s="88"/>
+      <c r="H38" s="88"/>
+      <c r="I38" s="88"/>
+      <c r="J38" s="88"/>
+      <c r="K38" s="89"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3984,36 +3984,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="120" t="s">
+      <c r="B39" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="121"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="121"/>
-      <c r="F39" s="121"/>
-      <c r="G39" s="121"/>
-      <c r="H39" s="121"/>
-      <c r="I39" s="121"/>
-      <c r="J39" s="121"/>
-      <c r="K39" s="122"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="88"/>
+      <c r="E39" s="88"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="88"/>
+      <c r="H39" s="88"/>
+      <c r="I39" s="88"/>
+      <c r="J39" s="88"/>
+      <c r="K39" s="89"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="120" t="s">
+      <c r="B40" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="121"/>
-      <c r="D40" s="121"/>
-      <c r="E40" s="121"/>
-      <c r="F40" s="121"/>
-      <c r="G40" s="121"/>
-      <c r="H40" s="121"/>
-      <c r="I40" s="121"/>
-      <c r="J40" s="121"/>
-      <c r="K40" s="122"/>
+      <c r="C40" s="88"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="88"/>
+      <c r="F40" s="88"/>
+      <c r="G40" s="88"/>
+      <c r="H40" s="88"/>
+      <c r="I40" s="88"/>
+      <c r="J40" s="88"/>
+      <c r="K40" s="89"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -4032,76 +4032,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="120" t="s">
+      <c r="B41" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="121"/>
-      <c r="D41" s="121"/>
-      <c r="E41" s="121"/>
-      <c r="F41" s="121"/>
-      <c r="G41" s="121"/>
-      <c r="H41" s="121"/>
-      <c r="I41" s="121"/>
-      <c r="J41" s="121"/>
-      <c r="K41" s="122"/>
+      <c r="C41" s="88"/>
+      <c r="D41" s="88"/>
+      <c r="E41" s="88"/>
+      <c r="F41" s="88"/>
+      <c r="G41" s="88"/>
+      <c r="H41" s="88"/>
+      <c r="I41" s="88"/>
+      <c r="J41" s="88"/>
+      <c r="K41" s="89"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="123" t="s">
+      <c r="M41" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="124"/>
-      <c r="O41" s="124"/>
-      <c r="P41" s="124"/>
-      <c r="Q41" s="124"/>
-      <c r="R41" s="124"/>
-      <c r="S41" s="124"/>
-      <c r="T41" s="124"/>
-      <c r="U41" s="124"/>
-      <c r="V41" s="124"/>
-      <c r="W41" s="124"/>
-      <c r="X41" s="125"/>
+      <c r="N41" s="55"/>
+      <c r="O41" s="55"/>
+      <c r="P41" s="55"/>
+      <c r="Q41" s="55"/>
+      <c r="R41" s="55"/>
+      <c r="S41" s="55"/>
+      <c r="T41" s="55"/>
+      <c r="U41" s="55"/>
+      <c r="V41" s="55"/>
+      <c r="W41" s="55"/>
+      <c r="X41" s="56"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="120"/>
-      <c r="C42" s="121"/>
-      <c r="D42" s="121"/>
-      <c r="E42" s="121"/>
-      <c r="F42" s="121"/>
-      <c r="G42" s="121"/>
-      <c r="H42" s="121"/>
-      <c r="I42" s="121"/>
-      <c r="J42" s="121"/>
-      <c r="K42" s="122"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="88"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="88"/>
+      <c r="H42" s="88"/>
+      <c r="I42" s="88"/>
+      <c r="J42" s="88"/>
+      <c r="K42" s="89"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="123" t="s">
+      <c r="M42" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="124"/>
-      <c r="O42" s="124"/>
-      <c r="P42" s="124"/>
-      <c r="Q42" s="124"/>
-      <c r="R42" s="124"/>
-      <c r="S42" s="124"/>
-      <c r="T42" s="124"/>
-      <c r="U42" s="124"/>
-      <c r="V42" s="124"/>
-      <c r="W42" s="124"/>
-      <c r="X42" s="125"/>
+      <c r="N42" s="55"/>
+      <c r="O42" s="55"/>
+      <c r="P42" s="55"/>
+      <c r="Q42" s="55"/>
+      <c r="R42" s="55"/>
+      <c r="S42" s="55"/>
+      <c r="T42" s="55"/>
+      <c r="U42" s="55"/>
+      <c r="V42" s="55"/>
+      <c r="W42" s="55"/>
+      <c r="X42" s="56"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="120"/>
-      <c r="C43" s="121"/>
-      <c r="D43" s="121"/>
-      <c r="E43" s="121"/>
-      <c r="F43" s="121"/>
-      <c r="G43" s="121"/>
-      <c r="H43" s="121"/>
-      <c r="I43" s="121"/>
-      <c r="J43" s="121"/>
-      <c r="K43" s="122"/>
+      <c r="B43" s="87"/>
+      <c r="C43" s="88"/>
+      <c r="D43" s="88"/>
+      <c r="E43" s="88"/>
+      <c r="F43" s="88"/>
+      <c r="G43" s="88"/>
+      <c r="H43" s="88"/>
+      <c r="I43" s="88"/>
+      <c r="J43" s="88"/>
+      <c r="K43" s="89"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -4119,16 +4119,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="120"/>
-      <c r="C44" s="121"/>
-      <c r="D44" s="121"/>
-      <c r="E44" s="121"/>
-      <c r="F44" s="121"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="121"/>
-      <c r="I44" s="121"/>
-      <c r="J44" s="121"/>
-      <c r="K44" s="122"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="88"/>
+      <c r="E44" s="88"/>
+      <c r="F44" s="88"/>
+      <c r="G44" s="88"/>
+      <c r="H44" s="88"/>
+      <c r="I44" s="88"/>
+      <c r="J44" s="88"/>
+      <c r="K44" s="89"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -4146,16 +4146,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="120"/>
-      <c r="C45" s="121"/>
-      <c r="D45" s="121"/>
-      <c r="E45" s="121"/>
-      <c r="F45" s="121"/>
-      <c r="G45" s="121"/>
-      <c r="H45" s="121"/>
-      <c r="I45" s="121"/>
-      <c r="J45" s="121"/>
-      <c r="K45" s="122"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="88"/>
+      <c r="D45" s="88"/>
+      <c r="E45" s="88"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="88"/>
+      <c r="H45" s="88"/>
+      <c r="I45" s="88"/>
+      <c r="J45" s="88"/>
+      <c r="K45" s="89"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -4173,16 +4173,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="120"/>
-      <c r="C46" s="121"/>
-      <c r="D46" s="121"/>
-      <c r="E46" s="121"/>
-      <c r="F46" s="121"/>
-      <c r="G46" s="121"/>
-      <c r="H46" s="121"/>
-      <c r="I46" s="121"/>
-      <c r="J46" s="121"/>
-      <c r="K46" s="122"/>
+      <c r="B46" s="87"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="88"/>
+      <c r="F46" s="88"/>
+      <c r="G46" s="88"/>
+      <c r="H46" s="88"/>
+      <c r="I46" s="88"/>
+      <c r="J46" s="88"/>
+      <c r="K46" s="89"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -4225,6 +4225,38 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:R10"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="Q19:X19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B42:K42"/>
     <mergeCell ref="M42:X42"/>
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="Q26:X27"/>
@@ -4235,38 +4267,6 @@
     <mergeCell ref="B35:K37"/>
     <mergeCell ref="M41:X41"/>
     <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Y1:Z3"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="Q19:X19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="J9:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
replaced arduinoReceiver script with laptop one, not testable arduino not working
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>try seperating all my ai attack pattern script from the original ai one and just feed the transform to it</t>
+  </si>
+  <si>
+    <t>make sure one version of arduino stuff and arduino works</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -721,6 +724,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="56">
     <border>
@@ -1399,7 +1408,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1528,22 +1537,277 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1567,261 +1831,7 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -2792,14 +2802,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="Y1" s="88" t="s">
+      <c r="Y1" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="89"/>
+      <c r="Z1" s="91"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="91"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="93"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
       <c r="AH2" s="35"/>
@@ -2808,8 +2818,8 @@
       <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="93"/>
+      <c r="Y3" s="94"/>
+      <c r="Z3" s="95"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="38" t="s">
         <v>58</v>
@@ -2827,16 +2837,16 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
-      <c r="G4" s="52" t="s">
+      <c r="C4" s="122"/>
+      <c r="D4" s="123"/>
+      <c r="G4" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="123"/>
       <c r="Z4" s="34"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
@@ -2850,12 +2860,12 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="57"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="57"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="131"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="131"/>
       <c r="Z5" s="34" t="s">
         <v>50</v>
       </c>
@@ -2897,12 +2907,12 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="60"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="145"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -2932,10 +2942,10 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="61"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="148"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2972,17 +2982,17 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="52" t="s">
+      <c r="J9" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="54"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="122"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="122"/>
+      <c r="O9" s="122"/>
+      <c r="P9" s="122"/>
+      <c r="Q9" s="122"/>
+      <c r="R9" s="123"/>
       <c r="Z9" s="34" t="s">
         <v>69</v>
       </c>
@@ -3010,25 +3020,25 @@
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="149"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="57"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="142"/>
+      <c r="Q10" s="142"/>
+      <c r="R10" s="131"/>
       <c r="Z10" s="34">
         <v>20</v>
       </c>
@@ -3060,10 +3070,10 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="103" t="s">
+      <c r="G11" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="104"/>
+      <c r="H11" s="106"/>
       <c r="I11" s="28"/>
       <c r="Z11" s="34">
         <v>5</v>
@@ -3099,16 +3109,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="65" t="s">
+      <c r="L12" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="105"/>
+      <c r="M12" s="108"/>
+      <c r="N12" s="108"/>
+      <c r="O12" s="108"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="109"/>
       <c r="Z12" s="34"/>
       <c r="AA12" s="34"/>
       <c r="AB12" s="34"/>
@@ -3131,14 +3141,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="68"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="106"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="111"/>
+      <c r="S13" s="112"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -3182,16 +3192,16 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="107" t="s">
+      <c r="Q15" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="108"/>
-      <c r="S15" s="108"/>
-      <c r="T15" s="108"/>
-      <c r="U15" s="108"/>
-      <c r="V15" s="108"/>
-      <c r="W15" s="108"/>
-      <c r="X15" s="109"/>
+      <c r="R15" s="114"/>
+      <c r="S15" s="114"/>
+      <c r="T15" s="114"/>
+      <c r="U15" s="114"/>
+      <c r="V15" s="114"/>
+      <c r="W15" s="114"/>
+      <c r="X15" s="115"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -3209,19 +3219,19 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="53" t="s">
+      <c r="M16" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="53"/>
-      <c r="O16" s="54"/>
-      <c r="Q16" s="110"/>
-      <c r="R16" s="111"/>
-      <c r="S16" s="111"/>
-      <c r="T16" s="111"/>
-      <c r="U16" s="111"/>
-      <c r="V16" s="111"/>
-      <c r="W16" s="111"/>
-      <c r="X16" s="112"/>
+      <c r="N16" s="122"/>
+      <c r="O16" s="123"/>
+      <c r="Q16" s="116"/>
+      <c r="R16" s="117"/>
+      <c r="S16" s="117"/>
+      <c r="T16" s="117"/>
+      <c r="U16" s="117"/>
+      <c r="V16" s="117"/>
+      <c r="W16" s="117"/>
+      <c r="X16" s="118"/>
       <c r="Z16" s="34"/>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
@@ -3235,31 +3245,31 @@
       <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="66"/>
+      <c r="C17" s="108"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="69" t="s">
+      <c r="E17" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="70"/>
-      <c r="G17" s="71"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="128"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="116"/>
-      <c r="N17" s="116"/>
-      <c r="O17" s="117"/>
-      <c r="Q17" s="113"/>
-      <c r="R17" s="114"/>
-      <c r="S17" s="114"/>
-      <c r="T17" s="114"/>
-      <c r="U17" s="114"/>
-      <c r="V17" s="114"/>
-      <c r="W17" s="114"/>
-      <c r="X17" s="115"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="124"/>
+      <c r="O17" s="125"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="120"/>
+      <c r="S17" s="120"/>
+      <c r="T17" s="120"/>
+      <c r="U17" s="120"/>
+      <c r="V17" s="120"/>
+      <c r="W17" s="120"/>
+      <c r="X17" s="121"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -3273,18 +3283,18 @@
       <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="67"/>
-      <c r="C18" s="68"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="111"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="72" t="s">
+      <c r="L18" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="73"/>
+      <c r="M18" s="89"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3309,32 +3319,32 @@
       <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="54"/>
+      <c r="C19" s="123"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="73"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="89"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="74" t="s">
+      <c r="Q19" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75"/>
-      <c r="T19" s="75"/>
-      <c r="U19" s="75"/>
-      <c r="V19" s="75"/>
-      <c r="W19" s="75"/>
-      <c r="X19" s="76"/>
+      <c r="R19" s="133"/>
+      <c r="S19" s="133"/>
+      <c r="T19" s="133"/>
+      <c r="U19" s="133"/>
+      <c r="V19" s="133"/>
+      <c r="W19" s="133"/>
+      <c r="X19" s="134"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -3348,32 +3358,32 @@
       <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="55"/>
-      <c r="C20" s="57"/>
-      <c r="F20" s="77" t="s">
+      <c r="B20" s="130"/>
+      <c r="C20" s="131"/>
+      <c r="F20" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="78"/>
+      <c r="G20" s="136"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="72" t="s">
+      <c r="L20" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="73"/>
+      <c r="M20" s="89"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="81" t="s">
+      <c r="Q20" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="82"/>
-      <c r="S20" s="82"/>
-      <c r="T20" s="82"/>
-      <c r="U20" s="82"/>
-      <c r="V20" s="82"/>
-      <c r="W20" s="82"/>
-      <c r="X20" s="83"/>
+      <c r="R20" s="56"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="56"/>
+      <c r="U20" s="56"/>
+      <c r="V20" s="56"/>
+      <c r="W20" s="56"/>
+      <c r="X20" s="64"/>
       <c r="Z20" s="34"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
@@ -3390,28 +3400,28 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="80"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="138"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="73"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="89"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="84" t="s">
+      <c r="Q21" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="85"/>
-      <c r="S21" s="85"/>
-      <c r="T21" s="85"/>
-      <c r="U21" s="85"/>
-      <c r="V21" s="85"/>
-      <c r="W21" s="85"/>
-      <c r="X21" s="86"/>
+      <c r="R21" s="140"/>
+      <c r="S21" s="140"/>
+      <c r="T21" s="140"/>
+      <c r="U21" s="140"/>
+      <c r="V21" s="140"/>
+      <c r="W21" s="140"/>
+      <c r="X21" s="141"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -3429,10 +3439,10 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="72" t="s">
+      <c r="L22" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="73"/>
+      <c r="M22" s="89"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -3452,28 +3462,28 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="81" t="s">
+      <c r="E23" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="82"/>
-      <c r="G23" s="87"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="57"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="73"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="89"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="94" t="s">
+      <c r="Q23" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="95"/>
-      <c r="S23" s="95"/>
-      <c r="T23" s="95"/>
-      <c r="U23" s="95"/>
-      <c r="V23" s="95"/>
-      <c r="W23" s="95"/>
-      <c r="X23" s="96"/>
+      <c r="R23" s="97"/>
+      <c r="S23" s="97"/>
+      <c r="T23" s="97"/>
+      <c r="U23" s="97"/>
+      <c r="V23" s="97"/>
+      <c r="W23" s="97"/>
+      <c r="X23" s="98"/>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
@@ -3491,20 +3501,20 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="72" t="s">
+      <c r="L24" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="73"/>
+      <c r="M24" s="89"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="97"/>
-      <c r="R24" s="98"/>
-      <c r="S24" s="98"/>
-      <c r="T24" s="98"/>
-      <c r="U24" s="98"/>
-      <c r="V24" s="98"/>
-      <c r="W24" s="98"/>
-      <c r="X24" s="99"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
+      <c r="S24" s="100"/>
+      <c r="T24" s="100"/>
+      <c r="U24" s="100"/>
+      <c r="V24" s="100"/>
+      <c r="W24" s="100"/>
+      <c r="X24" s="101"/>
       <c r="Z24" s="34"/>
       <c r="AA24" s="34"/>
       <c r="AB24" s="34"/>
@@ -3522,18 +3532,18 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="73"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="89"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="100"/>
-      <c r="R25" s="101"/>
-      <c r="S25" s="101"/>
-      <c r="T25" s="101"/>
-      <c r="U25" s="101"/>
-      <c r="V25" s="101"/>
-      <c r="W25" s="101"/>
-      <c r="X25" s="102"/>
+      <c r="Q25" s="102"/>
+      <c r="R25" s="103"/>
+      <c r="S25" s="103"/>
+      <c r="T25" s="103"/>
+      <c r="U25" s="103"/>
+      <c r="V25" s="103"/>
+      <c r="W25" s="103"/>
+      <c r="X25" s="104"/>
       <c r="Z25" s="34"/>
       <c r="AA25" s="34"/>
       <c r="AB25" s="34"/>
@@ -3550,26 +3560,26 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="81"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="82"/>
-      <c r="K26" s="87"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="57"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="124" t="s">
+      <c r="Q26" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="125"/>
-      <c r="S26" s="125"/>
-      <c r="T26" s="125"/>
-      <c r="U26" s="125"/>
-      <c r="V26" s="125"/>
-      <c r="W26" s="125"/>
-      <c r="X26" s="126"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="60"/>
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
       <c r="AB26" s="34"/>
@@ -3585,14 +3595,14 @@
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="127"/>
-      <c r="R27" s="128"/>
-      <c r="S27" s="128"/>
-      <c r="T27" s="128"/>
-      <c r="U27" s="128"/>
-      <c r="V27" s="128"/>
-      <c r="W27" s="128"/>
-      <c r="X27" s="129"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="63"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -3626,16 +3636,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="81" t="s">
+      <c r="Q29" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="82"/>
-      <c r="S29" s="82"/>
-      <c r="T29" s="82"/>
-      <c r="U29" s="82"/>
-      <c r="V29" s="82"/>
-      <c r="W29" s="82"/>
-      <c r="X29" s="83"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
+      <c r="X29" s="64"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -3676,32 +3686,32 @@
       <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="130" t="s">
+      <c r="A31" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="130"/>
-      <c r="C31" s="130"/>
-      <c r="D31" s="130"/>
-      <c r="E31" s="130"/>
-      <c r="F31" s="130"/>
-      <c r="G31" s="130"/>
-      <c r="H31" s="130"/>
-      <c r="I31" s="130"/>
-      <c r="J31" s="130"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="131" t="s">
+      <c r="P31" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="132"/>
-      <c r="R31" s="132"/>
-      <c r="S31" s="132"/>
-      <c r="T31" s="132"/>
-      <c r="U31" s="132"/>
-      <c r="V31" s="132"/>
-      <c r="W31" s="133"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="67"/>
+      <c r="T31" s="67"/>
+      <c r="U31" s="67"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="68"/>
       <c r="X31" s="13"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
@@ -3716,28 +3726,28 @@
       <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="130"/>
-      <c r="B32" s="130"/>
-      <c r="C32" s="130"/>
-      <c r="D32" s="130"/>
-      <c r="E32" s="130"/>
-      <c r="F32" s="130"/>
-      <c r="G32" s="130"/>
-      <c r="H32" s="130"/>
-      <c r="I32" s="130"/>
-      <c r="J32" s="130"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="134"/>
-      <c r="Q32" s="135"/>
-      <c r="R32" s="135"/>
-      <c r="S32" s="135"/>
-      <c r="T32" s="135"/>
-      <c r="U32" s="135"/>
-      <c r="V32" s="135"/>
-      <c r="W32" s="136"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="70"/>
+      <c r="R32" s="70"/>
+      <c r="S32" s="70"/>
+      <c r="T32" s="70"/>
+      <c r="U32" s="70"/>
+      <c r="V32" s="70"/>
+      <c r="W32" s="71"/>
       <c r="X32" s="13"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
@@ -3766,14 +3776,14 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="134"/>
-      <c r="Q33" s="135"/>
-      <c r="R33" s="135"/>
-      <c r="S33" s="135"/>
-      <c r="T33" s="135"/>
-      <c r="U33" s="135"/>
-      <c r="V33" s="135"/>
-      <c r="W33" s="136"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="70"/>
+      <c r="R33" s="70"/>
+      <c r="S33" s="70"/>
+      <c r="T33" s="70"/>
+      <c r="U33" s="70"/>
+      <c r="V33" s="70"/>
+      <c r="W33" s="71"/>
       <c r="X33" s="13"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="34"/>
@@ -3791,29 +3801,29 @@
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="140" t="s">
+      <c r="B34" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="140"/>
-      <c r="D34" s="140"/>
-      <c r="E34" s="140"/>
-      <c r="F34" s="140"/>
-      <c r="G34" s="140"/>
-      <c r="H34" s="140"/>
-      <c r="I34" s="140"/>
-      <c r="J34" s="140"/>
-      <c r="K34" s="140"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="134"/>
-      <c r="Q34" s="135"/>
-      <c r="R34" s="135"/>
-      <c r="S34" s="135"/>
-      <c r="T34" s="135"/>
-      <c r="U34" s="135"/>
-      <c r="V34" s="135"/>
-      <c r="W34" s="136"/>
+      <c r="P34" s="69"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="70"/>
+      <c r="W34" s="71"/>
       <c r="X34" s="13"/>
       <c r="Z34" s="34"/>
       <c r="AA34" s="34"/>
@@ -3828,32 +3838,32 @@
       <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="140" t="s">
+      <c r="A35" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="141" t="s">
+      <c r="B35" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="142"/>
-      <c r="D35" s="142"/>
-      <c r="E35" s="142"/>
-      <c r="F35" s="142"/>
-      <c r="G35" s="142"/>
-      <c r="H35" s="142"/>
-      <c r="I35" s="142"/>
-      <c r="J35" s="142"/>
-      <c r="K35" s="143"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="134"/>
-      <c r="Q35" s="135"/>
-      <c r="R35" s="135"/>
-      <c r="S35" s="135"/>
-      <c r="T35" s="135"/>
-      <c r="U35" s="135"/>
-      <c r="V35" s="135"/>
-      <c r="W35" s="136"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="70"/>
+      <c r="R35" s="70"/>
+      <c r="S35" s="70"/>
+      <c r="T35" s="70"/>
+      <c r="U35" s="70"/>
+      <c r="V35" s="70"/>
+      <c r="W35" s="71"/>
       <c r="X35" s="13"/>
       <c r="Z35" s="34"/>
       <c r="AA35" s="34"/>
@@ -3868,28 +3878,28 @@
       <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="140"/>
-      <c r="B36" s="144"/>
-      <c r="C36" s="145"/>
-      <c r="D36" s="145"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="145"/>
-      <c r="G36" s="145"/>
-      <c r="H36" s="145"/>
-      <c r="I36" s="145"/>
-      <c r="J36" s="145"/>
-      <c r="K36" s="146"/>
+      <c r="A36" s="75"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="81"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="134"/>
-      <c r="Q36" s="135"/>
-      <c r="R36" s="135"/>
-      <c r="S36" s="135"/>
-      <c r="T36" s="135"/>
-      <c r="U36" s="135"/>
-      <c r="V36" s="135"/>
-      <c r="W36" s="136"/>
+      <c r="P36" s="69"/>
+      <c r="Q36" s="70"/>
+      <c r="R36" s="70"/>
+      <c r="S36" s="70"/>
+      <c r="T36" s="70"/>
+      <c r="U36" s="70"/>
+      <c r="V36" s="70"/>
+      <c r="W36" s="71"/>
       <c r="X36" s="13"/>
       <c r="Z36" s="34"/>
       <c r="AA36" s="34"/>
@@ -3904,46 +3914,46 @@
       <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="140"/>
-      <c r="B37" s="147"/>
-      <c r="C37" s="148"/>
-      <c r="D37" s="148"/>
-      <c r="E37" s="148"/>
-      <c r="F37" s="148"/>
-      <c r="G37" s="148"/>
-      <c r="H37" s="148"/>
-      <c r="I37" s="148"/>
-      <c r="J37" s="148"/>
-      <c r="K37" s="149"/>
+      <c r="A37" s="75"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="84"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="137"/>
-      <c r="Q37" s="138"/>
-      <c r="R37" s="138"/>
-      <c r="S37" s="138"/>
-      <c r="T37" s="138"/>
-      <c r="U37" s="138"/>
-      <c r="V37" s="138"/>
-      <c r="W37" s="139"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="73"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="73"/>
+      <c r="V37" s="73"/>
+      <c r="W37" s="74"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="118" t="s">
+      <c r="B38" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="119"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="119"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="119"/>
-      <c r="H38" s="119"/>
-      <c r="I38" s="119"/>
-      <c r="J38" s="119"/>
-      <c r="K38" s="120"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="86"/>
+      <c r="K38" s="87"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3961,36 +3971,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="118" t="s">
+      <c r="B39" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="119"/>
-      <c r="D39" s="119"/>
-      <c r="E39" s="119"/>
-      <c r="F39" s="119"/>
-      <c r="G39" s="119"/>
-      <c r="H39" s="119"/>
-      <c r="I39" s="119"/>
-      <c r="J39" s="119"/>
-      <c r="K39" s="120"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="87"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="118" t="s">
+      <c r="B40" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="119"/>
-      <c r="D40" s="119"/>
-      <c r="E40" s="119"/>
-      <c r="F40" s="119"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="119"/>
-      <c r="I40" s="119"/>
-      <c r="J40" s="119"/>
-      <c r="K40" s="120"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="86"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="86"/>
+      <c r="K40" s="87"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -4009,76 +4019,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="118" t="s">
+      <c r="B41" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="119"/>
-      <c r="D41" s="119"/>
-      <c r="E41" s="119"/>
-      <c r="F41" s="119"/>
-      <c r="G41" s="119"/>
-      <c r="H41" s="119"/>
-      <c r="I41" s="119"/>
-      <c r="J41" s="119"/>
-      <c r="K41" s="120"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="86"/>
+      <c r="H41" s="86"/>
+      <c r="I41" s="86"/>
+      <c r="J41" s="86"/>
+      <c r="K41" s="87"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="121" t="s">
+      <c r="M41" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="122"/>
-      <c r="O41" s="122"/>
-      <c r="P41" s="122"/>
-      <c r="Q41" s="122"/>
-      <c r="R41" s="122"/>
-      <c r="S41" s="122"/>
-      <c r="T41" s="122"/>
-      <c r="U41" s="122"/>
-      <c r="V41" s="122"/>
-      <c r="W41" s="122"/>
-      <c r="X41" s="123"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="54"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="118"/>
-      <c r="C42" s="119"/>
-      <c r="D42" s="119"/>
-      <c r="E42" s="119"/>
-      <c r="F42" s="119"/>
-      <c r="G42" s="119"/>
-      <c r="H42" s="119"/>
-      <c r="I42" s="119"/>
-      <c r="J42" s="119"/>
-      <c r="K42" s="120"/>
+      <c r="B42" s="85"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="86"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="86"/>
+      <c r="J42" s="86"/>
+      <c r="K42" s="87"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="121" t="s">
+      <c r="M42" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="122"/>
-      <c r="O42" s="122"/>
-      <c r="P42" s="122"/>
-      <c r="Q42" s="122"/>
-      <c r="R42" s="122"/>
-      <c r="S42" s="122"/>
-      <c r="T42" s="122"/>
-      <c r="U42" s="122"/>
-      <c r="V42" s="122"/>
-      <c r="W42" s="122"/>
-      <c r="X42" s="123"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="53"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="54"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="118"/>
-      <c r="C43" s="119"/>
-      <c r="D43" s="119"/>
-      <c r="E43" s="119"/>
-      <c r="F43" s="119"/>
-      <c r="G43" s="119"/>
-      <c r="H43" s="119"/>
-      <c r="I43" s="119"/>
-      <c r="J43" s="119"/>
-      <c r="K43" s="120"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
+      <c r="G43" s="86"/>
+      <c r="H43" s="86"/>
+      <c r="I43" s="86"/>
+      <c r="J43" s="86"/>
+      <c r="K43" s="87"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -4096,16 +4106,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="118"/>
-      <c r="C44" s="119"/>
-      <c r="D44" s="119"/>
-      <c r="E44" s="119"/>
-      <c r="F44" s="119"/>
-      <c r="G44" s="119"/>
-      <c r="H44" s="119"/>
-      <c r="I44" s="119"/>
-      <c r="J44" s="119"/>
-      <c r="K44" s="120"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="86"/>
+      <c r="H44" s="86"/>
+      <c r="I44" s="86"/>
+      <c r="J44" s="86"/>
+      <c r="K44" s="87"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -4123,16 +4133,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="118"/>
-      <c r="C45" s="119"/>
-      <c r="D45" s="119"/>
-      <c r="E45" s="119"/>
-      <c r="F45" s="119"/>
-      <c r="G45" s="119"/>
-      <c r="H45" s="119"/>
-      <c r="I45" s="119"/>
-      <c r="J45" s="119"/>
-      <c r="K45" s="120"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="86"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="87"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -4150,16 +4160,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="118"/>
-      <c r="C46" s="119"/>
-      <c r="D46" s="119"/>
-      <c r="E46" s="119"/>
-      <c r="F46" s="119"/>
-      <c r="G46" s="119"/>
-      <c r="H46" s="119"/>
-      <c r="I46" s="119"/>
-      <c r="J46" s="119"/>
-      <c r="K46" s="120"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
+      <c r="G46" s="86"/>
+      <c r="H46" s="86"/>
+      <c r="I46" s="86"/>
+      <c r="J46" s="86"/>
+      <c r="K46" s="87"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -4202,6 +4212,38 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:R10"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="Q19:X19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B42:K42"/>
     <mergeCell ref="M42:X42"/>
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="Q26:X27"/>
@@ -4212,38 +4254,6 @@
     <mergeCell ref="B35:K37"/>
     <mergeCell ref="M41:X41"/>
     <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Y1:Z3"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="Q19:X19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="J9:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4254,10 +4264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4555,6 +4565,11 @@
         <v>131</v>
       </c>
     </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="150" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added smoke next will be explosions got noises and songs explosions next
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -270,15 +270,9 @@
     <t>play test speeds of player and get right numbers</t>
   </si>
   <si>
-    <t>set all tags on boats</t>
-  </si>
-  <si>
     <t>lights need to turn off during day</t>
   </si>
   <si>
-    <t>tactical cam off bow sides</t>
-  </si>
-  <si>
     <t>do green the yellow orange red blue white is it necessary - pink get playtest feed back give them experience of two options</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>setup option attack only humans</t>
   </si>
   <si>
-    <t>stop coroutine fire, stop friendly targetting, stop shooting when an enemy falls</t>
-  </si>
-  <si>
     <t>replace tags sorting layers</t>
   </si>
   <si>
@@ -327,9 +318,6 @@
     <t>angle change of boat or spray as turn or lean so feel the turn</t>
   </si>
   <si>
-    <t>error handler spelling changed with anduino version and uncomment in arduino code - is this why getting odd results at times</t>
-  </si>
-  <si>
     <t>playerscript for ai make ai as similar to player as possible to make more options easier to code so ai has as much shared functionality as possible</t>
   </si>
   <si>
@@ -342,9 +330,6 @@
     <t>android monitor on bike and button to divert power to shooting</t>
   </si>
   <si>
-    <t>sfx</t>
-  </si>
-  <si>
     <t>ram damage ram script and black flags when ai go to ram made</t>
   </si>
   <si>
@@ -360,15 +345,9 @@
     <t>hi graphic and low graphic mode</t>
   </si>
   <si>
-    <t>build</t>
-  </si>
-  <si>
     <t>family mode kid bike and adut bikes drop fdown volt max range</t>
   </si>
   <si>
-    <t>explosion graphic</t>
-  </si>
-  <si>
     <t>do something with team names etc</t>
   </si>
   <si>
@@ -378,36 +357,18 @@
     <t>laptop version to pc</t>
   </si>
   <si>
-    <t>put arduino code into the pedal pirates file - update with new library</t>
-  </si>
-  <si>
     <t>auto find comms preset baud</t>
   </si>
   <si>
-    <t>improve code to arduino so if open then close, then reopen on the open option as with crashes etc stays open we reopen and cause error</t>
-  </si>
-  <si>
     <t>research how to run faster over xmas and tweak on laptop for play</t>
   </si>
   <si>
-    <t>canon ball smoke impact explosion etc</t>
-  </si>
-  <si>
     <t>experiment and read about camera views</t>
   </si>
   <si>
     <t>have playerSetup mode - which is current game mode with selectors for ai behaviour etc, then have noSetup mode which games on maybe specific maps where just pedal to start new game teams preset, have constant play mode with constant spawning and player respawning</t>
   </si>
   <si>
-    <t>its actually really hard to hit so maybe boat damage, sail damage and bow damage will need new strategy for chosing between colliders, cube colliders for each sail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add text 60x for bow damage 4x for hull damage 1x for sail damage and you can fire - if all cannons hit hull that 20 damage or sails 5 </t>
-  </si>
-  <si>
-    <t>teraain thickness and bounce</t>
-  </si>
-  <si>
     <t>on die get rid all colliders inc new box ones</t>
   </si>
   <si>
@@ -420,12 +381,6 @@
     <t>new terrain when do on laptop, no light details etc small get rid all files dont us make it light, try turning off scripts to see what slows it</t>
   </si>
   <si>
-    <t>cannons not stopping firing as count things inand out change to just when triggered with cool down</t>
-  </si>
-  <si>
-    <t>bake nav mesh</t>
-  </si>
-  <si>
     <t>fix gizmo failed jumps</t>
   </si>
   <si>
@@ -439,6 +394,30 @@
   </si>
   <si>
     <t>make sure one version of arduino stuff and arduino works</t>
+  </si>
+  <si>
+    <t>bake nav mesh - for laptop version ensure set terrain not walkable not a navmesh and the tile to one</t>
+  </si>
+  <si>
+    <t>cannons not stopping firing as count things inand out change to just when triggered with cool down - done but not ideal just stops coding so has a check would be better and so doesnt shoot on allies</t>
+  </si>
+  <si>
+    <t>teraain thickness and bounce + physic settings</t>
+  </si>
+  <si>
+    <t>reduce physics sorting and tag layers so efficient replan structure and what does what</t>
+  </si>
+  <si>
+    <t>tactical cam off bow sides OR AT LEAST SO SEE WHOLE OF TRIGGER AREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfx to do this need 1d sound so map is the listner and the sounds are not based on distance and only sounds are made for players dealing or receiving damage. Have a bool that says playercannon ball </t>
+  </si>
+  <si>
+    <t>canon ball impact explosion etc if triggered by a player sets the ball to playerBall maybe rename bool, playersCannonBallOrFiredAtPlayer, make the smoke be created by the cannonballs</t>
+  </si>
+  <si>
+    <t>enemy and players maybe shoot after death!</t>
   </si>
 </sst>
 </file>
@@ -596,7 +575,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,12 +628,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,12 +687,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -727,6 +694,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1408,7 +1381,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1831,7 +1804,6 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -4264,169 +4236,169 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A59"/>
+  <dimension ref="A1:A52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="146.85546875" customWidth="1"/>
+    <col min="1" max="1" width="231.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="42" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" s="41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="42" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" s="42" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="41" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" s="43" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" s="39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="39" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="43" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="43" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="44" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="43" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="42" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="41" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" s="41" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="43" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="42" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" s="43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="42" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" s="44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" s="48" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="50.25" customHeight="1">
+      <c r="A27" s="40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="48" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="49" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="49" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="50" t="s">
+      <c r="A31" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4441,133 +4413,98 @@
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" t="s">
+      <c r="A34" s="47" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" t="s">
+      <c r="A35" s="48" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="43" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" t="s">
+      <c r="A37" s="39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="49" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="47" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="48" t="s">
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="49" t="s">
+    <row r="44" spans="1:1">
+      <c r="A44" s="43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="46" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="40" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="44" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="42" t="s">
+    <row r="47" spans="1:1">
+      <c r="A47" s="51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="43" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="51" t="s">
+    <row r="50" spans="1:1">
+      <c r="A50" s="50" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="42" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="44" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="44" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="44" t="s">
+      <c r="A52" s="50" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="47" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="44" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="39" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="44" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="150" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
frozen cam and gave death image that i should set to fade in and out later, no longer assumes right rect for 1player incase goes mult then single later, reset player setup require gm not to be static which means maybe ps should be reseting itself rather than reloading the scene to do so. havent tested any of it yet
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -264,9 +264,6 @@
     <t>GM - hold info</t>
   </si>
   <si>
-    <t>make rects worked out at the end so if ppl drop out dont get wrong devision of screen</t>
-  </si>
-  <si>
     <t>play test speeds of player and get right numbers</t>
   </si>
   <si>
@@ -399,9 +396,6 @@
     <t>bake nav mesh - for laptop version ensure set terrain not walkable not a navmesh and the tile to one</t>
   </si>
   <si>
-    <t>cannons not stopping firing as count things inand out change to just when triggered with cool down - done but not ideal just stops coding so has a check would be better and so doesnt shoot on allies</t>
-  </si>
-  <si>
     <t>teraain thickness and bounce + physic settings</t>
   </si>
   <si>
@@ -411,13 +405,10 @@
     <t>tactical cam off bow sides OR AT LEAST SO SEE WHOLE OF TRIGGER AREA</t>
   </si>
   <si>
-    <t xml:space="preserve">sfx to do this need 1d sound so map is the listner and the sounds are not based on distance and only sounds are made for players dealing or receiving damage. Have a bool that says playercannon ball </t>
-  </si>
-  <si>
-    <t>canon ball impact explosion etc if triggered by a player sets the ball to playerBall maybe rename bool, playersCannonBallOrFiredAtPlayer, make the smoke be created by the cannonballs</t>
-  </si>
-  <si>
-    <t>enemy and players maybe shoot after death!</t>
+    <t>cannons not stopping firing as count things inand out change to just when triggered with cool down - done but not ideal just stops coding so has a check would be better and so doesnt shoot on allies - think need a raycast to check</t>
+  </si>
+  <si>
+    <t>make the smoke be created by the cannonballs not the cannon</t>
   </si>
 </sst>
 </file>
@@ -575,7 +566,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -628,12 +619,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1381,7 +1366,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1509,7 +1494,213 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1517,15 +1708,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1546,9 +1728,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1608,201 +1787,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2774,14 +2758,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="Y1" s="90" t="s">
+      <c r="Y1" s="87" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="91"/>
+      <c r="Z1" s="88"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="Y2" s="92"/>
-      <c r="Z2" s="93"/>
+      <c r="Y2" s="89"/>
+      <c r="Z2" s="90"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
       <c r="AH2" s="35"/>
@@ -2790,8 +2774,8 @@
       <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="Y3" s="94"/>
-      <c r="Z3" s="95"/>
+      <c r="Y3" s="91"/>
+      <c r="Z3" s="92"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="38" t="s">
         <v>58</v>
@@ -2809,16 +2793,16 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="122"/>
-      <c r="D4" s="123"/>
-      <c r="G4" s="129" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="G4" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="122"/>
-      <c r="I4" s="123"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53"/>
       <c r="Z4" s="34"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
@@ -2832,12 +2816,12 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="130"/>
-      <c r="C5" s="142"/>
-      <c r="D5" s="131"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="142"/>
-      <c r="I5" s="131"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="56"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="56"/>
       <c r="Z5" s="34" t="s">
         <v>50</v>
       </c>
@@ -2879,12 +2863,12 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="144"/>
-      <c r="D7" s="144"/>
-      <c r="E7" s="145"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="59"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -2914,10 +2898,10 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="146"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="147"/>
-      <c r="E8" s="148"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="62"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2954,17 +2938,17 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="129" t="s">
+      <c r="J9" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="122"/>
-      <c r="L9" s="122"/>
-      <c r="M9" s="122"/>
-      <c r="N9" s="122"/>
-      <c r="O9" s="122"/>
-      <c r="P9" s="122"/>
-      <c r="Q9" s="122"/>
-      <c r="R9" s="123"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="53"/>
       <c r="Z9" s="34" t="s">
         <v>69</v>
       </c>
@@ -2992,25 +2976,25 @@
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="149" t="s">
+      <c r="B10" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="149"/>
-      <c r="D10" s="149"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="142"/>
-      <c r="L10" s="142"/>
-      <c r="M10" s="142"/>
-      <c r="N10" s="142"/>
-      <c r="O10" s="142"/>
-      <c r="P10" s="142"/>
-      <c r="Q10" s="142"/>
-      <c r="R10" s="131"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="56"/>
       <c r="Z10" s="34">
         <v>20</v>
       </c>
@@ -3042,10 +3026,10 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="105" t="s">
+      <c r="G11" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="106"/>
+      <c r="H11" s="103"/>
       <c r="I11" s="28"/>
       <c r="Z11" s="34">
         <v>5</v>
@@ -3081,16 +3065,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="107" t="s">
+      <c r="L12" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="108"/>
-      <c r="N12" s="108"/>
-      <c r="O12" s="108"/>
-      <c r="P12" s="108"/>
-      <c r="Q12" s="108"/>
-      <c r="R12" s="108"/>
-      <c r="S12" s="109"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="65"/>
+      <c r="S12" s="104"/>
       <c r="Z12" s="34"/>
       <c r="AA12" s="34"/>
       <c r="AB12" s="34"/>
@@ -3113,14 +3097,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="110"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
-      <c r="O13" s="111"/>
-      <c r="P13" s="111"/>
-      <c r="Q13" s="111"/>
-      <c r="R13" s="111"/>
-      <c r="S13" s="112"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="105"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -3164,16 +3148,16 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="113" t="s">
+      <c r="Q15" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="114"/>
-      <c r="S15" s="114"/>
-      <c r="T15" s="114"/>
-      <c r="U15" s="114"/>
-      <c r="V15" s="114"/>
-      <c r="W15" s="114"/>
-      <c r="X15" s="115"/>
+      <c r="R15" s="107"/>
+      <c r="S15" s="107"/>
+      <c r="T15" s="107"/>
+      <c r="U15" s="107"/>
+      <c r="V15" s="107"/>
+      <c r="W15" s="107"/>
+      <c r="X15" s="108"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -3191,19 +3175,19 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="122" t="s">
+      <c r="M16" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="122"/>
-      <c r="O16" s="123"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="117"/>
-      <c r="S16" s="117"/>
-      <c r="T16" s="117"/>
-      <c r="U16" s="117"/>
-      <c r="V16" s="117"/>
-      <c r="W16" s="117"/>
-      <c r="X16" s="118"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="53"/>
+      <c r="Q16" s="109"/>
+      <c r="R16" s="110"/>
+      <c r="S16" s="110"/>
+      <c r="T16" s="110"/>
+      <c r="U16" s="110"/>
+      <c r="V16" s="110"/>
+      <c r="W16" s="110"/>
+      <c r="X16" s="111"/>
       <c r="Z16" s="34"/>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
@@ -3217,31 +3201,31 @@
       <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="108"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="126" t="s">
+      <c r="E17" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="127"/>
-      <c r="G17" s="128"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="124"/>
-      <c r="N17" s="124"/>
-      <c r="O17" s="125"/>
-      <c r="Q17" s="119"/>
-      <c r="R17" s="120"/>
-      <c r="S17" s="120"/>
-      <c r="T17" s="120"/>
-      <c r="U17" s="120"/>
-      <c r="V17" s="120"/>
-      <c r="W17" s="120"/>
-      <c r="X17" s="121"/>
+      <c r="M17" s="115"/>
+      <c r="N17" s="115"/>
+      <c r="O17" s="116"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="113"/>
+      <c r="S17" s="113"/>
+      <c r="T17" s="113"/>
+      <c r="U17" s="113"/>
+      <c r="V17" s="113"/>
+      <c r="W17" s="113"/>
+      <c r="X17" s="114"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -3255,18 +3239,18 @@
       <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="110"/>
-      <c r="C18" s="111"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="67"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="88" t="s">
+      <c r="L18" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="89"/>
+      <c r="M18" s="72"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3291,32 +3275,32 @@
       <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="129" t="s">
+      <c r="B19" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="123"/>
+      <c r="C19" s="53"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="88"/>
-      <c r="M19" s="89"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="132" t="s">
+      <c r="Q19" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="133"/>
-      <c r="S19" s="133"/>
-      <c r="T19" s="133"/>
-      <c r="U19" s="133"/>
-      <c r="V19" s="133"/>
-      <c r="W19" s="133"/>
-      <c r="X19" s="134"/>
+      <c r="R19" s="74"/>
+      <c r="S19" s="74"/>
+      <c r="T19" s="74"/>
+      <c r="U19" s="74"/>
+      <c r="V19" s="74"/>
+      <c r="W19" s="74"/>
+      <c r="X19" s="75"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -3330,32 +3314,32 @@
       <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="130"/>
-      <c r="C20" s="131"/>
-      <c r="F20" s="135" t="s">
+      <c r="B20" s="54"/>
+      <c r="C20" s="56"/>
+      <c r="F20" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="136"/>
+      <c r="G20" s="77"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="88" t="s">
+      <c r="L20" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="89"/>
+      <c r="M20" s="72"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="55" t="s">
+      <c r="Q20" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="64"/>
+      <c r="R20" s="81"/>
+      <c r="S20" s="81"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="81"/>
+      <c r="V20" s="81"/>
+      <c r="W20" s="81"/>
+      <c r="X20" s="82"/>
       <c r="Z20" s="34"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
@@ -3372,28 +3356,28 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="138"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="79"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="89"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="72"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="139" t="s">
+      <c r="Q21" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="140"/>
-      <c r="S21" s="140"/>
-      <c r="T21" s="140"/>
-      <c r="U21" s="140"/>
-      <c r="V21" s="140"/>
-      <c r="W21" s="140"/>
-      <c r="X21" s="141"/>
+      <c r="R21" s="84"/>
+      <c r="S21" s="84"/>
+      <c r="T21" s="84"/>
+      <c r="U21" s="84"/>
+      <c r="V21" s="84"/>
+      <c r="W21" s="84"/>
+      <c r="X21" s="85"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -3411,10 +3395,10 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="88" t="s">
+      <c r="L22" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="89"/>
+      <c r="M22" s="72"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -3434,28 +3418,28 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="57"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="86"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="88"/>
-      <c r="M23" s="89"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="72"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="96" t="s">
+      <c r="Q23" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="97"/>
-      <c r="S23" s="97"/>
-      <c r="T23" s="97"/>
-      <c r="U23" s="97"/>
-      <c r="V23" s="97"/>
-      <c r="W23" s="97"/>
-      <c r="X23" s="98"/>
+      <c r="R23" s="94"/>
+      <c r="S23" s="94"/>
+      <c r="T23" s="94"/>
+      <c r="U23" s="94"/>
+      <c r="V23" s="94"/>
+      <c r="W23" s="94"/>
+      <c r="X23" s="95"/>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
@@ -3473,20 +3457,20 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="88" t="s">
+      <c r="L24" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="89"/>
+      <c r="M24" s="72"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="99"/>
-      <c r="R24" s="100"/>
-      <c r="S24" s="100"/>
-      <c r="T24" s="100"/>
-      <c r="U24" s="100"/>
-      <c r="V24" s="100"/>
-      <c r="W24" s="100"/>
-      <c r="X24" s="101"/>
+      <c r="Q24" s="96"/>
+      <c r="R24" s="97"/>
+      <c r="S24" s="97"/>
+      <c r="T24" s="97"/>
+      <c r="U24" s="97"/>
+      <c r="V24" s="97"/>
+      <c r="W24" s="97"/>
+      <c r="X24" s="98"/>
       <c r="Z24" s="34"/>
       <c r="AA24" s="34"/>
       <c r="AB24" s="34"/>
@@ -3504,18 +3488,18 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="88"/>
-      <c r="M25" s="89"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="72"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="102"/>
-      <c r="R25" s="103"/>
-      <c r="S25" s="103"/>
-      <c r="T25" s="103"/>
-      <c r="U25" s="103"/>
-      <c r="V25" s="103"/>
-      <c r="W25" s="103"/>
-      <c r="X25" s="104"/>
+      <c r="Q25" s="99"/>
+      <c r="R25" s="100"/>
+      <c r="S25" s="100"/>
+      <c r="T25" s="100"/>
+      <c r="U25" s="100"/>
+      <c r="V25" s="100"/>
+      <c r="W25" s="100"/>
+      <c r="X25" s="101"/>
       <c r="Z25" s="34"/>
       <c r="AA25" s="34"/>
       <c r="AB25" s="34"/>
@@ -3532,26 +3516,26 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="57"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="81"/>
+      <c r="J26" s="81"/>
+      <c r="K26" s="86"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="58" t="s">
+      <c r="Q26" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59"/>
-      <c r="T26" s="59"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="59"/>
-      <c r="W26" s="59"/>
-      <c r="X26" s="60"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="124"/>
+      <c r="T26" s="124"/>
+      <c r="U26" s="124"/>
+      <c r="V26" s="124"/>
+      <c r="W26" s="124"/>
+      <c r="X26" s="125"/>
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
       <c r="AB26" s="34"/>
@@ -3567,14 +3551,14 @@
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="62"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="62"/>
-      <c r="V27" s="62"/>
-      <c r="W27" s="62"/>
-      <c r="X27" s="63"/>
+      <c r="Q27" s="126"/>
+      <c r="R27" s="127"/>
+      <c r="S27" s="127"/>
+      <c r="T27" s="127"/>
+      <c r="U27" s="127"/>
+      <c r="V27" s="127"/>
+      <c r="W27" s="127"/>
+      <c r="X27" s="128"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -3608,16 +3592,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="55" t="s">
+      <c r="Q29" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
-      <c r="X29" s="64"/>
+      <c r="R29" s="81"/>
+      <c r="S29" s="81"/>
+      <c r="T29" s="81"/>
+      <c r="U29" s="81"/>
+      <c r="V29" s="81"/>
+      <c r="W29" s="81"/>
+      <c r="X29" s="82"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -3658,32 +3642,32 @@
       <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
+      <c r="E31" s="129"/>
+      <c r="F31" s="129"/>
+      <c r="G31" s="129"/>
+      <c r="H31" s="129"/>
+      <c r="I31" s="129"/>
+      <c r="J31" s="129"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="66" t="s">
+      <c r="P31" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="67"/>
-      <c r="S31" s="67"/>
-      <c r="T31" s="67"/>
-      <c r="U31" s="67"/>
-      <c r="V31" s="67"/>
-      <c r="W31" s="68"/>
+      <c r="Q31" s="131"/>
+      <c r="R31" s="131"/>
+      <c r="S31" s="131"/>
+      <c r="T31" s="131"/>
+      <c r="U31" s="131"/>
+      <c r="V31" s="131"/>
+      <c r="W31" s="132"/>
       <c r="X31" s="13"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
@@ -3698,28 +3682,28 @@
       <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="65"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
+      <c r="A32" s="129"/>
+      <c r="B32" s="129"/>
+      <c r="C32" s="129"/>
+      <c r="D32" s="129"/>
+      <c r="E32" s="129"/>
+      <c r="F32" s="129"/>
+      <c r="G32" s="129"/>
+      <c r="H32" s="129"/>
+      <c r="I32" s="129"/>
+      <c r="J32" s="129"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="70"/>
-      <c r="R32" s="70"/>
-      <c r="S32" s="70"/>
-      <c r="T32" s="70"/>
-      <c r="U32" s="70"/>
-      <c r="V32" s="70"/>
-      <c r="W32" s="71"/>
+      <c r="P32" s="133"/>
+      <c r="Q32" s="134"/>
+      <c r="R32" s="134"/>
+      <c r="S32" s="134"/>
+      <c r="T32" s="134"/>
+      <c r="U32" s="134"/>
+      <c r="V32" s="134"/>
+      <c r="W32" s="135"/>
       <c r="X32" s="13"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
@@ -3748,14 +3732,14 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="70"/>
-      <c r="R33" s="70"/>
-      <c r="S33" s="70"/>
-      <c r="T33" s="70"/>
-      <c r="U33" s="70"/>
-      <c r="V33" s="70"/>
-      <c r="W33" s="71"/>
+      <c r="P33" s="133"/>
+      <c r="Q33" s="134"/>
+      <c r="R33" s="134"/>
+      <c r="S33" s="134"/>
+      <c r="T33" s="134"/>
+      <c r="U33" s="134"/>
+      <c r="V33" s="134"/>
+      <c r="W33" s="135"/>
       <c r="X33" s="13"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="34"/>
@@ -3773,29 +3757,29 @@
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="75" t="s">
+      <c r="B34" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
+      <c r="C34" s="139"/>
+      <c r="D34" s="139"/>
+      <c r="E34" s="139"/>
+      <c r="F34" s="139"/>
+      <c r="G34" s="139"/>
+      <c r="H34" s="139"/>
+      <c r="I34" s="139"/>
+      <c r="J34" s="139"/>
+      <c r="K34" s="139"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="70"/>
-      <c r="T34" s="70"/>
-      <c r="U34" s="70"/>
-      <c r="V34" s="70"/>
-      <c r="W34" s="71"/>
+      <c r="P34" s="133"/>
+      <c r="Q34" s="134"/>
+      <c r="R34" s="134"/>
+      <c r="S34" s="134"/>
+      <c r="T34" s="134"/>
+      <c r="U34" s="134"/>
+      <c r="V34" s="134"/>
+      <c r="W34" s="135"/>
       <c r="X34" s="13"/>
       <c r="Z34" s="34"/>
       <c r="AA34" s="34"/>
@@ -3810,32 +3794,32 @@
       <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="75" t="s">
+      <c r="A35" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="76" t="s">
+      <c r="B35" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="78"/>
+      <c r="C35" s="141"/>
+      <c r="D35" s="141"/>
+      <c r="E35" s="141"/>
+      <c r="F35" s="141"/>
+      <c r="G35" s="141"/>
+      <c r="H35" s="141"/>
+      <c r="I35" s="141"/>
+      <c r="J35" s="141"/>
+      <c r="K35" s="142"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="70"/>
-      <c r="R35" s="70"/>
-      <c r="S35" s="70"/>
-      <c r="T35" s="70"/>
-      <c r="U35" s="70"/>
-      <c r="V35" s="70"/>
-      <c r="W35" s="71"/>
+      <c r="P35" s="133"/>
+      <c r="Q35" s="134"/>
+      <c r="R35" s="134"/>
+      <c r="S35" s="134"/>
+      <c r="T35" s="134"/>
+      <c r="U35" s="134"/>
+      <c r="V35" s="134"/>
+      <c r="W35" s="135"/>
       <c r="X35" s="13"/>
       <c r="Z35" s="34"/>
       <c r="AA35" s="34"/>
@@ -3850,28 +3834,28 @@
       <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="75"/>
-      <c r="B36" s="79"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="80"/>
-      <c r="F36" s="80"/>
-      <c r="G36" s="80"/>
-      <c r="H36" s="80"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="81"/>
+      <c r="A36" s="139"/>
+      <c r="B36" s="143"/>
+      <c r="C36" s="144"/>
+      <c r="D36" s="144"/>
+      <c r="E36" s="144"/>
+      <c r="F36" s="144"/>
+      <c r="G36" s="144"/>
+      <c r="H36" s="144"/>
+      <c r="I36" s="144"/>
+      <c r="J36" s="144"/>
+      <c r="K36" s="145"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="69"/>
-      <c r="Q36" s="70"/>
-      <c r="R36" s="70"/>
-      <c r="S36" s="70"/>
-      <c r="T36" s="70"/>
-      <c r="U36" s="70"/>
-      <c r="V36" s="70"/>
-      <c r="W36" s="71"/>
+      <c r="P36" s="133"/>
+      <c r="Q36" s="134"/>
+      <c r="R36" s="134"/>
+      <c r="S36" s="134"/>
+      <c r="T36" s="134"/>
+      <c r="U36" s="134"/>
+      <c r="V36" s="134"/>
+      <c r="W36" s="135"/>
       <c r="X36" s="13"/>
       <c r="Z36" s="34"/>
       <c r="AA36" s="34"/>
@@ -3886,46 +3870,46 @@
       <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="75"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="84"/>
+      <c r="A37" s="139"/>
+      <c r="B37" s="146"/>
+      <c r="C37" s="147"/>
+      <c r="D37" s="147"/>
+      <c r="E37" s="147"/>
+      <c r="F37" s="147"/>
+      <c r="G37" s="147"/>
+      <c r="H37" s="147"/>
+      <c r="I37" s="147"/>
+      <c r="J37" s="147"/>
+      <c r="K37" s="148"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="73"/>
-      <c r="R37" s="73"/>
-      <c r="S37" s="73"/>
-      <c r="T37" s="73"/>
-      <c r="U37" s="73"/>
-      <c r="V37" s="73"/>
-      <c r="W37" s="74"/>
+      <c r="P37" s="136"/>
+      <c r="Q37" s="137"/>
+      <c r="R37" s="137"/>
+      <c r="S37" s="137"/>
+      <c r="T37" s="137"/>
+      <c r="U37" s="137"/>
+      <c r="V37" s="137"/>
+      <c r="W37" s="138"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="85" t="s">
+      <c r="B38" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="87"/>
+      <c r="C38" s="118"/>
+      <c r="D38" s="118"/>
+      <c r="E38" s="118"/>
+      <c r="F38" s="118"/>
+      <c r="G38" s="118"/>
+      <c r="H38" s="118"/>
+      <c r="I38" s="118"/>
+      <c r="J38" s="118"/>
+      <c r="K38" s="119"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3943,36 +3927,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="85" t="s">
+      <c r="B39" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="86"/>
-      <c r="D39" s="86"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="86"/>
-      <c r="H39" s="86"/>
-      <c r="I39" s="86"/>
-      <c r="J39" s="86"/>
-      <c r="K39" s="87"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="118"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="118"/>
+      <c r="H39" s="118"/>
+      <c r="I39" s="118"/>
+      <c r="J39" s="118"/>
+      <c r="K39" s="119"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="85" t="s">
+      <c r="B40" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
-      <c r="H40" s="86"/>
-      <c r="I40" s="86"/>
-      <c r="J40" s="86"/>
-      <c r="K40" s="87"/>
+      <c r="C40" s="118"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
+      <c r="F40" s="118"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="118"/>
+      <c r="I40" s="118"/>
+      <c r="J40" s="118"/>
+      <c r="K40" s="119"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -3991,76 +3975,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="85" t="s">
+      <c r="B41" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="86"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="87"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="118"/>
+      <c r="F41" s="118"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="118"/>
+      <c r="I41" s="118"/>
+      <c r="J41" s="118"/>
+      <c r="K41" s="119"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="52" t="s">
+      <c r="M41" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="53"/>
-      <c r="O41" s="53"/>
-      <c r="P41" s="53"/>
-      <c r="Q41" s="53"/>
-      <c r="R41" s="53"/>
-      <c r="S41" s="53"/>
-      <c r="T41" s="53"/>
-      <c r="U41" s="53"/>
-      <c r="V41" s="53"/>
-      <c r="W41" s="53"/>
-      <c r="X41" s="54"/>
+      <c r="N41" s="121"/>
+      <c r="O41" s="121"/>
+      <c r="P41" s="121"/>
+      <c r="Q41" s="121"/>
+      <c r="R41" s="121"/>
+      <c r="S41" s="121"/>
+      <c r="T41" s="121"/>
+      <c r="U41" s="121"/>
+      <c r="V41" s="121"/>
+      <c r="W41" s="121"/>
+      <c r="X41" s="122"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="85"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
-      <c r="E42" s="86"/>
-      <c r="F42" s="86"/>
-      <c r="G42" s="86"/>
-      <c r="H42" s="86"/>
-      <c r="I42" s="86"/>
-      <c r="J42" s="86"/>
-      <c r="K42" s="87"/>
+      <c r="B42" s="117"/>
+      <c r="C42" s="118"/>
+      <c r="D42" s="118"/>
+      <c r="E42" s="118"/>
+      <c r="F42" s="118"/>
+      <c r="G42" s="118"/>
+      <c r="H42" s="118"/>
+      <c r="I42" s="118"/>
+      <c r="J42" s="118"/>
+      <c r="K42" s="119"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="52" t="s">
+      <c r="M42" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="53"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
-      <c r="U42" s="53"/>
-      <c r="V42" s="53"/>
-      <c r="W42" s="53"/>
-      <c r="X42" s="54"/>
+      <c r="N42" s="121"/>
+      <c r="O42" s="121"/>
+      <c r="P42" s="121"/>
+      <c r="Q42" s="121"/>
+      <c r="R42" s="121"/>
+      <c r="S42" s="121"/>
+      <c r="T42" s="121"/>
+      <c r="U42" s="121"/>
+      <c r="V42" s="121"/>
+      <c r="W42" s="121"/>
+      <c r="X42" s="122"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="85"/>
-      <c r="C43" s="86"/>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="86"/>
-      <c r="G43" s="86"/>
-      <c r="H43" s="86"/>
-      <c r="I43" s="86"/>
-      <c r="J43" s="86"/>
-      <c r="K43" s="87"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="118"/>
+      <c r="D43" s="118"/>
+      <c r="E43" s="118"/>
+      <c r="F43" s="118"/>
+      <c r="G43" s="118"/>
+      <c r="H43" s="118"/>
+      <c r="I43" s="118"/>
+      <c r="J43" s="118"/>
+      <c r="K43" s="119"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -4078,16 +4062,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="85"/>
-      <c r="C44" s="86"/>
-      <c r="D44" s="86"/>
-      <c r="E44" s="86"/>
-      <c r="F44" s="86"/>
-      <c r="G44" s="86"/>
-      <c r="H44" s="86"/>
-      <c r="I44" s="86"/>
-      <c r="J44" s="86"/>
-      <c r="K44" s="87"/>
+      <c r="B44" s="117"/>
+      <c r="C44" s="118"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="118"/>
+      <c r="I44" s="118"/>
+      <c r="J44" s="118"/>
+      <c r="K44" s="119"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -4105,16 +4089,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="85"/>
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
-      <c r="E45" s="86"/>
-      <c r="F45" s="86"/>
-      <c r="G45" s="86"/>
-      <c r="H45" s="86"/>
-      <c r="I45" s="86"/>
-      <c r="J45" s="86"/>
-      <c r="K45" s="87"/>
+      <c r="B45" s="117"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="118"/>
+      <c r="I45" s="118"/>
+      <c r="J45" s="118"/>
+      <c r="K45" s="119"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -4132,16 +4116,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="85"/>
-      <c r="C46" s="86"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="86"/>
-      <c r="G46" s="86"/>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-      <c r="J46" s="86"/>
-      <c r="K46" s="87"/>
+      <c r="B46" s="117"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="118"/>
+      <c r="I46" s="118"/>
+      <c r="J46" s="118"/>
+      <c r="K46" s="119"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -4184,38 +4168,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="J9:R10"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="Q19:X19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Y1:Z3"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
-    <mergeCell ref="B42:K42"/>
     <mergeCell ref="M42:X42"/>
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="Q26:X27"/>
@@ -4226,6 +4178,38 @@
     <mergeCell ref="B35:K37"/>
     <mergeCell ref="M41:X41"/>
     <mergeCell ref="B34:K34"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="Q19:X19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4236,10 +4220,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A52"/>
+  <dimension ref="A1:A49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4249,46 +4233,46 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="40" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="43" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="45" t="s">
-        <v>122</v>
-      </c>
-    </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="41" t="s">
+      <c r="A6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="A7" s="40" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="41" t="s">
+      <c r="A8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" t="s">
+      <c r="A9" s="41" t="s">
         <v>81</v>
       </c>
     </row>
@@ -4298,17 +4282,17 @@
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="43" t="s">
-        <v>83</v>
+      <c r="A11" s="39" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="39" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="39" t="s">
+      <c r="A13" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4323,188 +4307,173 @@
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" t="s">
+      <c r="A16" s="41" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="40" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="40" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="A20" s="42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="43" t="s">
-        <v>104</v>
-      </c>
-    </row>
     <row r="22" spans="1:1">
-      <c r="A22" t="s">
+      <c r="A22" s="43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="47" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="44" t="s">
-        <v>99</v>
-      </c>
-    </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="47" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="48" t="s">
+      <c r="A25" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" t="s">
+      <c r="A26" s="47" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="50.25" customHeight="1">
-      <c r="A27" s="40" t="s">
-        <v>123</v>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="48" t="s">
-        <v>96</v>
+      <c r="A28" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>101</v>
+      <c r="A32" s="46" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>102</v>
+      <c r="A33" s="47" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="47" t="s">
-        <v>103</v>
+      <c r="A34" s="42" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="48" t="s">
-        <v>105</v>
+      <c r="A35" s="41" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="48" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="39" t="s">
-        <v>124</v>
+      <c r="A37" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="49" t="s">
-        <v>107</v>
+      <c r="A38" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>108</v>
+      <c r="A39" s="39" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="39" t="s">
-        <v>120</v>
+      <c r="A41" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>109</v>
+      <c r="A42" s="42" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>110</v>
+      <c r="A43" s="42" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="43" t="s">
-        <v>111</v>
+      <c r="A44" s="45" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="43" t="s">
-        <v>112</v>
+      <c r="A45" s="50" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="46" t="s">
-        <v>113</v>
+      <c r="A46" s="39" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="51" t="s">
+      <c r="A47" s="41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="39" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="43" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="50" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="50" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dont have water splash but the jmparted fire looks great lots of particle systems though
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="120">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -288,12 +288,6 @@
     <t>box around drop boxes and tick box or colour code panel behind so clear what tick box for</t>
   </si>
   <si>
-    <t>on death top down view or and pirate flag over screen</t>
-  </si>
-  <si>
-    <t>reset the setup if everyone drops out</t>
-  </si>
-  <si>
     <t>player prefs so that can skip team set up stage and set max</t>
   </si>
   <si>
@@ -306,9 +300,6 @@
     <t>daycycle starts at game start</t>
   </si>
   <si>
-    <t>check max bar working properly saught text</t>
-  </si>
-  <si>
     <t>read through notes made so far in notes document</t>
   </si>
   <si>
@@ -384,9 +375,6 @@
     <t>addindicator strip for deal damage e.g. Flag flashes red with bow hit or just leave a fire particle effect</t>
   </si>
   <si>
-    <t>reset the thisplayersetting not sure worked</t>
-  </si>
-  <si>
     <t>try seperating all my ai attack pattern script from the original ai one and just feed the transform to it</t>
   </si>
   <si>
@@ -409,6 +397,9 @@
   </si>
   <si>
     <t>make the smoke be created by the cannonballs not the cannon</t>
+  </si>
+  <si>
+    <t>check max bar working properly saught text - pretty certain theyre not setting the maxes to anything but default</t>
   </si>
 </sst>
 </file>
@@ -1494,22 +1485,277 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1532,261 +1778,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="41" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="40" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2758,14 +2749,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="Y1" s="87" t="s">
+      <c r="Y1" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="88"/>
+      <c r="Z1" s="90"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="90"/>
+      <c r="Y2" s="91"/>
+      <c r="Z2" s="92"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
       <c r="AH2" s="35"/>
@@ -2774,8 +2765,8 @@
       <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="Y3" s="91"/>
-      <c r="Z3" s="92"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="94"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="38" t="s">
         <v>58</v>
@@ -2793,16 +2784,16 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="53"/>
-      <c r="G4" s="51" t="s">
+      <c r="C4" s="121"/>
+      <c r="D4" s="122"/>
+      <c r="G4" s="128" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="52"/>
-      <c r="I4" s="53"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="122"/>
       <c r="Z4" s="34"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
@@ -2816,12 +2807,12 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="54"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="56"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="130"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="130"/>
       <c r="Z5" s="34" t="s">
         <v>50</v>
       </c>
@@ -2863,12 +2854,12 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="59"/>
+      <c r="C7" s="143"/>
+      <c r="D7" s="143"/>
+      <c r="E7" s="144"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -2898,10 +2889,10 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="60"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="62"/>
+      <c r="B8" s="145"/>
+      <c r="C8" s="146"/>
+      <c r="D8" s="146"/>
+      <c r="E8" s="147"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2938,17 +2929,17 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="51" t="s">
+      <c r="J9" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="53"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="121"/>
+      <c r="R9" s="122"/>
       <c r="Z9" s="34" t="s">
         <v>69</v>
       </c>
@@ -2976,25 +2967,25 @@
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
+      <c r="C10" s="148"/>
+      <c r="D10" s="148"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="56"/>
+      <c r="J10" s="129"/>
+      <c r="K10" s="141"/>
+      <c r="L10" s="141"/>
+      <c r="M10" s="141"/>
+      <c r="N10" s="141"/>
+      <c r="O10" s="141"/>
+      <c r="P10" s="141"/>
+      <c r="Q10" s="141"/>
+      <c r="R10" s="130"/>
       <c r="Z10" s="34">
         <v>20</v>
       </c>
@@ -3026,10 +3017,10 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="102" t="s">
+      <c r="G11" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="103"/>
+      <c r="H11" s="105"/>
       <c r="I11" s="28"/>
       <c r="Z11" s="34">
         <v>5</v>
@@ -3065,16 +3056,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="64" t="s">
+      <c r="L12" s="106" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="65"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="104"/>
+      <c r="M12" s="107"/>
+      <c r="N12" s="107"/>
+      <c r="O12" s="107"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="107"/>
+      <c r="S12" s="108"/>
       <c r="Z12" s="34"/>
       <c r="AA12" s="34"/>
       <c r="AB12" s="34"/>
@@ -3097,14 +3088,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
-      <c r="O13" s="67"/>
-      <c r="P13" s="67"/>
-      <c r="Q13" s="67"/>
-      <c r="R13" s="67"/>
-      <c r="S13" s="105"/>
+      <c r="L13" s="109"/>
+      <c r="M13" s="110"/>
+      <c r="N13" s="110"/>
+      <c r="O13" s="110"/>
+      <c r="P13" s="110"/>
+      <c r="Q13" s="110"/>
+      <c r="R13" s="110"/>
+      <c r="S13" s="111"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -3148,16 +3139,16 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="106" t="s">
+      <c r="Q15" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107"/>
-      <c r="U15" s="107"/>
-      <c r="V15" s="107"/>
-      <c r="W15" s="107"/>
-      <c r="X15" s="108"/>
+      <c r="R15" s="113"/>
+      <c r="S15" s="113"/>
+      <c r="T15" s="113"/>
+      <c r="U15" s="113"/>
+      <c r="V15" s="113"/>
+      <c r="W15" s="113"/>
+      <c r="X15" s="114"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -3175,19 +3166,19 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="52" t="s">
+      <c r="M16" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="52"/>
-      <c r="O16" s="53"/>
-      <c r="Q16" s="109"/>
-      <c r="R16" s="110"/>
-      <c r="S16" s="110"/>
-      <c r="T16" s="110"/>
-      <c r="U16" s="110"/>
-      <c r="V16" s="110"/>
-      <c r="W16" s="110"/>
-      <c r="X16" s="111"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="122"/>
+      <c r="Q16" s="115"/>
+      <c r="R16" s="116"/>
+      <c r="S16" s="116"/>
+      <c r="T16" s="116"/>
+      <c r="U16" s="116"/>
+      <c r="V16" s="116"/>
+      <c r="W16" s="116"/>
+      <c r="X16" s="117"/>
       <c r="Z16" s="34"/>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
@@ -3201,31 +3192,31 @@
       <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="65"/>
+      <c r="C17" s="107"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="68" t="s">
+      <c r="E17" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="127"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="115"/>
-      <c r="N17" s="115"/>
-      <c r="O17" s="116"/>
-      <c r="Q17" s="112"/>
-      <c r="R17" s="113"/>
-      <c r="S17" s="113"/>
-      <c r="T17" s="113"/>
-      <c r="U17" s="113"/>
-      <c r="V17" s="113"/>
-      <c r="W17" s="113"/>
-      <c r="X17" s="114"/>
+      <c r="M17" s="123"/>
+      <c r="N17" s="123"/>
+      <c r="O17" s="124"/>
+      <c r="Q17" s="118"/>
+      <c r="R17" s="119"/>
+      <c r="S17" s="119"/>
+      <c r="T17" s="119"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="119"/>
+      <c r="W17" s="119"/>
+      <c r="X17" s="120"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -3239,18 +3230,18 @@
       <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="66"/>
-      <c r="C18" s="67"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="110"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="71" t="s">
+      <c r="L18" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="72"/>
+      <c r="M18" s="88"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3275,32 +3266,32 @@
       <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="53"/>
+      <c r="C19" s="122"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="72"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="88"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="73" t="s">
+      <c r="Q19" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="74"/>
-      <c r="S19" s="74"/>
-      <c r="T19" s="74"/>
-      <c r="U19" s="74"/>
-      <c r="V19" s="74"/>
-      <c r="W19" s="74"/>
-      <c r="X19" s="75"/>
+      <c r="R19" s="132"/>
+      <c r="S19" s="132"/>
+      <c r="T19" s="132"/>
+      <c r="U19" s="132"/>
+      <c r="V19" s="132"/>
+      <c r="W19" s="132"/>
+      <c r="X19" s="133"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -3314,32 +3305,32 @@
       <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="54"/>
-      <c r="C20" s="56"/>
-      <c r="F20" s="76" t="s">
+      <c r="B20" s="129"/>
+      <c r="C20" s="130"/>
+      <c r="F20" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="77"/>
+      <c r="G20" s="135"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="71" t="s">
+      <c r="L20" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="72"/>
+      <c r="M20" s="88"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="80" t="s">
+      <c r="Q20" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="81"/>
-      <c r="S20" s="81"/>
-      <c r="T20" s="81"/>
-      <c r="U20" s="81"/>
-      <c r="V20" s="81"/>
-      <c r="W20" s="81"/>
-      <c r="X20" s="82"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
+      <c r="T20" s="55"/>
+      <c r="U20" s="55"/>
+      <c r="V20" s="55"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="63"/>
       <c r="Z20" s="34"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
@@ -3356,28 +3347,28 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="79"/>
+      <c r="F21" s="136"/>
+      <c r="G21" s="137"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="72"/>
+      <c r="L21" s="87"/>
+      <c r="M21" s="88"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="83" t="s">
+      <c r="Q21" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="84"/>
-      <c r="S21" s="84"/>
-      <c r="T21" s="84"/>
-      <c r="U21" s="84"/>
-      <c r="V21" s="84"/>
-      <c r="W21" s="84"/>
-      <c r="X21" s="85"/>
+      <c r="R21" s="139"/>
+      <c r="S21" s="139"/>
+      <c r="T21" s="139"/>
+      <c r="U21" s="139"/>
+      <c r="V21" s="139"/>
+      <c r="W21" s="139"/>
+      <c r="X21" s="140"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -3395,10 +3386,10 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="71" t="s">
+      <c r="L22" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="72"/>
+      <c r="M22" s="88"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -3418,28 +3409,28 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="80" t="s">
+      <c r="E23" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="81"/>
-      <c r="G23" s="86"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="56"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="71"/>
-      <c r="M23" s="72"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="88"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="93" t="s">
+      <c r="Q23" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="94"/>
-      <c r="S23" s="94"/>
-      <c r="T23" s="94"/>
-      <c r="U23" s="94"/>
-      <c r="V23" s="94"/>
-      <c r="W23" s="94"/>
-      <c r="X23" s="95"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="96"/>
+      <c r="T23" s="96"/>
+      <c r="U23" s="96"/>
+      <c r="V23" s="96"/>
+      <c r="W23" s="96"/>
+      <c r="X23" s="97"/>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
@@ -3457,20 +3448,20 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="71" t="s">
+      <c r="L24" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="72"/>
+      <c r="M24" s="88"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="96"/>
-      <c r="R24" s="97"/>
-      <c r="S24" s="97"/>
-      <c r="T24" s="97"/>
-      <c r="U24" s="97"/>
-      <c r="V24" s="97"/>
-      <c r="W24" s="97"/>
-      <c r="X24" s="98"/>
+      <c r="Q24" s="98"/>
+      <c r="R24" s="99"/>
+      <c r="S24" s="99"/>
+      <c r="T24" s="99"/>
+      <c r="U24" s="99"/>
+      <c r="V24" s="99"/>
+      <c r="W24" s="99"/>
+      <c r="X24" s="100"/>
       <c r="Z24" s="34"/>
       <c r="AA24" s="34"/>
       <c r="AB24" s="34"/>
@@ -3488,18 +3479,18 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="71"/>
-      <c r="M25" s="72"/>
+      <c r="L25" s="87"/>
+      <c r="M25" s="88"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="99"/>
-      <c r="R25" s="100"/>
-      <c r="S25" s="100"/>
-      <c r="T25" s="100"/>
-      <c r="U25" s="100"/>
-      <c r="V25" s="100"/>
-      <c r="W25" s="100"/>
-      <c r="X25" s="101"/>
+      <c r="Q25" s="101"/>
+      <c r="R25" s="102"/>
+      <c r="S25" s="102"/>
+      <c r="T25" s="102"/>
+      <c r="U25" s="102"/>
+      <c r="V25" s="102"/>
+      <c r="W25" s="102"/>
+      <c r="X25" s="103"/>
       <c r="Z25" s="34"/>
       <c r="AA25" s="34"/>
       <c r="AB25" s="34"/>
@@ -3516,26 +3507,26 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="80"/>
-      <c r="I26" s="81"/>
-      <c r="J26" s="81"/>
-      <c r="K26" s="86"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="56"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="123" t="s">
+      <c r="Q26" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="124"/>
-      <c r="S26" s="124"/>
-      <c r="T26" s="124"/>
-      <c r="U26" s="124"/>
-      <c r="V26" s="124"/>
-      <c r="W26" s="124"/>
-      <c r="X26" s="125"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="59"/>
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
       <c r="AB26" s="34"/>
@@ -3551,14 +3542,14 @@
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="126"/>
-      <c r="R27" s="127"/>
-      <c r="S27" s="127"/>
-      <c r="T27" s="127"/>
-      <c r="U27" s="127"/>
-      <c r="V27" s="127"/>
-      <c r="W27" s="127"/>
-      <c r="X27" s="128"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="61"/>
+      <c r="U27" s="61"/>
+      <c r="V27" s="61"/>
+      <c r="W27" s="61"/>
+      <c r="X27" s="62"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -3592,16 +3583,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="80" t="s">
+      <c r="Q29" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="81"/>
-      <c r="S29" s="81"/>
-      <c r="T29" s="81"/>
-      <c r="U29" s="81"/>
-      <c r="V29" s="81"/>
-      <c r="W29" s="81"/>
-      <c r="X29" s="82"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="55"/>
+      <c r="V29" s="55"/>
+      <c r="W29" s="55"/>
+      <c r="X29" s="63"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -3642,32 +3633,32 @@
       <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="129" t="s">
+      <c r="A31" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="129"/>
-      <c r="C31" s="129"/>
-      <c r="D31" s="129"/>
-      <c r="E31" s="129"/>
-      <c r="F31" s="129"/>
-      <c r="G31" s="129"/>
-      <c r="H31" s="129"/>
-      <c r="I31" s="129"/>
-      <c r="J31" s="129"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="130" t="s">
+      <c r="P31" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="131"/>
-      <c r="R31" s="131"/>
-      <c r="S31" s="131"/>
-      <c r="T31" s="131"/>
-      <c r="U31" s="131"/>
-      <c r="V31" s="131"/>
-      <c r="W31" s="132"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="66"/>
+      <c r="S31" s="66"/>
+      <c r="T31" s="66"/>
+      <c r="U31" s="66"/>
+      <c r="V31" s="66"/>
+      <c r="W31" s="67"/>
       <c r="X31" s="13"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
@@ -3682,28 +3673,28 @@
       <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="129"/>
-      <c r="B32" s="129"/>
-      <c r="C32" s="129"/>
-      <c r="D32" s="129"/>
-      <c r="E32" s="129"/>
-      <c r="F32" s="129"/>
-      <c r="G32" s="129"/>
-      <c r="H32" s="129"/>
-      <c r="I32" s="129"/>
-      <c r="J32" s="129"/>
+      <c r="A32" s="64"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="133"/>
-      <c r="Q32" s="134"/>
-      <c r="R32" s="134"/>
-      <c r="S32" s="134"/>
-      <c r="T32" s="134"/>
-      <c r="U32" s="134"/>
-      <c r="V32" s="134"/>
-      <c r="W32" s="135"/>
+      <c r="P32" s="68"/>
+      <c r="Q32" s="69"/>
+      <c r="R32" s="69"/>
+      <c r="S32" s="69"/>
+      <c r="T32" s="69"/>
+      <c r="U32" s="69"/>
+      <c r="V32" s="69"/>
+      <c r="W32" s="70"/>
       <c r="X32" s="13"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
@@ -3732,14 +3723,14 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="133"/>
-      <c r="Q33" s="134"/>
-      <c r="R33" s="134"/>
-      <c r="S33" s="134"/>
-      <c r="T33" s="134"/>
-      <c r="U33" s="134"/>
-      <c r="V33" s="134"/>
-      <c r="W33" s="135"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="69"/>
+      <c r="R33" s="69"/>
+      <c r="S33" s="69"/>
+      <c r="T33" s="69"/>
+      <c r="U33" s="69"/>
+      <c r="V33" s="69"/>
+      <c r="W33" s="70"/>
       <c r="X33" s="13"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="34"/>
@@ -3757,29 +3748,29 @@
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="139" t="s">
+      <c r="B34" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="139"/>
-      <c r="D34" s="139"/>
-      <c r="E34" s="139"/>
-      <c r="F34" s="139"/>
-      <c r="G34" s="139"/>
-      <c r="H34" s="139"/>
-      <c r="I34" s="139"/>
-      <c r="J34" s="139"/>
-      <c r="K34" s="139"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="133"/>
-      <c r="Q34" s="134"/>
-      <c r="R34" s="134"/>
-      <c r="S34" s="134"/>
-      <c r="T34" s="134"/>
-      <c r="U34" s="134"/>
-      <c r="V34" s="134"/>
-      <c r="W34" s="135"/>
+      <c r="P34" s="68"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="69"/>
+      <c r="S34" s="69"/>
+      <c r="T34" s="69"/>
+      <c r="U34" s="69"/>
+      <c r="V34" s="69"/>
+      <c r="W34" s="70"/>
       <c r="X34" s="13"/>
       <c r="Z34" s="34"/>
       <c r="AA34" s="34"/>
@@ -3794,32 +3785,32 @@
       <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="139" t="s">
+      <c r="A35" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="140" t="s">
+      <c r="B35" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="141"/>
-      <c r="D35" s="141"/>
-      <c r="E35" s="141"/>
-      <c r="F35" s="141"/>
-      <c r="G35" s="141"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="141"/>
-      <c r="J35" s="141"/>
-      <c r="K35" s="142"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="77"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="133"/>
-      <c r="Q35" s="134"/>
-      <c r="R35" s="134"/>
-      <c r="S35" s="134"/>
-      <c r="T35" s="134"/>
-      <c r="U35" s="134"/>
-      <c r="V35" s="134"/>
-      <c r="W35" s="135"/>
+      <c r="P35" s="68"/>
+      <c r="Q35" s="69"/>
+      <c r="R35" s="69"/>
+      <c r="S35" s="69"/>
+      <c r="T35" s="69"/>
+      <c r="U35" s="69"/>
+      <c r="V35" s="69"/>
+      <c r="W35" s="70"/>
       <c r="X35" s="13"/>
       <c r="Z35" s="34"/>
       <c r="AA35" s="34"/>
@@ -3834,28 +3825,28 @@
       <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="139"/>
-      <c r="B36" s="143"/>
-      <c r="C36" s="144"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="144"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="144"/>
-      <c r="H36" s="144"/>
-      <c r="I36" s="144"/>
-      <c r="J36" s="144"/>
-      <c r="K36" s="145"/>
+      <c r="A36" s="74"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="80"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="133"/>
-      <c r="Q36" s="134"/>
-      <c r="R36" s="134"/>
-      <c r="S36" s="134"/>
-      <c r="T36" s="134"/>
-      <c r="U36" s="134"/>
-      <c r="V36" s="134"/>
-      <c r="W36" s="135"/>
+      <c r="P36" s="68"/>
+      <c r="Q36" s="69"/>
+      <c r="R36" s="69"/>
+      <c r="S36" s="69"/>
+      <c r="T36" s="69"/>
+      <c r="U36" s="69"/>
+      <c r="V36" s="69"/>
+      <c r="W36" s="70"/>
       <c r="X36" s="13"/>
       <c r="Z36" s="34"/>
       <c r="AA36" s="34"/>
@@ -3870,46 +3861,46 @@
       <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="139"/>
-      <c r="B37" s="146"/>
-      <c r="C37" s="147"/>
-      <c r="D37" s="147"/>
-      <c r="E37" s="147"/>
-      <c r="F37" s="147"/>
-      <c r="G37" s="147"/>
-      <c r="H37" s="147"/>
-      <c r="I37" s="147"/>
-      <c r="J37" s="147"/>
-      <c r="K37" s="148"/>
+      <c r="A37" s="74"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="83"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="136"/>
-      <c r="Q37" s="137"/>
-      <c r="R37" s="137"/>
-      <c r="S37" s="137"/>
-      <c r="T37" s="137"/>
-      <c r="U37" s="137"/>
-      <c r="V37" s="137"/>
-      <c r="W37" s="138"/>
+      <c r="P37" s="71"/>
+      <c r="Q37" s="72"/>
+      <c r="R37" s="72"/>
+      <c r="S37" s="72"/>
+      <c r="T37" s="72"/>
+      <c r="U37" s="72"/>
+      <c r="V37" s="72"/>
+      <c r="W37" s="73"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="117" t="s">
+      <c r="B38" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="118"/>
-      <c r="D38" s="118"/>
-      <c r="E38" s="118"/>
-      <c r="F38" s="118"/>
-      <c r="G38" s="118"/>
-      <c r="H38" s="118"/>
-      <c r="I38" s="118"/>
-      <c r="J38" s="118"/>
-      <c r="K38" s="119"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="85"/>
+      <c r="I38" s="85"/>
+      <c r="J38" s="85"/>
+      <c r="K38" s="86"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3927,36 +3918,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="117" t="s">
+      <c r="B39" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="118"/>
-      <c r="D39" s="118"/>
-      <c r="E39" s="118"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="118"/>
-      <c r="H39" s="118"/>
-      <c r="I39" s="118"/>
-      <c r="J39" s="118"/>
-      <c r="K39" s="119"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+      <c r="I39" s="85"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="86"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="117" t="s">
+      <c r="B40" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="118"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="118"/>
-      <c r="J40" s="118"/>
-      <c r="K40" s="119"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="85"/>
+      <c r="I40" s="85"/>
+      <c r="J40" s="85"/>
+      <c r="K40" s="86"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -3975,76 +3966,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="117" t="s">
+      <c r="B41" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="118"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
-      <c r="G41" s="118"/>
-      <c r="H41" s="118"/>
-      <c r="I41" s="118"/>
-      <c r="J41" s="118"/>
-      <c r="K41" s="119"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="85"/>
+      <c r="H41" s="85"/>
+      <c r="I41" s="85"/>
+      <c r="J41" s="85"/>
+      <c r="K41" s="86"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="120" t="s">
+      <c r="M41" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="121"/>
-      <c r="O41" s="121"/>
-      <c r="P41" s="121"/>
-      <c r="Q41" s="121"/>
-      <c r="R41" s="121"/>
-      <c r="S41" s="121"/>
-      <c r="T41" s="121"/>
-      <c r="U41" s="121"/>
-      <c r="V41" s="121"/>
-      <c r="W41" s="121"/>
-      <c r="X41" s="122"/>
+      <c r="N41" s="52"/>
+      <c r="O41" s="52"/>
+      <c r="P41" s="52"/>
+      <c r="Q41" s="52"/>
+      <c r="R41" s="52"/>
+      <c r="S41" s="52"/>
+      <c r="T41" s="52"/>
+      <c r="U41" s="52"/>
+      <c r="V41" s="52"/>
+      <c r="W41" s="52"/>
+      <c r="X41" s="53"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="117"/>
-      <c r="C42" s="118"/>
-      <c r="D42" s="118"/>
-      <c r="E42" s="118"/>
-      <c r="F42" s="118"/>
-      <c r="G42" s="118"/>
-      <c r="H42" s="118"/>
-      <c r="I42" s="118"/>
-      <c r="J42" s="118"/>
-      <c r="K42" s="119"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="85"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="85"/>
+      <c r="G42" s="85"/>
+      <c r="H42" s="85"/>
+      <c r="I42" s="85"/>
+      <c r="J42" s="85"/>
+      <c r="K42" s="86"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="120" t="s">
+      <c r="M42" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="121"/>
-      <c r="O42" s="121"/>
-      <c r="P42" s="121"/>
-      <c r="Q42" s="121"/>
-      <c r="R42" s="121"/>
-      <c r="S42" s="121"/>
-      <c r="T42" s="121"/>
-      <c r="U42" s="121"/>
-      <c r="V42" s="121"/>
-      <c r="W42" s="121"/>
-      <c r="X42" s="122"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="52"/>
+      <c r="P42" s="52"/>
+      <c r="Q42" s="52"/>
+      <c r="R42" s="52"/>
+      <c r="S42" s="52"/>
+      <c r="T42" s="52"/>
+      <c r="U42" s="52"/>
+      <c r="V42" s="52"/>
+      <c r="W42" s="52"/>
+      <c r="X42" s="53"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="117"/>
-      <c r="C43" s="118"/>
-      <c r="D43" s="118"/>
-      <c r="E43" s="118"/>
-      <c r="F43" s="118"/>
-      <c r="G43" s="118"/>
-      <c r="H43" s="118"/>
-      <c r="I43" s="118"/>
-      <c r="J43" s="118"/>
-      <c r="K43" s="119"/>
+      <c r="B43" s="84"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="85"/>
+      <c r="I43" s="85"/>
+      <c r="J43" s="85"/>
+      <c r="K43" s="86"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -4062,16 +4053,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="117"/>
-      <c r="C44" s="118"/>
-      <c r="D44" s="118"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="118"/>
-      <c r="H44" s="118"/>
-      <c r="I44" s="118"/>
-      <c r="J44" s="118"/>
-      <c r="K44" s="119"/>
+      <c r="B44" s="84"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="85"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="85"/>
+      <c r="I44" s="85"/>
+      <c r="J44" s="85"/>
+      <c r="K44" s="86"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -4089,16 +4080,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="117"/>
-      <c r="C45" s="118"/>
-      <c r="D45" s="118"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="118"/>
-      <c r="G45" s="118"/>
-      <c r="H45" s="118"/>
-      <c r="I45" s="118"/>
-      <c r="J45" s="118"/>
-      <c r="K45" s="119"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="85"/>
+      <c r="D45" s="85"/>
+      <c r="E45" s="85"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="85"/>
+      <c r="H45" s="85"/>
+      <c r="I45" s="85"/>
+      <c r="J45" s="85"/>
+      <c r="K45" s="86"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -4116,16 +4107,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="117"/>
-      <c r="C46" s="118"/>
-      <c r="D46" s="118"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118"/>
-      <c r="G46" s="118"/>
-      <c r="H46" s="118"/>
-      <c r="I46" s="118"/>
-      <c r="J46" s="118"/>
-      <c r="K46" s="119"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="85"/>
+      <c r="D46" s="85"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="85"/>
+      <c r="I46" s="85"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="86"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -4168,6 +4159,38 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B4:D5"/>
+    <mergeCell ref="G4:I5"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="J9:R10"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="Q19:X19"/>
+    <mergeCell ref="F20:G21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="Q20:X20"/>
+    <mergeCell ref="Q21:X21"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="Q23:X25"/>
+    <mergeCell ref="L24:M25"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="L12:S13"/>
+    <mergeCell ref="Q15:X17"/>
+    <mergeCell ref="M16:O17"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="B45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:K41"/>
+    <mergeCell ref="B42:K42"/>
     <mergeCell ref="M42:X42"/>
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="Q26:X27"/>
@@ -4178,38 +4201,6 @@
     <mergeCell ref="B35:K37"/>
     <mergeCell ref="M41:X41"/>
     <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B44:K44"/>
-    <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:K41"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="Y1:Z3"/>
-    <mergeCell ref="Q23:X25"/>
-    <mergeCell ref="L24:M25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="L12:S13"/>
-    <mergeCell ref="Q15:X17"/>
-    <mergeCell ref="M16:O17"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="Q19:X19"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="Q20:X20"/>
-    <mergeCell ref="Q21:X21"/>
-    <mergeCell ref="B4:D5"/>
-    <mergeCell ref="G4:I5"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="J9:R10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4220,10 +4211,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:A46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4248,7 +4239,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="44" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -4277,68 +4268,68 @@
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="42" t="s">
+      <c r="A10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="39" t="s">
-        <v>114</v>
+    <row r="11" spans="1:1" ht="15.75" customHeight="1">
+      <c r="A11" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="39" t="s">
-        <v>83</v>
+      <c r="A12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>84</v>
+      <c r="A13" s="41" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>85</v>
+      <c r="A14" s="40" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" t="s">
+      <c r="A15" s="40" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="41" t="s">
+      <c r="A16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="40" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="47" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" s="47" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="43" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:1">
@@ -4347,7 +4338,7 @@
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="47" t="s">
+      <c r="A24" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4357,123 +4348,108 @@
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="47" t="s">
-        <v>95</v>
+      <c r="A26" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" t="s">
+      <c r="A29" s="46" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>100</v>
+      <c r="A30" s="47" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>101</v>
+      <c r="A31" s="42" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="46" t="s">
-        <v>102</v>
+      <c r="A32" s="50" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="42" t="s">
-        <v>105</v>
-      </c>
-    </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="41" t="s">
-        <v>122</v>
+      <c r="A35" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="48" t="s">
-        <v>106</v>
+      <c r="A36" s="39" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="45" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="39" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="39" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="42" t="s">
+    <row r="44" spans="1:1">
+      <c r="A44" s="41" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="45" t="s">
+    <row r="45" spans="1:1">
+      <c r="A45" s="49" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="50" t="s">
-        <v>121</v>
-      </c>
-    </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="39" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="41" t="s">
+      <c r="A46" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="49" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
THIS IS THE STABLE MOST RECENT VERSION TODATE IT HAS A NAFF TERRAIN GOOD AFFORDANCE WITH FIRES AND SOUND TEXT NEEDS UPDATING SO DO MAXBARS ETC NEXT IM WORKING ON PEDAL PIRATE LITE
</commit_message>
<xml_diff>
--- a/visualforprogramstructure.xlsx
+++ b/visualforprogramstructure.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
   <si>
     <t>Understanding methods or script just run for so many seconds</t>
   </si>
@@ -273,9 +273,6 @@
     <t>do green the yellow orange red blue white is it necessary - pink get playtest feed back give them experience of two options</t>
   </si>
   <si>
-    <t>redo land so dont get stuck going forward maybe lots of bounce or some kind of current push</t>
-  </si>
-  <si>
     <t>find solution to display health - flag damage using a material layer?</t>
   </si>
   <si>
@@ -297,9 +294,6 @@
     <t>esc to return to setup</t>
   </si>
   <si>
-    <t>daycycle starts at game start</t>
-  </si>
-  <si>
     <t>read through notes made so far in notes document</t>
   </si>
   <si>
@@ -309,9 +303,6 @@
     <t>playerscript for ai make ai as similar to player as possible to make more options easier to code so ai has as much shared functionality as possible</t>
   </si>
   <si>
-    <t>shorten win screen visual</t>
-  </si>
-  <si>
     <t>redo pirate text</t>
   </si>
   <si>
@@ -339,9 +330,6 @@
     <t>do something with team names etc</t>
   </si>
   <si>
-    <t>individual win screns in middle screen countdown to next game</t>
-  </si>
-  <si>
     <t>laptop version to pc</t>
   </si>
   <si>
@@ -384,9 +372,6 @@
     <t>bake nav mesh - for laptop version ensure set terrain not walkable not a navmesh and the tile to one</t>
   </si>
   <si>
-    <t>teraain thickness and bounce + physic settings</t>
-  </si>
-  <si>
     <t>reduce physics sorting and tag layers so efficient replan structure and what does what</t>
   </si>
   <si>
@@ -400,6 +385,15 @@
   </si>
   <si>
     <t>check max bar working properly saught text - pretty certain theyre not setting the maxes to anything but default</t>
+  </si>
+  <si>
+    <t>individual win screns in middle screen countdown to next game - use the death image replace it with a canvas and have it shared with details if you lost won as your own text and a table how everyone is doing dead or what health</t>
+  </si>
+  <si>
+    <t>give black smoke plume to the bow shots maybe allow it to last longer spread more - it is 60x damage so needs alot more differentiating from the other two</t>
+  </si>
+  <si>
+    <t>daycycle starts at game start - have its start angle in start script as dawn and have script off until gamestarts and have the light set straight down until script changes it, would be good if it had a lighting static so ship lights know when to turn on and off</t>
   </si>
 </sst>
 </file>
@@ -557,7 +551,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -651,12 +645,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -679,6 +667,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="56">
     <border>
@@ -1357,7 +1357,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -1485,6 +1485,7 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -2749,14 +2750,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1">
-      <c r="Y1" s="89" t="s">
+      <c r="Y1" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="90"/>
+      <c r="Z1" s="91"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="Y2" s="91"/>
-      <c r="Z2" s="92"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="93"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
       <c r="AH2" s="35"/>
@@ -2765,8 +2766,8 @@
       <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="94"/>
+      <c r="Y3" s="94"/>
+      <c r="Z3" s="95"/>
       <c r="AA3" s="34"/>
       <c r="AB3" s="38" t="s">
         <v>58</v>
@@ -2784,16 +2785,16 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="122"/>
-      <c r="G4" s="128" t="s">
+      <c r="C4" s="122"/>
+      <c r="D4" s="123"/>
+      <c r="G4" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="121"/>
-      <c r="I4" s="122"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="123"/>
       <c r="Z4" s="34"/>
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
@@ -2807,12 +2808,12 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="1:37" ht="15" customHeight="1">
-      <c r="B5" s="129"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="130"/>
-      <c r="G5" s="129"/>
-      <c r="H5" s="141"/>
-      <c r="I5" s="130"/>
+      <c r="B5" s="130"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="131"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="131"/>
       <c r="Z5" s="34" t="s">
         <v>50</v>
       </c>
@@ -2854,12 +2855,12 @@
       <c r="AK6" s="35"/>
     </row>
     <row r="7" spans="1:37" ht="15" customHeight="1">
-      <c r="B7" s="142" t="s">
+      <c r="B7" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="144"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="145"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -2889,10 +2890,10 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="1:37" ht="15" customHeight="1">
-      <c r="B8" s="145"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
-      <c r="E8" s="147"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="148"/>
       <c r="G8" s="33"/>
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
@@ -2929,17 +2930,17 @@
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="128" t="s">
+      <c r="J9" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="121"/>
-      <c r="L9" s="121"/>
-      <c r="M9" s="121"/>
-      <c r="N9" s="121"/>
-      <c r="O9" s="121"/>
-      <c r="P9" s="121"/>
-      <c r="Q9" s="121"/>
-      <c r="R9" s="122"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="122"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="122"/>
+      <c r="O9" s="122"/>
+      <c r="P9" s="122"/>
+      <c r="Q9" s="122"/>
+      <c r="R9" s="123"/>
       <c r="Z9" s="34" t="s">
         <v>69</v>
       </c>
@@ -2967,25 +2968,25 @@
     </row>
     <row r="10" spans="1:37" ht="15" customHeight="1">
       <c r="A10" s="12"/>
-      <c r="B10" s="148" t="s">
+      <c r="B10" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="148"/>
-      <c r="D10" s="148"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="149"/>
       <c r="E10" s="31"/>
       <c r="F10" s="4"/>
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="129"/>
-      <c r="K10" s="141"/>
-      <c r="L10" s="141"/>
-      <c r="M10" s="141"/>
-      <c r="N10" s="141"/>
-      <c r="O10" s="141"/>
-      <c r="P10" s="141"/>
-      <c r="Q10" s="141"/>
-      <c r="R10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="142"/>
+      <c r="Q10" s="142"/>
+      <c r="R10" s="131"/>
       <c r="Z10" s="34">
         <v>20</v>
       </c>
@@ -3017,10 +3018,10 @@
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="104" t="s">
+      <c r="G11" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="105"/>
+      <c r="H11" s="106"/>
       <c r="I11" s="28"/>
       <c r="Z11" s="34">
         <v>5</v>
@@ -3056,16 +3057,16 @@
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
-      <c r="L12" s="106" t="s">
+      <c r="L12" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="M12" s="107"/>
-      <c r="N12" s="107"/>
-      <c r="O12" s="107"/>
-      <c r="P12" s="107"/>
-      <c r="Q12" s="107"/>
-      <c r="R12" s="107"/>
-      <c r="S12" s="108"/>
+      <c r="M12" s="108"/>
+      <c r="N12" s="108"/>
+      <c r="O12" s="108"/>
+      <c r="P12" s="108"/>
+      <c r="Q12" s="108"/>
+      <c r="R12" s="108"/>
+      <c r="S12" s="109"/>
       <c r="Z12" s="34"/>
       <c r="AA12" s="34"/>
       <c r="AB12" s="34"/>
@@ -3088,14 +3089,14 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
-      <c r="L13" s="109"/>
-      <c r="M13" s="110"/>
-      <c r="N13" s="110"/>
-      <c r="O13" s="110"/>
-      <c r="P13" s="110"/>
-      <c r="Q13" s="110"/>
-      <c r="R13" s="110"/>
-      <c r="S13" s="111"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="111"/>
+      <c r="O13" s="111"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="111"/>
+      <c r="S13" s="112"/>
       <c r="Z13" s="34"/>
       <c r="AA13" s="34"/>
       <c r="AB13" s="34"/>
@@ -3139,16 +3140,16 @@
       <c r="J15" s="18"/>
       <c r="K15" s="27"/>
       <c r="L15"/>
-      <c r="Q15" s="112" t="s">
+      <c r="Q15" s="113" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="113"/>
-      <c r="S15" s="113"/>
-      <c r="T15" s="113"/>
-      <c r="U15" s="113"/>
-      <c r="V15" s="113"/>
-      <c r="W15" s="113"/>
-      <c r="X15" s="114"/>
+      <c r="R15" s="114"/>
+      <c r="S15" s="114"/>
+      <c r="T15" s="114"/>
+      <c r="U15" s="114"/>
+      <c r="V15" s="114"/>
+      <c r="W15" s="114"/>
+      <c r="X15" s="115"/>
       <c r="Z15" s="34"/>
       <c r="AA15" s="34"/>
       <c r="AB15" s="34"/>
@@ -3166,19 +3167,19 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="26"/>
-      <c r="M16" s="121" t="s">
+      <c r="M16" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="121"/>
-      <c r="O16" s="122"/>
-      <c r="Q16" s="115"/>
-      <c r="R16" s="116"/>
-      <c r="S16" s="116"/>
-      <c r="T16" s="116"/>
-      <c r="U16" s="116"/>
-      <c r="V16" s="116"/>
-      <c r="W16" s="116"/>
-      <c r="X16" s="117"/>
+      <c r="N16" s="122"/>
+      <c r="O16" s="123"/>
+      <c r="Q16" s="116"/>
+      <c r="R16" s="117"/>
+      <c r="S16" s="117"/>
+      <c r="T16" s="117"/>
+      <c r="U16" s="117"/>
+      <c r="V16" s="117"/>
+      <c r="W16" s="117"/>
+      <c r="X16" s="118"/>
       <c r="Z16" s="34"/>
       <c r="AA16" s="34"/>
       <c r="AB16" s="34"/>
@@ -3192,31 +3193,31 @@
       <c r="AK16" s="35"/>
     </row>
     <row r="17" spans="1:37" ht="15" customHeight="1" thickBot="1">
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="107"/>
+      <c r="C17" s="108"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="125" t="s">
+      <c r="E17" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="126"/>
-      <c r="G17" s="127"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="128"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="24"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="123"/>
-      <c r="O17" s="124"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="119"/>
-      <c r="S17" s="119"/>
-      <c r="T17" s="119"/>
-      <c r="U17" s="119"/>
-      <c r="V17" s="119"/>
-      <c r="W17" s="119"/>
-      <c r="X17" s="120"/>
+      <c r="M17" s="124"/>
+      <c r="N17" s="124"/>
+      <c r="O17" s="125"/>
+      <c r="Q17" s="119"/>
+      <c r="R17" s="120"/>
+      <c r="S17" s="120"/>
+      <c r="T17" s="120"/>
+      <c r="U17" s="120"/>
+      <c r="V17" s="120"/>
+      <c r="W17" s="120"/>
+      <c r="X17" s="121"/>
       <c r="Z17" s="34"/>
       <c r="AA17" s="34"/>
       <c r="AB17" s="34"/>
@@ -3230,18 +3231,18 @@
       <c r="AK17" s="35"/>
     </row>
     <row r="18" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B18" s="109"/>
-      <c r="C18" s="110"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="111"/>
       <c r="F18" s="23"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="18"/>
       <c r="K18" s="17"/>
-      <c r="L18" s="87" t="s">
+      <c r="L18" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="88"/>
+      <c r="M18" s="89"/>
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3266,32 +3267,32 @@
       <c r="AK18" s="35"/>
     </row>
     <row r="19" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B19" s="128" t="s">
+      <c r="B19" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="122"/>
+      <c r="C19" s="123"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="18"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="88"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="89"/>
       <c r="N19" s="6"/>
       <c r="O19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="P19" s="21"/>
-      <c r="Q19" s="131" t="s">
+      <c r="Q19" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="R19" s="132"/>
-      <c r="S19" s="132"/>
-      <c r="T19" s="132"/>
-      <c r="U19" s="132"/>
-      <c r="V19" s="132"/>
-      <c r="W19" s="132"/>
-      <c r="X19" s="133"/>
+      <c r="R19" s="133"/>
+      <c r="S19" s="133"/>
+      <c r="T19" s="133"/>
+      <c r="U19" s="133"/>
+      <c r="V19" s="133"/>
+      <c r="W19" s="133"/>
+      <c r="X19" s="134"/>
       <c r="Z19" s="34"/>
       <c r="AA19" s="34"/>
       <c r="AB19" s="34"/>
@@ -3305,32 +3306,32 @@
       <c r="AK19" s="35"/>
     </row>
     <row r="20" spans="1:37" ht="15" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B20" s="129"/>
-      <c r="C20" s="130"/>
-      <c r="F20" s="134" t="s">
+      <c r="B20" s="130"/>
+      <c r="C20" s="131"/>
+      <c r="F20" s="135" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="135"/>
+      <c r="G20" s="136"/>
       <c r="H20" s="20"/>
       <c r="I20" s="19"/>
       <c r="J20" s="18"/>
       <c r="K20" s="17"/>
-      <c r="L20" s="87" t="s">
+      <c r="L20" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="88"/>
+      <c r="M20" s="89"/>
       <c r="N20" s="6"/>
       <c r="O20" s="14"/>
-      <c r="Q20" s="54" t="s">
+      <c r="Q20" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="R20" s="55"/>
-      <c r="S20" s="55"/>
-      <c r="T20" s="55"/>
-      <c r="U20" s="55"/>
-      <c r="V20" s="55"/>
-      <c r="W20" s="55"/>
-      <c r="X20" s="63"/>
+      <c r="R20" s="56"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="56"/>
+      <c r="U20" s="56"/>
+      <c r="V20" s="56"/>
+      <c r="W20" s="56"/>
+      <c r="X20" s="64"/>
       <c r="Z20" s="34"/>
       <c r="AA20" s="34"/>
       <c r="AB20" s="34"/>
@@ -3347,28 +3348,28 @@
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="F21" s="136"/>
-      <c r="G21" s="137"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="138"/>
       <c r="H21" s="20"/>
       <c r="I21" s="19"/>
       <c r="J21" s="18"/>
       <c r="K21" s="17"/>
-      <c r="L21" s="87"/>
-      <c r="M21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="89"/>
       <c r="N21" s="6"/>
       <c r="O21" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" s="138" t="s">
+      <c r="Q21" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="139"/>
-      <c r="S21" s="139"/>
-      <c r="T21" s="139"/>
-      <c r="U21" s="139"/>
-      <c r="V21" s="139"/>
-      <c r="W21" s="139"/>
-      <c r="X21" s="140"/>
+      <c r="R21" s="140"/>
+      <c r="S21" s="140"/>
+      <c r="T21" s="140"/>
+      <c r="U21" s="140"/>
+      <c r="V21" s="140"/>
+      <c r="W21" s="140"/>
+      <c r="X21" s="141"/>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
       <c r="AB21" s="34"/>
@@ -3386,10 +3387,10 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="K22" s="17"/>
-      <c r="L22" s="87" t="s">
+      <c r="L22" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="88"/>
+      <c r="M22" s="89"/>
       <c r="N22" s="6"/>
       <c r="O22" s="14"/>
       <c r="X22" s="13"/>
@@ -3409,28 +3410,28 @@
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="55"/>
-      <c r="G23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="57"/>
       <c r="K23" s="17"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="88"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="89"/>
       <c r="N23" s="6"/>
       <c r="O23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="95" t="s">
+      <c r="Q23" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="96"/>
-      <c r="S23" s="96"/>
-      <c r="T23" s="96"/>
-      <c r="U23" s="96"/>
-      <c r="V23" s="96"/>
-      <c r="W23" s="96"/>
-      <c r="X23" s="97"/>
+      <c r="R23" s="97"/>
+      <c r="S23" s="97"/>
+      <c r="T23" s="97"/>
+      <c r="U23" s="97"/>
+      <c r="V23" s="97"/>
+      <c r="W23" s="97"/>
+      <c r="X23" s="98"/>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
       <c r="AB23" s="34"/>
@@ -3448,20 +3449,20 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="K24" s="17"/>
-      <c r="L24" s="87" t="s">
+      <c r="L24" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="88"/>
+      <c r="M24" s="89"/>
       <c r="N24" s="6"/>
       <c r="O24" s="14"/>
-      <c r="Q24" s="98"/>
-      <c r="R24" s="99"/>
-      <c r="S24" s="99"/>
-      <c r="T24" s="99"/>
-      <c r="U24" s="99"/>
-      <c r="V24" s="99"/>
-      <c r="W24" s="99"/>
-      <c r="X24" s="100"/>
+      <c r="Q24" s="99"/>
+      <c r="R24" s="100"/>
+      <c r="S24" s="100"/>
+      <c r="T24" s="100"/>
+      <c r="U24" s="100"/>
+      <c r="V24" s="100"/>
+      <c r="W24" s="100"/>
+      <c r="X24" s="101"/>
       <c r="Z24" s="34"/>
       <c r="AA24" s="34"/>
       <c r="AB24" s="34"/>
@@ -3479,18 +3480,18 @@
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="K25" s="17"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="89"/>
       <c r="N25" s="6"/>
       <c r="O25" s="14"/>
-      <c r="Q25" s="101"/>
-      <c r="R25" s="102"/>
-      <c r="S25" s="102"/>
-      <c r="T25" s="102"/>
-      <c r="U25" s="102"/>
-      <c r="V25" s="102"/>
-      <c r="W25" s="102"/>
-      <c r="X25" s="103"/>
+      <c r="Q25" s="102"/>
+      <c r="R25" s="103"/>
+      <c r="S25" s="103"/>
+      <c r="T25" s="103"/>
+      <c r="U25" s="103"/>
+      <c r="V25" s="103"/>
+      <c r="W25" s="103"/>
+      <c r="X25" s="104"/>
       <c r="Z25" s="34"/>
       <c r="AA25" s="34"/>
       <c r="AB25" s="34"/>
@@ -3507,26 +3508,26 @@
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="56"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="57"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="12"/>
       <c r="O26" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="57" t="s">
+      <c r="Q26" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="R26" s="58"/>
-      <c r="S26" s="58"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="58"/>
-      <c r="V26" s="58"/>
-      <c r="W26" s="58"/>
-      <c r="X26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="60"/>
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
       <c r="AB26" s="34"/>
@@ -3542,14 +3543,14 @@
     <row r="27" spans="1:37" ht="15" customHeight="1">
       <c r="N27" s="12"/>
       <c r="O27" s="14"/>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61"/>
-      <c r="T27" s="61"/>
-      <c r="U27" s="61"/>
-      <c r="V27" s="61"/>
-      <c r="W27" s="61"/>
-      <c r="X27" s="62"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="63"/>
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
       <c r="AB27" s="34"/>
@@ -3583,16 +3584,16 @@
       <c r="O29" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="54" t="s">
+      <c r="Q29" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="R29" s="55"/>
-      <c r="S29" s="55"/>
-      <c r="T29" s="55"/>
-      <c r="U29" s="55"/>
-      <c r="V29" s="55"/>
-      <c r="W29" s="55"/>
-      <c r="X29" s="63"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
+      <c r="X29" s="64"/>
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
       <c r="AB29" s="34"/>
@@ -3633,32 +3634,32 @@
       <c r="AK30" s="34"/>
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
       <c r="K31" s="15"/>
       <c r="L31" s="4"/>
       <c r="N31" s="12"/>
       <c r="O31" s="14"/>
-      <c r="P31" s="65" t="s">
+      <c r="P31" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="Q31" s="66"/>
-      <c r="R31" s="66"/>
-      <c r="S31" s="66"/>
-      <c r="T31" s="66"/>
-      <c r="U31" s="66"/>
-      <c r="V31" s="66"/>
-      <c r="W31" s="67"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="67"/>
+      <c r="T31" s="67"/>
+      <c r="U31" s="67"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="68"/>
       <c r="X31" s="13"/>
       <c r="Z31" s="34"/>
       <c r="AA31" s="34"/>
@@ -3673,28 +3674,28 @@
       <c r="AK31" s="34"/>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1">
-      <c r="A32" s="64"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
       <c r="K32" s="15"/>
       <c r="L32" s="4"/>
       <c r="N32" s="12"/>
       <c r="O32" s="14"/>
-      <c r="P32" s="68"/>
-      <c r="Q32" s="69"/>
-      <c r="R32" s="69"/>
-      <c r="S32" s="69"/>
-      <c r="T32" s="69"/>
-      <c r="U32" s="69"/>
-      <c r="V32" s="69"/>
-      <c r="W32" s="70"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="70"/>
+      <c r="R32" s="70"/>
+      <c r="S32" s="70"/>
+      <c r="T32" s="70"/>
+      <c r="U32" s="70"/>
+      <c r="V32" s="70"/>
+      <c r="W32" s="71"/>
       <c r="X32" s="13"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="34"/>
@@ -3723,14 +3724,14 @@
       <c r="L33" s="4"/>
       <c r="N33" s="12"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="68"/>
-      <c r="Q33" s="69"/>
-      <c r="R33" s="69"/>
-      <c r="S33" s="69"/>
-      <c r="T33" s="69"/>
-      <c r="U33" s="69"/>
-      <c r="V33" s="69"/>
-      <c r="W33" s="70"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="70"/>
+      <c r="R33" s="70"/>
+      <c r="S33" s="70"/>
+      <c r="T33" s="70"/>
+      <c r="U33" s="70"/>
+      <c r="V33" s="70"/>
+      <c r="W33" s="71"/>
       <c r="X33" s="13"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="34"/>
@@ -3748,29 +3749,29 @@
       <c r="A34" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="74"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
       <c r="L34" s="4"/>
       <c r="N34" s="12"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="68"/>
-      <c r="Q34" s="69"/>
-      <c r="R34" s="69"/>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="69"/>
-      <c r="W34" s="70"/>
+      <c r="P34" s="69"/>
+      <c r="Q34" s="70"/>
+      <c r="R34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="70"/>
+      <c r="W34" s="71"/>
       <c r="X34" s="13"/>
       <c r="Z34" s="34"/>
       <c r="AA34" s="34"/>
@@ -3785,32 +3786,32 @@
       <c r="AK34" s="34"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1">
-      <c r="A35" s="74" t="s">
+      <c r="A35" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="75" t="s">
+      <c r="B35" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
       <c r="L35" s="4"/>
       <c r="N35" s="12"/>
       <c r="O35" s="14"/>
-      <c r="P35" s="68"/>
-      <c r="Q35" s="69"/>
-      <c r="R35" s="69"/>
-      <c r="S35" s="69"/>
-      <c r="T35" s="69"/>
-      <c r="U35" s="69"/>
-      <c r="V35" s="69"/>
-      <c r="W35" s="70"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="70"/>
+      <c r="R35" s="70"/>
+      <c r="S35" s="70"/>
+      <c r="T35" s="70"/>
+      <c r="U35" s="70"/>
+      <c r="V35" s="70"/>
+      <c r="W35" s="71"/>
       <c r="X35" s="13"/>
       <c r="Z35" s="34"/>
       <c r="AA35" s="34"/>
@@ -3825,28 +3826,28 @@
       <c r="AK35" s="34"/>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1">
-      <c r="A36" s="74"/>
-      <c r="B36" s="78"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="79"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="80"/>
+      <c r="A36" s="75"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="81"/>
       <c r="L36" s="4"/>
       <c r="N36" s="12"/>
       <c r="O36" s="14"/>
-      <c r="P36" s="68"/>
-      <c r="Q36" s="69"/>
-      <c r="R36" s="69"/>
-      <c r="S36" s="69"/>
-      <c r="T36" s="69"/>
-      <c r="U36" s="69"/>
-      <c r="V36" s="69"/>
-      <c r="W36" s="70"/>
+      <c r="P36" s="69"/>
+      <c r="Q36" s="70"/>
+      <c r="R36" s="70"/>
+      <c r="S36" s="70"/>
+      <c r="T36" s="70"/>
+      <c r="U36" s="70"/>
+      <c r="V36" s="70"/>
+      <c r="W36" s="71"/>
       <c r="X36" s="13"/>
       <c r="Z36" s="34"/>
       <c r="AA36" s="34"/>
@@ -3861,46 +3862,46 @@
       <c r="AK36" s="34"/>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1">
-      <c r="A37" s="74"/>
-      <c r="B37" s="81"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="82"/>
-      <c r="K37" s="83"/>
+      <c r="A37" s="75"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="84"/>
       <c r="L37" s="4"/>
       <c r="N37" s="12"/>
       <c r="O37" s="14"/>
-      <c r="P37" s="71"/>
-      <c r="Q37" s="72"/>
-      <c r="R37" s="72"/>
-      <c r="S37" s="72"/>
-      <c r="T37" s="72"/>
-      <c r="U37" s="72"/>
-      <c r="V37" s="72"/>
-      <c r="W37" s="73"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="73"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="73"/>
+      <c r="V37" s="73"/>
+      <c r="W37" s="74"/>
       <c r="X37" s="13"/>
     </row>
     <row r="38" spans="1:37" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="84" t="s">
+      <c r="B38" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="85"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="85"/>
-      <c r="I38" s="85"/>
-      <c r="J38" s="85"/>
-      <c r="K38" s="86"/>
+      <c r="C38" s="86"/>
+      <c r="D38" s="86"/>
+      <c r="E38" s="86"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="86"/>
+      <c r="J38" s="86"/>
+      <c r="K38" s="87"/>
       <c r="L38" s="4"/>
       <c r="N38" s="12"/>
       <c r="O38" s="11"/>
@@ -3918,36 +3919,36 @@
       <c r="A39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="84" t="s">
+      <c r="B39" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="85"/>
-      <c r="J39" s="85"/>
-      <c r="K39" s="86"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="87"/>
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:37" ht="15" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="84" t="s">
+      <c r="B40" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="85"/>
-      <c r="D40" s="85"/>
-      <c r="E40" s="85"/>
-      <c r="F40" s="85"/>
-      <c r="G40" s="85"/>
-      <c r="H40" s="85"/>
-      <c r="I40" s="85"/>
-      <c r="J40" s="85"/>
-      <c r="K40" s="86"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="86"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="86"/>
+      <c r="K40" s="87"/>
       <c r="L40" s="4"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -3966,76 +3967,76 @@
       <c r="A41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="84" t="s">
+      <c r="B41" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="85"/>
-      <c r="D41" s="85"/>
-      <c r="E41" s="85"/>
-      <c r="F41" s="85"/>
-      <c r="G41" s="85"/>
-      <c r="H41" s="85"/>
-      <c r="I41" s="85"/>
-      <c r="J41" s="85"/>
-      <c r="K41" s="86"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="86"/>
+      <c r="H41" s="86"/>
+      <c r="I41" s="86"/>
+      <c r="J41" s="86"/>
+      <c r="K41" s="87"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="51" t="s">
+      <c r="M41" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="52"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="52"/>
-      <c r="Q41" s="52"/>
-      <c r="R41" s="52"/>
-      <c r="S41" s="52"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="53"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="54"/>
       <c r="Y41" s="4"/>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1">
       <c r="A42" s="7"/>
-      <c r="B42" s="84"/>
-      <c r="C42" s="85"/>
-      <c r="D42" s="85"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="85"/>
-      <c r="G42" s="85"/>
-      <c r="H42" s="85"/>
-      <c r="I42" s="85"/>
-      <c r="J42" s="85"/>
-      <c r="K42" s="86"/>
+      <c r="B42" s="85"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="86"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="86"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="86"/>
+      <c r="J42" s="86"/>
+      <c r="K42" s="87"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="51" t="s">
+      <c r="M42" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="52"/>
-      <c r="R42" s="52"/>
-      <c r="S42" s="52"/>
-      <c r="T42" s="52"/>
-      <c r="U42" s="52"/>
-      <c r="V42" s="52"/>
-      <c r="W42" s="52"/>
-      <c r="X42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="53"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="54"/>
       <c r="Y42" s="4"/>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1">
       <c r="A43" s="7"/>
-      <c r="B43" s="84"/>
-      <c r="C43" s="85"/>
-      <c r="D43" s="85"/>
-      <c r="E43" s="85"/>
-      <c r="F43" s="85"/>
-      <c r="G43" s="85"/>
-      <c r="H43" s="85"/>
-      <c r="I43" s="85"/>
-      <c r="J43" s="85"/>
-      <c r="K43" s="86"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
+      <c r="G43" s="86"/>
+      <c r="H43" s="86"/>
+      <c r="I43" s="86"/>
+      <c r="J43" s="86"/>
+      <c r="K43" s="87"/>
       <c r="L43" s="6"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -4053,16 +4054,16 @@
     </row>
     <row r="44" spans="1:37" ht="15" customHeight="1">
       <c r="A44" s="7"/>
-      <c r="B44" s="84"/>
-      <c r="C44" s="85"/>
-      <c r="D44" s="85"/>
-      <c r="E44" s="85"/>
-      <c r="F44" s="85"/>
-      <c r="G44" s="85"/>
-      <c r="H44" s="85"/>
-      <c r="I44" s="85"/>
-      <c r="J44" s="85"/>
-      <c r="K44" s="86"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="86"/>
+      <c r="E44" s="86"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="86"/>
+      <c r="H44" s="86"/>
+      <c r="I44" s="86"/>
+      <c r="J44" s="86"/>
+      <c r="K44" s="87"/>
       <c r="L44" s="6"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -4080,16 +4081,16 @@
     </row>
     <row r="45" spans="1:37" ht="15" customHeight="1">
       <c r="A45" s="7"/>
-      <c r="B45" s="84"/>
-      <c r="C45" s="85"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="85"/>
-      <c r="H45" s="85"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
-      <c r="K45" s="86"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="86"/>
+      <c r="H45" s="86"/>
+      <c r="I45" s="86"/>
+      <c r="J45" s="86"/>
+      <c r="K45" s="87"/>
       <c r="L45" s="6"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
@@ -4107,16 +4108,16 @@
     </row>
     <row r="46" spans="1:37" ht="15" customHeight="1">
       <c r="A46" s="7"/>
-      <c r="B46" s="84"/>
-      <c r="C46" s="85"/>
-      <c r="D46" s="85"/>
-      <c r="E46" s="85"/>
-      <c r="F46" s="85"/>
-      <c r="G46" s="85"/>
-      <c r="H46" s="85"/>
-      <c r="I46" s="85"/>
-      <c r="J46" s="85"/>
-      <c r="K46" s="86"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
+      <c r="G46" s="86"/>
+      <c r="H46" s="86"/>
+      <c r="I46" s="86"/>
+      <c r="J46" s="86"/>
+      <c r="K46" s="87"/>
       <c r="L46" s="6"/>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -4211,10 +4212,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A46"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4228,7 +4229,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="39" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4239,102 +4240,102 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="44" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="40" t="s">
+      <c r="A5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="A6" s="40" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="40" t="s">
+      <c r="A7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" t="s">
+      <c r="A8" s="41" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="41" t="s">
+      <c r="A9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" t="s">
+      <c r="A12" s="41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="42" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="41" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="40" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="40" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" s="39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="46" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="47" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" s="46" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="47" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="47" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -4349,107 +4350,97 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="A27" s="51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="46" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" s="39" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="46" t="s">
+    <row r="30" spans="1:1">
+      <c r="A30" s="49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="47" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="42" t="s">
-        <v>102</v>
-      </c>
-    </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="50" t="s">
-        <v>118</v>
+      <c r="A32" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="48" t="s">
-        <v>103</v>
+      <c r="A33" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="39" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" t="s">
+      <c r="A37" s="39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="45" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>106</v>
-      </c>
-    </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="41" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="42" t="s">
+    <row r="42" spans="1:1">
+      <c r="A42" s="48" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="45" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="50" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="39" t="s">
-        <v>113</v>
+      <c r="A43" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="49" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>